<commit_message>
Added code for iterating over vintage dates & backtesting (v0.11)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A029381-0BA5-4126-92AB-41E552D27003}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0463BB7A-9BB6-407E-B354-2C4ADEE6C361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="355">
   <si>
     <t>gdp</t>
   </si>
@@ -991,6 +991,117 @@
   </si>
   <si>
     <t>d2</t>
+  </si>
+  <si>
+    <t>%5EGSPC</t>
+  </si>
+  <si>
+    <t>%5EVIX</t>
+  </si>
+  <si>
+    <t>snyfed</t>
+  </si>
+  <si>
+    <t>stxfed</t>
+  </si>
+  <si>
+    <t>sphfed</t>
+  </si>
+  <si>
+    <t>Philadelphia Fed: Future Capital Expenditures Survey</t>
+  </si>
+  <si>
+    <t>CEFDFSA066MSFRBPHI</t>
+  </si>
+  <si>
+    <t>Dallas Fed: Current General Business Activity</t>
+  </si>
+  <si>
+    <t>houst</t>
+  </si>
+  <si>
+    <t>Housing Starts</t>
+  </si>
+  <si>
+    <t>HOUST</t>
+  </si>
+  <si>
+    <t>thousands of houses</t>
+  </si>
+  <si>
+    <t>emp</t>
+  </si>
+  <si>
+    <t>All Employees (Nonfarm)</t>
+  </si>
+  <si>
+    <t>Unemployment Rate</t>
+  </si>
+  <si>
+    <t>PAYEMS</t>
+  </si>
+  <si>
+    <t>thousands of persons</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>Total Construction Spending</t>
+  </si>
+  <si>
+    <t>Business Sector</t>
+  </si>
+  <si>
+    <t>TTLCONS</t>
+  </si>
+  <si>
+    <t>millions of dollars</t>
+  </si>
+  <si>
+    <t>hsold</t>
+  </si>
+  <si>
+    <t>Houses Sold</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>HSN1F</t>
+  </si>
+  <si>
+    <t>thousands</t>
+  </si>
+  <si>
+    <t>mnodg</t>
+  </si>
+  <si>
+    <t>DGORDER</t>
+  </si>
+  <si>
+    <t>cu</t>
+  </si>
+  <si>
+    <t>Capacity Utilization: Total Index</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>% of total capacity</t>
+  </si>
+  <si>
+    <t>hpermits</t>
+  </si>
+  <si>
+    <t>New Private Housing Permits</t>
+  </si>
+  <si>
+    <t>PERMIT</t>
+  </si>
+  <si>
+    <t>Manufacturers New Orders: Durable Goods</t>
   </si>
 </sst>
 </file>
@@ -1059,25 +1170,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color theme="9"/>
@@ -1381,6 +1473,20 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1397,20 +1503,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1545,6 +1637,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1618,45 +1729,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N85" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:N85" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N93" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:N93" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="34"/>
     <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="33"/>
     <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="32"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:M88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1959,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M83" sqref="M83"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3825,7 +3936,7 @@
         <v>30</v>
       </c>
       <c r="M42" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>170</v>
@@ -3869,7 +3980,7 @@
         <v>30</v>
       </c>
       <c r="M43" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>170</v>
@@ -3913,7 +4024,7 @@
         <v>30</v>
       </c>
       <c r="M44" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="6" t="s">
         <v>170</v>
@@ -3957,7 +4068,7 @@
         <v>30</v>
       </c>
       <c r="M45" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>170</v>
@@ -4194,7 +4305,7 @@
         <v>182</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>178</v>
@@ -4229,25 +4340,25 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>75</v>
+        <v>327</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>178</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>42</v>
+        <v>328</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>105</v>
+        <v>329</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>44</v>
@@ -4256,7 +4367,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>30</v>
@@ -4268,30 +4379,30 @@
         <v>1</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>17</v>
+        <v>340</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>76</v>
+        <v>341</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>178</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>43</v>
+        <v>343</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>105</v>
+        <v>344</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>44</v>
@@ -4300,7 +4411,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>30</v>
@@ -4309,33 +4420,33 @@
         <v>311</v>
       </c>
       <c r="M53" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>18</v>
+        <v>351</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>77</v>
+        <v>352</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>178</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>33</v>
+        <v>353</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>105</v>
+        <v>344</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>44</v>
@@ -4344,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>30</v>
@@ -4356,18 +4467,18 @@
         <v>1</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>19</v>
+        <v>345</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>78</v>
+        <v>354</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>183</v>
+        <v>337</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>311</v>
@@ -4376,10 +4487,10 @@
         <v>178</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>35</v>
+        <v>346</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>105</v>
+        <v>339</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>44</v>
@@ -4388,7 +4499,7 @@
         <v>0</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>30</v>
@@ -4397,21 +4508,21 @@
         <v>311</v>
       </c>
       <c r="M55" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>20</v>
+        <v>347</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>80</v>
+        <v>348</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>183</v>
+        <v>337</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>311</v>
@@ -4420,10 +4531,10 @@
         <v>178</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>36</v>
+        <v>349</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>105</v>
+        <v>350</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>44</v>
@@ -4432,7 +4543,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>30</v>
@@ -4441,21 +4552,21 @@
         <v>311</v>
       </c>
       <c r="M56" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>21</v>
+        <v>335</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>81</v>
+        <v>336</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>183</v>
+        <v>337</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>311</v>
@@ -4464,10 +4575,10 @@
         <v>178</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>37</v>
+        <v>338</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>105</v>
+        <v>339</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>44</v>
@@ -4476,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>30</v>
@@ -4485,18 +4596,18 @@
         <v>311</v>
       </c>
       <c r="M57" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>183</v>
@@ -4508,7 +4619,7 @@
         <v>178</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>105</v>
@@ -4537,10 +4648,10 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>183</v>
@@ -4552,7 +4663,7 @@
         <v>178</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>105</v>
@@ -4581,10 +4692,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>183</v>
@@ -4596,7 +4707,7 @@
         <v>178</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>105</v>
@@ -4617,7 +4728,7 @@
         <v>311</v>
       </c>
       <c r="M60" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60" s="6" t="s">
         <v>190</v>
@@ -4625,10 +4736,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>183</v>
@@ -4640,7 +4751,7 @@
         <v>178</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>105</v>
@@ -4669,10 +4780,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>183</v>
@@ -4684,7 +4795,7 @@
         <v>178</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>105</v>
@@ -4713,10 +4824,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>183</v>
@@ -4728,7 +4839,7 @@
         <v>178</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>105</v>
@@ -4757,13 +4868,13 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>311</v>
@@ -4772,10 +4883,10 @@
         <v>178</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>219</v>
+        <v>105</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>44</v>
@@ -4796,18 +4907,18 @@
         <v>1</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>278</v>
+        <v>183</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>311</v>
@@ -4816,7 +4927,7 @@
         <v>178</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>105</v>
@@ -4828,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K65" s="6" t="s">
         <v>30</v>
@@ -4837,21 +4948,21 @@
         <v>311</v>
       </c>
       <c r="M65" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>311</v>
@@ -4860,10 +4971,10 @@
         <v>178</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>44</v>
@@ -4881,30 +4992,33 @@
         <v>311</v>
       </c>
       <c r="M66" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>261</v>
+        <v>183</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>275</v>
+        <v>178</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>44</v>
@@ -4913,7 +5027,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K67" s="6" t="s">
         <v>30</v>
@@ -4922,21 +5036,21 @@
         <v>311</v>
       </c>
       <c r="M67" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>261</v>
+        <v>183</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>311</v>
@@ -4945,10 +5059,10 @@
         <v>178</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>44</v>
@@ -4966,21 +5080,21 @@
         <v>311</v>
       </c>
       <c r="M68" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>311</v>
@@ -4989,10 +5103,10 @@
         <v>178</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>313</v>
+        <v>105</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>44</v>
@@ -5001,27 +5115,27 @@
         <v>0</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K69" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L69" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M69" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>184</v>
@@ -5033,10 +5147,10 @@
         <v>178</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>313</v>
+        <v>219</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>44</v>
@@ -5045,10 +5159,10 @@
         <v>0</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L70" s="6" t="s">
         <v>311</v>
@@ -5062,13 +5176,13 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>93</v>
+        <v>332</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>311</v>
@@ -5077,28 +5191,28 @@
         <v>178</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>220</v>
+        <v>105</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I71" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M71" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="M71" s="6" t="b">
-        <v>0</v>
       </c>
       <c r="N71" s="6" t="s">
         <v>170</v>
@@ -5106,13 +5220,13 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>62</v>
+        <v>330</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>94</v>
+        <v>331</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>311</v>
@@ -5121,10 +5235,10 @@
         <v>178</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>63</v>
+        <v>333</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>110</v>
+        <v>334</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>44</v>
@@ -5133,7 +5247,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>30</v>
@@ -5150,13 +5264,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>261</v>
+        <v>181</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>311</v>
@@ -5165,7 +5279,7 @@
         <v>178</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>110</v>
@@ -5194,25 +5308,25 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>67</v>
+        <v>318</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>44</v>
@@ -5221,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>30</v>
@@ -5238,25 +5352,25 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>107</v>
+        <v>319</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>44</v>
@@ -5265,10 +5379,10 @@
         <v>0</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L75" s="6" t="s">
         <v>311</v>
@@ -5282,13 +5396,13 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>311</v>
@@ -5297,10 +5411,10 @@
         <v>178</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>110</v>
+        <v>313</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>44</v>
@@ -5309,10 +5423,10 @@
         <v>0</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L76" s="6" t="s">
         <v>311</v>
@@ -5326,10 +5440,10 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>184</v>
@@ -5341,10 +5455,10 @@
         <v>178</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>189</v>
+        <v>313</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>44</v>
@@ -5353,10 +5467,10 @@
         <v>0</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L77" s="6" t="s">
         <v>311</v>
@@ -5370,13 +5484,13 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>254</v>
+        <v>60</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>311</v>
@@ -5385,16 +5499,16 @@
         <v>178</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I78" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" s="6" t="s">
         <v>29</v>
@@ -5405,8 +5519,8 @@
       <c r="L78" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="M78" s="5" t="b">
-        <v>1</v>
+      <c r="M78" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="N78" s="6" t="s">
         <v>170</v>
@@ -5414,13 +5528,13 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>185</v>
+        <v>261</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>311</v>
@@ -5429,10 +5543,10 @@
         <v>178</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>44</v>
@@ -5441,16 +5555,16 @@
         <v>0</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L79" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M79" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N79" s="6" t="s">
         <v>170</v>
@@ -5458,10 +5572,10 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>255</v>
+        <v>64</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>256</v>
+        <v>95</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>261</v>
@@ -5473,13 +5587,13 @@
         <v>178</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>262</v>
+        <v>65</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I80" s="6" t="b">
         <v>0</v>
@@ -5494,21 +5608,21 @@
         <v>311</v>
       </c>
       <c r="M80" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N80" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>257</v>
+        <v>66</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>258</v>
+        <v>106</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>311</v>
@@ -5517,13 +5631,13 @@
         <v>178</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>263</v>
+        <v>67</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I81" s="6" t="b">
         <v>0</v>
@@ -5538,21 +5652,21 @@
         <v>311</v>
       </c>
       <c r="M81" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>259</v>
+        <v>68</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>260</v>
+        <v>108</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>311</v>
@@ -5561,42 +5675,42 @@
         <v>178</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>264</v>
+        <v>107</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I82" s="6" t="b">
         <v>0</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L82" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M82" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N82" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>268</v>
+        <v>69</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>266</v>
+        <v>109</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>311</v>
@@ -5605,10 +5719,10 @@
         <v>178</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>267</v>
+        <v>70</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>44</v>
@@ -5634,13 +5748,13 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>269</v>
+        <v>96</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>280</v>
+        <v>97</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>265</v>
+        <v>184</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>311</v>
@@ -5649,10 +5763,10 @@
         <v>178</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>270</v>
+        <v>98</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>44</v>
@@ -5678,10 +5792,10 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>277</v>
+        <v>99</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>181</v>
@@ -5693,7 +5807,7 @@
         <v>178</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>279</v>
+        <v>100</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>110</v>
@@ -5705,10 +5819,10 @@
         <v>0</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>311</v>
@@ -5720,19 +5834,371 @@
         <v>170</v>
       </c>
     </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I86" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L86" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M86" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N86" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I87" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K87" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L87" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M87" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I88" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M88" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N88" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I89" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M89" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N89" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I90" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L90" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M90" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N90" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I91" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J91" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L91" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M91" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N91" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H92" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I92" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J92" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K92" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M92" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N92" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I93" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K93" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L93" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M93" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N93" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:N85">
-    <cfRule type="expression" dxfId="6" priority="3">
+  <conditionalFormatting sqref="N2:N93">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M85">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="M2:M93">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8909,17 +9375,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M88">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$L2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L88">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$G2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added JOLTS data to model input (v0.11)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0463BB7A-9BB6-407E-B354-2C4ADEE6C361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C3CAB-D32B-436E-979F-A85516F0190C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="361">
   <si>
     <t>gdp</t>
   </si>
@@ -1102,6 +1102,24 @@
   </si>
   <si>
     <t>Manufacturers New Orders: Durable Goods</t>
+  </si>
+  <si>
+    <t>jolts</t>
+  </si>
+  <si>
+    <t>Job Openings: Total Nonfarm</t>
+  </si>
+  <si>
+    <t>JTSJOL</t>
+  </si>
+  <si>
+    <t>joltshires</t>
+  </si>
+  <si>
+    <t>Hires: Total Nonfarm</t>
+  </si>
+  <si>
+    <t>JTSHIL</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1747,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N93" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:N93" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N95" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:N95" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="34"/>
     <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="33"/>
@@ -2070,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
-  <dimension ref="A1:N93"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5264,13 +5282,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>51</v>
+        <v>355</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>89</v>
+        <v>356</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>311</v>
@@ -5279,10 +5297,10 @@
         <v>178</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>52</v>
+        <v>357</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>44</v>
@@ -5291,7 +5309,7 @@
         <v>0</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K73" s="6" t="s">
         <v>30</v>
@@ -5308,25 +5326,25 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>53</v>
+        <v>358</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>90</v>
+        <v>359</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>275</v>
+        <v>178</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>318</v>
+        <v>360</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>110</v>
+        <v>344</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>44</v>
@@ -5335,7 +5353,7 @@
         <v>0</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K74" s="6" t="s">
         <v>30</v>
@@ -5352,22 +5370,22 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>261</v>
+        <v>181</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>275</v>
+        <v>178</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>319</v>
+        <v>52</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>110</v>
@@ -5396,25 +5414,25 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>57</v>
+        <v>318</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>44</v>
@@ -5426,7 +5444,7 @@
         <v>29</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L76" s="6" t="s">
         <v>311</v>
@@ -5440,25 +5458,25 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>311</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>178</v>
+        <v>275</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>59</v>
+        <v>319</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>313</v>
+        <v>110</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>44</v>
@@ -5467,10 +5485,10 @@
         <v>0</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L77" s="6" t="s">
         <v>311</v>
@@ -5484,10 +5502,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>182</v>
@@ -5499,28 +5517,28 @@
         <v>178</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>220</v>
+        <v>313</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I78" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M78" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="J78" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L78" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="M78" s="6" t="b">
-        <v>0</v>
       </c>
       <c r="N78" s="6" t="s">
         <v>170</v>
@@ -5528,13 +5546,13 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>311</v>
@@ -5543,10 +5561,10 @@
         <v>178</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>110</v>
+        <v>313</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>44</v>
@@ -5555,10 +5573,10 @@
         <v>0</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L79" s="6" t="s">
         <v>311</v>
@@ -5572,13 +5590,13 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>261</v>
+        <v>182</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>311</v>
@@ -5587,28 +5605,28 @@
         <v>178</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I80" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L80" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="M80" s="5" t="b">
-        <v>1</v>
+      <c r="M80" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="N80" s="6" t="s">
         <v>170</v>
@@ -5616,13 +5634,13 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>311</v>
@@ -5631,10 +5649,10 @@
         <v>178</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>44</v>
@@ -5660,13 +5678,13 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>184</v>
+        <v>261</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>311</v>
@@ -5675,10 +5693,10 @@
         <v>178</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>44</v>
@@ -5687,10 +5705,10 @@
         <v>0</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L82" s="6" t="s">
         <v>311</v>
@@ -5704,10 +5722,10 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>278</v>
@@ -5719,10 +5737,10 @@
         <v>178</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>44</v>
@@ -5748,10 +5766,10 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>184</v>
@@ -5763,10 +5781,10 @@
         <v>178</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>44</v>
@@ -5775,10 +5793,10 @@
         <v>0</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L84" s="6" t="s">
         <v>311</v>
@@ -5792,13 +5810,13 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>181</v>
+        <v>278</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>311</v>
@@ -5807,7 +5825,7 @@
         <v>178</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>110</v>
@@ -5819,10 +5837,10 @@
         <v>0</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>311</v>
@@ -5836,13 +5854,13 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>311</v>
@@ -5851,10 +5869,10 @@
         <v>178</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>44</v>
@@ -5863,10 +5881,10 @@
         <v>0</v>
       </c>
       <c r="J86" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K86" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L86" s="6" t="s">
         <v>311</v>
@@ -5880,13 +5898,13 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>256</v>
+        <v>99</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>261</v>
+        <v>181</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>311</v>
@@ -5895,42 +5913,42 @@
         <v>178</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>262</v>
+        <v>100</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I87" s="6" t="b">
         <v>0</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L87" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M87" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>257</v>
+        <v>112</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>258</v>
+        <v>114</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>261</v>
+        <v>185</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>311</v>
@@ -5939,39 +5957,39 @@
         <v>178</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>263</v>
+        <v>113</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I88" s="6" t="b">
         <v>0</v>
       </c>
       <c r="J88" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L88" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M88" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>261</v>
@@ -5983,7 +6001,7 @@
         <v>178</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>105</v>
@@ -6012,13 +6030,13 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>320</v>
+        <v>257</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>311</v>
@@ -6027,13 +6045,13 @@
         <v>178</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I90" s="6" t="b">
         <v>0</v>
@@ -6048,21 +6066,21 @@
         <v>311</v>
       </c>
       <c r="M90" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>321</v>
+        <v>259</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>325</v>
+        <v>260</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>311</v>
@@ -6071,13 +6089,13 @@
         <v>178</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I91" s="6" t="b">
         <v>0</v>
@@ -6092,18 +6110,18 @@
         <v>311</v>
       </c>
       <c r="M91" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N91" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>323</v>
+        <v>266</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>265</v>
@@ -6115,7 +6133,7 @@
         <v>178</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>324</v>
+        <v>267</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>110</v>
@@ -6144,13 +6162,13 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>277</v>
+        <v>325</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>181</v>
+        <v>265</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>311</v>
@@ -6159,7 +6177,7 @@
         <v>178</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>110</v>
@@ -6186,13 +6204,101 @@
         <v>170</v>
       </c>
     </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I94" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J94" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K94" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L94" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M94" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N94" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I95" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J95" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K95" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L95" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M95" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N95" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:N93">
+  <conditionalFormatting sqref="N2:N95">
     <cfRule type="expression" dxfId="5" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M93">
+  <conditionalFormatting sqref="M2:M95">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added elastic net regularization process to covariate selection for quarterly DFMs (v0.11)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276C3CAB-D32B-436E-979F-A85516F0190C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837DE5D1-F9C5-43A0-8251-67A51A6EE41F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="371">
   <si>
     <t>gdp</t>
   </si>
@@ -1120,6 +1120,36 @@
   </si>
   <si>
     <t>JTSHIL</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>Crude Oil Price (West Texas Intermediate)</t>
+  </si>
+  <si>
+    <t>DCOILWTICO</t>
+  </si>
+  <si>
+    <t>dollars per barrel</t>
+  </si>
+  <si>
+    <t>baa</t>
+  </si>
+  <si>
+    <t>Baa Corporate Bond Yield</t>
+  </si>
+  <si>
+    <t>DBAA</t>
+  </si>
+  <si>
+    <t>lfpr</t>
+  </si>
+  <si>
+    <t>Labor Force Participation Rate</t>
+  </si>
+  <si>
+    <t>CIVPART</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1217,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="9"/>
@@ -1747,45 +1791,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N95" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:N95" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N98" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="A1:N98" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="32"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="25"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:M88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2088,10 +2132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
-  <dimension ref="A1:N95"/>
+  <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5274,7 +5318,7 @@
         <v>311</v>
       </c>
       <c r="M72" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N72" s="6" t="s">
         <v>170</v>
@@ -5318,7 +5362,7 @@
         <v>311</v>
       </c>
       <c r="M73" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N73" s="6" t="s">
         <v>170</v>
@@ -5502,13 +5546,13 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>56</v>
+        <v>361</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>91</v>
+        <v>362</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>311</v>
@@ -5517,10 +5561,10 @@
         <v>178</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>57</v>
+        <v>363</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>313</v>
+        <v>364</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>44</v>
@@ -5529,10 +5573,10 @@
         <v>0</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K78" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L78" s="6" t="s">
         <v>311</v>
@@ -5546,13 +5590,13 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>311</v>
@@ -5561,7 +5605,7 @@
         <v>178</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>313</v>
@@ -5590,13 +5634,13 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>311</v>
@@ -5605,28 +5649,28 @@
         <v>178</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>220</v>
+        <v>313</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I80" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K80" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L80" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M80" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="J80" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K80" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L80" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="M80" s="6" t="b">
-        <v>0</v>
       </c>
       <c r="N80" s="6" t="s">
         <v>170</v>
@@ -5634,13 +5678,13 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>261</v>
+        <v>182</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>311</v>
@@ -5649,28 +5693,28 @@
         <v>178</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I81" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L81" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="M81" s="5" t="b">
-        <v>1</v>
+      <c r="M81" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="N81" s="6" t="s">
         <v>170</v>
@@ -5678,10 +5722,10 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>261</v>
@@ -5693,7 +5737,7 @@
         <v>178</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G82" s="7" t="s">
         <v>110</v>
@@ -5722,13 +5766,13 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>311</v>
@@ -5737,10 +5781,10 @@
         <v>178</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>44</v>
@@ -5766,13 +5810,13 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>184</v>
+        <v>278</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>311</v>
@@ -5781,10 +5825,10 @@
         <v>178</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>44</v>
@@ -5793,10 +5837,10 @@
         <v>0</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L84" s="6" t="s">
         <v>311</v>
@@ -5810,13 +5854,13 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>278</v>
+        <v>184</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>311</v>
@@ -5825,10 +5869,10 @@
         <v>178</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H85" s="6" t="s">
         <v>44</v>
@@ -5837,10 +5881,10 @@
         <v>0</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>311</v>
@@ -5854,13 +5898,13 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>184</v>
+        <v>278</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>311</v>
@@ -5869,10 +5913,10 @@
         <v>178</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>189</v>
+        <v>110</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>44</v>
@@ -5898,13 +5942,13 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>254</v>
+        <v>96</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>311</v>
@@ -5913,10 +5957,10 @@
         <v>178</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>110</v>
+        <v>189</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>44</v>
@@ -5925,10 +5969,10 @@
         <v>0</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K87" s="6" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="L87" s="6" t="s">
         <v>311</v>
@@ -5942,13 +5986,13 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>112</v>
+        <v>254</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>311</v>
@@ -5957,10 +6001,10 @@
         <v>178</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>44</v>
@@ -5986,13 +6030,13 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>255</v>
+        <v>112</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>256</v>
+        <v>114</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>261</v>
+        <v>185</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>311</v>
@@ -6001,39 +6045,39 @@
         <v>178</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>262</v>
+        <v>113</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I89" s="6" t="b">
         <v>0</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K89" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="L89" s="6" t="s">
         <v>311</v>
       </c>
       <c r="M89" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>261</v>
@@ -6045,7 +6089,7 @@
         <v>178</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>105</v>
@@ -6074,10 +6118,10 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>261</v>
@@ -6089,7 +6133,7 @@
         <v>178</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>105</v>
@@ -6118,13 +6162,13 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>311</v>
@@ -6133,13 +6177,13 @@
         <v>178</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I92" s="6" t="b">
         <v>0</v>
@@ -6154,18 +6198,18 @@
         <v>311</v>
       </c>
       <c r="M92" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>325</v>
+        <v>266</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>265</v>
@@ -6177,7 +6221,7 @@
         <v>178</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>110</v>
@@ -6206,10 +6250,10 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>265</v>
@@ -6221,7 +6265,7 @@
         <v>178</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>324</v>
+        <v>270</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>110</v>
@@ -6250,13 +6294,13 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>276</v>
+        <v>322</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>181</v>
+        <v>265</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>311</v>
@@ -6265,7 +6309,7 @@
         <v>178</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>279</v>
+        <v>324</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>110</v>
@@ -6292,19 +6336,151 @@
         <v>170</v>
       </c>
     </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I96" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J96" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K96" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M96" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N96" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I97" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J97" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K97" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L97" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M97" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N97" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I98" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L98" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="M98" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N98" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:N95">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="N2:N98">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M95">
-    <cfRule type="expression" dxfId="4" priority="2">
+  <conditionalFormatting sqref="M2:M98">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9481,17 +9657,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M88">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$L2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L88">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$G2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added trailing inflation (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6FD2A3-85D3-460C-9DC5-61A8302BE096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48FDC19-5E6C-4A24-8B14-9709C315030F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
     <sheet name="baseline-variables" sheetId="5" r:id="rId2"/>
-    <sheet name="baseline-forecasts" sheetId="3" r:id="rId3"/>
+    <sheet name="external-forecasts" sheetId="3" r:id="rId3"/>
     <sheet name="etc" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="415">
   <si>
     <t>gdp</t>
   </si>
@@ -1273,6 +1273,15 @@
   </si>
   <si>
     <t>pchg</t>
+  </si>
+  <si>
+    <t>dns1</t>
+  </si>
+  <si>
+    <t>dns2</t>
+  </si>
+  <si>
+    <t>dns3</t>
   </si>
 </sst>
 </file>
@@ -1347,39 +1356,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <font>
-        <color theme="9"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1399,20 +1389,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1624,6 +1600,13 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1888,6 +1871,25 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1902,45 +1904,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="forecasters" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="forecasters" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6537,17 +6539,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="34" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="33" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6564,7 +6566,7 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7346,14 +7348,23 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>412</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>413</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>414</v>
+      </c>
       <c r="D25" s="5"/>
       <c r="F25" s="6"/>
     </row>
@@ -7613,7 +7624,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L2:L9999">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>AND($G2 &lt;&gt;"d", $G2 &lt;&gt; "w")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added calculation of full DNS history (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48FDC19-5E6C-4A24-8B14-9709C315030F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EA5C51-7544-4AC9-A874-CADF672C3244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="418">
   <si>
     <t>gdp</t>
   </si>
@@ -1275,13 +1275,22 @@
     <t>pchg</t>
   </si>
   <si>
-    <t>dns1</t>
-  </si>
-  <si>
-    <t>dns2</t>
-  </si>
-  <si>
-    <t>dns3</t>
+    <t>tdns1</t>
+  </si>
+  <si>
+    <t>tdns2</t>
+  </si>
+  <si>
+    <t>tdns3</t>
+  </si>
+  <si>
+    <t>Treasury-FFR Spread Level (10-Year Level)</t>
+  </si>
+  <si>
+    <t>Treasury-FFR Spread Slope (Negative of 10Y-3M Spread)</t>
+  </si>
+  <si>
+    <t>Treasury-FFR Spread Curvature</t>
   </si>
 </sst>
 </file>
@@ -6566,7 +6575,7 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7351,22 +7360,88 @@
       <c r="A23" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="F23" s="6"/>
+      <c r="B23" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="F24" s="6"/>
+      <c r="B24" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="F25" s="6"/>
+      <c r="B25" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D26" s="5"/>

</xml_diff>

<commit_message>
Added model flow docs and DNS forecasts (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE66744-7CF6-420F-89B8-FE32EB361C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6C2E5E-B9DE-46BD-AE22-43745426DFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="433">
   <si>
     <t>gdp</t>
   </si>
@@ -1333,6 +1333,9 @@
   </si>
   <si>
     <t>use_nowcast</t>
+  </si>
+  <si>
+    <t>DGS1</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1416,56 +1419,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <fill>
         <patternFill>
@@ -1521,44 +1482,49 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1704,6 +1670,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2086,49 +2071,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="41"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="37"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Q30" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A1:Q30" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Q31" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:Q31" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{76C1F842-CBA6-48BF-9BF9-40A610019A16}" name="initial_forecast" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nowcast.method" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{2DF3733D-2972-4623-B6A5-9F29AA386FF9}" name="use_nowcast" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{76C1F842-CBA6-48BF-9BF9-40A610019A16}" name="initial_forecast" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="dfm_input" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nowcast.method" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{2DF3733D-2972-4623-B6A5-9F29AA386FF9}" name="use_nowcast" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2141,7 +2126,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2447,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:N97"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5258,7 +5243,7 @@
         <v>158</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>21</v>
+        <v>432</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>91</v>
@@ -6739,17 +6724,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6763,10 +6748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6911,7 +6896,9 @@
       <c r="M3" s="4">
         <v>1</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -7125,7 +7112,7 @@
         <v>158</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>21</v>
+        <v>432</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>91</v>
@@ -7529,7 +7516,9 @@
       <c r="L19" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="N19" s="6"/>
+      <c r="N19" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -7562,7 +7551,9 @@
       <c r="L20" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="N20" s="6"/>
+      <c r="N20" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
@@ -7601,7 +7592,9 @@
       <c r="M21" s="4">
         <v>1</v>
       </c>
-      <c r="N21" s="6"/>
+      <c r="N21" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -7706,7 +7699,9 @@
       <c r="L24" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="N24" s="6"/>
+      <c r="N24" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -7772,7 +7767,9 @@
       <c r="L26" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="N26" s="6"/>
+      <c r="N26" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
@@ -7805,7 +7802,9 @@
       <c r="L27" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="N27" s="6"/>
+      <c r="N27" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -7877,31 +7876,109 @@
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="E30" s="4"/>
-      <c r="G30" s="5"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
+      <c r="A30" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="N30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P30" s="10"/>
       <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="N31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="M2:M9941">
-    <cfRule type="expression" dxfId="8" priority="6">
+  <conditionalFormatting sqref="M2:M9942">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>OR($H2="q", $H2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7918,7 +7995,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Instead of forecasting Diebold-Li factors, use Diebold-Li to generate external only and use qual adjustments to generate initial forecasts (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B9491E-6859-47D9-8DA2-756031BFDB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF14CB-D9F2-43A8-91AB-3917F1885A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="all-variables" sheetId="5" r:id="rId3"/>
     <sheet name="ext-forecasts" sheetId="7" r:id="rId4"/>
     <sheet name="initial-forecasts-qual" sheetId="1" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="474">
   <si>
     <t>gdp</t>
   </si>
@@ -1285,15 +1286,6 @@
     <t>2024Q4</t>
   </si>
   <si>
-    <t>t10y3mspread</t>
-  </si>
-  <si>
-    <t>tffr3mspread</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>Treasury Bill - FFR Spread</t>
   </si>
   <si>
@@ -1457,6 +1449,18 @@
   </si>
   <si>
     <t>[cme]-.25</t>
+  </si>
+  <si>
+    <t>inf.d1_baseline</t>
+  </si>
+  <si>
+    <t>inf.d1_strong</t>
+  </si>
+  <si>
+    <t>tdns1.d1_baseline</t>
+  </si>
+  <si>
+    <t>[cmef.tdns1]</t>
   </si>
 </sst>
 </file>
@@ -1580,140 +1584,6 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1967,6 +1837,25 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1998,6 +1887,25 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2127,6 +2035,83 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2394,6 +2379,25 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2414,23 +2418,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2443,7 +2447,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="38"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2451,33 +2455,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X110" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X110" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:X110" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="35"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="27"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="26"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="24"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="23"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="21"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="18"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="21"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2490,7 +2494,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5607,7 +5611,7 @@
         <v>156</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>89</v>
@@ -7088,17 +7092,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="57" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="56" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7115,7 +7119,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7377,7 +7381,7 @@
   <dimension ref="A1:X110"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7414,7 +7418,7 @@
         <v>286</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>155</v>
@@ -7444,34 +7448,34 @@
         <v>289</v>
       </c>
       <c r="O1" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>431</v>
-      </c>
       <c r="S1" s="8" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="T1" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>440</v>
-      </c>
       <c r="X1" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -7503,7 +7507,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>15</v>
@@ -7542,7 +7546,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>159</v>
@@ -7566,7 +7570,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>15</v>
@@ -7617,7 +7621,7 @@
         <v>18</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>15</v>
@@ -7662,7 +7666,7 @@
         <v>18</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>15</v>
@@ -7707,7 +7711,7 @@
         <v>18</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>15</v>
@@ -7752,7 +7756,7 @@
         <v>18</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>15</v>
@@ -7797,7 +7801,7 @@
         <v>18</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>15</v>
@@ -7842,7 +7846,7 @@
         <v>18</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>15</v>
@@ -7887,7 +7891,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>15</v>
@@ -7932,7 +7936,7 @@
         <v>18</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>15</v>
@@ -7977,7 +7981,7 @@
         <v>18</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>15</v>
@@ -8022,7 +8026,7 @@
         <v>18</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>15</v>
@@ -8067,7 +8071,7 @@
         <v>18</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>15</v>
@@ -8112,7 +8116,7 @@
         <v>18</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>15</v>
@@ -8157,7 +8161,7 @@
         <v>18</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>15</v>
@@ -8202,7 +8206,7 @@
         <v>18</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>15</v>
@@ -8247,7 +8251,7 @@
         <v>18</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>15</v>
@@ -8292,7 +8296,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>15</v>
@@ -8337,7 +8341,7 @@
         <v>18</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>15</v>
@@ -8382,7 +8386,7 @@
         <v>18</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>15</v>
@@ -8427,7 +8431,7 @@
         <v>18</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>15</v>
@@ -8472,7 +8476,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>15</v>
@@ -8517,7 +8521,7 @@
         <v>18</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>15</v>
@@ -8562,7 +8566,7 @@
         <v>18</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>15</v>
@@ -8607,7 +8611,7 @@
         <v>18</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L26" s="10" t="s">
         <v>15</v>
@@ -8652,7 +8656,7 @@
         <v>18</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>15</v>
@@ -8697,7 +8701,7 @@
         <v>18</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>15</v>
@@ -8742,7 +8746,7 @@
         <v>18</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>15</v>
@@ -8787,7 +8791,7 @@
         <v>18</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>16</v>
@@ -8832,7 +8836,7 @@
         <v>18</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>16</v>
@@ -8877,7 +8881,7 @@
         <v>18</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>15</v>
@@ -8922,7 +8926,7 @@
         <v>18</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L33" s="10" t="s">
         <v>15</v>
@@ -8967,7 +8971,7 @@
         <v>18</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L34" s="10" t="s">
         <v>15</v>
@@ -9012,7 +9016,7 @@
         <v>18</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L35" s="10" t="s">
         <v>15</v>
@@ -9057,7 +9061,7 @@
         <v>18</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L36" s="10" t="s">
         <v>15</v>
@@ -9102,7 +9106,7 @@
         <v>18</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L37" s="10" t="s">
         <v>15</v>
@@ -9147,7 +9151,7 @@
         <v>18</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>15</v>
@@ -9192,7 +9196,7 @@
         <v>18</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>15</v>
@@ -9237,7 +9241,7 @@
         <v>18</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>15</v>
@@ -9264,7 +9268,7 @@
         <v>162</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>156</v>
@@ -9279,7 +9283,7 @@
         <v>30</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>15</v>
@@ -9308,7 +9312,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>156</v>
@@ -9323,7 +9327,7 @@
         <v>30</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>15</v>
@@ -9352,7 +9356,7 @@
         <v>162</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>156</v>
@@ -9367,7 +9371,7 @@
         <v>30</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>15</v>
@@ -9396,7 +9400,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>156</v>
@@ -9411,7 +9415,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>15</v>
@@ -9440,7 +9444,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>156</v>
@@ -9455,7 +9459,7 @@
         <v>30</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>15</v>
@@ -9502,7 +9506,7 @@
         <v>30</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>15</v>
@@ -9549,7 +9553,7 @@
         <v>30</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>15</v>
@@ -9596,7 +9600,7 @@
         <v>30</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>16</v>
@@ -9640,7 +9644,7 @@
         <v>30</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>15</v>
@@ -9684,7 +9688,7 @@
         <v>30</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>15</v>
@@ -9728,7 +9732,7 @@
         <v>30</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>15</v>
@@ -9772,7 +9776,7 @@
         <v>30</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>15</v>
@@ -9801,7 +9805,7 @@
         <v>309</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>156</v>
@@ -9816,7 +9820,7 @@
         <v>30</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>15</v>
@@ -9845,7 +9849,7 @@
         <v>309</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>156</v>
@@ -9860,7 +9864,7 @@
         <v>30</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>15</v>
@@ -9889,7 +9893,7 @@
         <v>309</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>156</v>
@@ -9904,7 +9908,7 @@
         <v>30</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>15</v>
@@ -9933,7 +9937,7 @@
         <v>162</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>156</v>
@@ -9948,7 +9952,7 @@
         <v>30</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>16</v>
@@ -9977,7 +9981,7 @@
         <v>253</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>156</v>
@@ -9992,7 +9996,7 @@
         <v>30</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>15</v>
@@ -10021,7 +10025,7 @@
         <v>253</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>156</v>
@@ -10036,7 +10040,7 @@
         <v>30</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>15</v>
@@ -10065,7 +10069,7 @@
         <v>253</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>156</v>
@@ -10080,7 +10084,7 @@
         <v>30</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L59" s="10" t="s">
         <v>15</v>
@@ -10109,7 +10113,7 @@
         <v>159</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>156</v>
@@ -10124,7 +10128,7 @@
         <v>30</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>16</v>
@@ -10153,7 +10157,7 @@
         <v>238</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>156</v>
@@ -10168,7 +10172,7 @@
         <v>30</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>16</v>
@@ -10197,7 +10201,7 @@
         <v>160</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>156</v>
@@ -10212,7 +10216,7 @@
         <v>30</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>15</v>
@@ -10241,7 +10245,7 @@
         <v>162</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>156</v>
@@ -10256,7 +10260,7 @@
         <v>30</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>15</v>
@@ -10285,7 +10289,7 @@
         <v>238</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>156</v>
@@ -10300,7 +10304,7 @@
         <v>30</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>16</v>
@@ -10329,7 +10333,7 @@
         <v>238</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>156</v>
@@ -10344,7 +10348,7 @@
         <v>30</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>16</v>
@@ -10373,7 +10377,7 @@
         <v>253</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>156</v>
@@ -10388,7 +10392,7 @@
         <v>30</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>16</v>
@@ -10417,7 +10421,7 @@
         <v>162</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>156</v>
@@ -10432,7 +10436,7 @@
         <v>30</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>15</v>
@@ -10461,7 +10465,7 @@
         <v>253</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>156</v>
@@ -10476,7 +10480,7 @@
         <v>30</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>16</v>
@@ -10505,7 +10509,7 @@
         <v>162</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F69" s="10" t="s">
         <v>156</v>
@@ -10520,7 +10524,7 @@
         <v>30</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L69" s="10" t="s">
         <v>16</v>
@@ -10549,7 +10553,7 @@
         <v>159</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>156</v>
@@ -10564,7 +10568,7 @@
         <v>30</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>15</v>
@@ -10593,7 +10597,7 @@
         <v>163</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F71" s="10" t="s">
         <v>156</v>
@@ -10608,7 +10612,7 @@
         <v>30</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>15</v>
@@ -10637,7 +10641,7 @@
         <v>238</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F72" s="10" t="s">
         <v>156</v>
@@ -10652,7 +10656,7 @@
         <v>18</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>16</v>
@@ -10679,7 +10683,7 @@
         <v>238</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F73" s="10" t="s">
         <v>156</v>
@@ -10694,7 +10698,7 @@
         <v>18</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>16</v>
@@ -10721,7 +10725,7 @@
         <v>238</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>156</v>
@@ -10736,7 +10740,7 @@
         <v>18</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>16</v>
@@ -10763,7 +10767,7 @@
         <v>242</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F75" s="10" t="s">
         <v>156</v>
@@ -10778,7 +10782,7 @@
         <v>30</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L75" s="10" t="s">
         <v>16</v>
@@ -10807,7 +10811,7 @@
         <v>242</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>156</v>
@@ -10822,7 +10826,7 @@
         <v>30</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L76" s="10" t="s">
         <v>16</v>
@@ -10851,7 +10855,7 @@
         <v>242</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>156</v>
@@ -10866,7 +10870,7 @@
         <v>30</v>
       </c>
       <c r="K77" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L77" s="10" t="s">
         <v>16</v>
@@ -10895,7 +10899,7 @@
         <v>159</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>156</v>
@@ -10910,7 +10914,7 @@
         <v>30</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L78" s="10" t="s">
         <v>16</v>
@@ -10939,7 +10943,7 @@
         <v>161</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>156</v>
@@ -10954,7 +10958,7 @@
         <v>30</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L79" s="10" t="s">
         <v>16</v>
@@ -10983,7 +10987,7 @@
         <v>253</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>156</v>
@@ -10998,7 +11002,7 @@
         <v>30</v>
       </c>
       <c r="K80" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L80" s="10" t="s">
         <v>16</v>
@@ -11027,7 +11031,7 @@
         <v>161</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>156</v>
@@ -11045,7 +11049,7 @@
         <v>1</v>
       </c>
       <c r="K81" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>399</v>
@@ -11063,13 +11067,13 @@
         <v>1</v>
       </c>
       <c r="V81" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W81" s="11">
         <v>1</v>
       </c>
       <c r="X81" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
@@ -11083,7 +11087,7 @@
         <v>161</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>156</v>
@@ -11101,7 +11105,7 @@
         <v>1</v>
       </c>
       <c r="K82" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L82" s="10" t="s">
         <v>399</v>
@@ -11116,13 +11120,13 @@
         <v>1</v>
       </c>
       <c r="V82" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W82" s="11">
         <v>0</v>
       </c>
       <c r="X82" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
@@ -11136,7 +11140,7 @@
         <v>161</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>156</v>
@@ -11154,7 +11158,7 @@
         <v>1</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L83" s="10" t="s">
         <v>399</v>
@@ -11178,7 +11182,7 @@
         <v>1</v>
       </c>
       <c r="X83" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
@@ -11192,7 +11196,7 @@
         <v>161</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>156</v>
@@ -11210,7 +11214,7 @@
         <v>1</v>
       </c>
       <c r="K84" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L84" s="10" t="s">
         <v>399</v>
@@ -11228,7 +11232,7 @@
         <v>0</v>
       </c>
       <c r="X84" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -11242,7 +11246,7 @@
         <v>161</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>156</v>
@@ -11260,7 +11264,7 @@
         <v>1</v>
       </c>
       <c r="K85" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L85" s="10" t="s">
         <v>399</v>
@@ -11278,7 +11282,7 @@
         <v>0</v>
       </c>
       <c r="X85" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
@@ -11292,7 +11296,7 @@
         <v>161</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>156</v>
@@ -11310,7 +11314,7 @@
         <v>1</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L86" s="10" t="s">
         <v>399</v>
@@ -11328,7 +11332,7 @@
         <v>0</v>
       </c>
       <c r="X86" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
@@ -11342,13 +11346,13 @@
         <v>161</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>89</v>
@@ -11360,7 +11364,7 @@
         <v>1</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L87" s="10" t="s">
         <v>399</v>
@@ -11381,7 +11385,7 @@
         <v>1</v>
       </c>
       <c r="X87" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
@@ -11395,7 +11399,7 @@
         <v>161</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>156</v>
@@ -11413,7 +11417,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L88" s="10" t="s">
         <v>399</v>
@@ -11431,7 +11435,7 @@
         <v>0</v>
       </c>
       <c r="X88" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
@@ -11445,7 +11449,7 @@
         <v>161</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>156</v>
@@ -11463,7 +11467,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L89" s="10" t="s">
         <v>399</v>
@@ -11484,7 +11488,7 @@
         <v>0</v>
       </c>
       <c r="X89" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
@@ -11498,7 +11502,7 @@
         <v>161</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>156</v>
@@ -11516,7 +11520,7 @@
         <v>1</v>
       </c>
       <c r="K90" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L90" s="10" t="s">
         <v>399</v>
@@ -11534,7 +11538,7 @@
         <v>0</v>
       </c>
       <c r="X90" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
@@ -11548,7 +11552,7 @@
         <v>161</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>156</v>
@@ -11566,7 +11570,7 @@
         <v>1</v>
       </c>
       <c r="K91" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L91" s="10" t="s">
         <v>399</v>
@@ -11584,7 +11588,7 @@
         <v>0</v>
       </c>
       <c r="X91" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
@@ -11598,7 +11602,7 @@
         <v>161</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F92" s="10" t="s">
         <v>156</v>
@@ -11616,7 +11620,7 @@
         <v>1</v>
       </c>
       <c r="K92" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L92" s="10" t="s">
         <v>399</v>
@@ -11634,7 +11638,7 @@
         <v>0</v>
       </c>
       <c r="X92" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
@@ -11648,7 +11652,7 @@
         <v>314</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>156</v>
@@ -11666,7 +11670,7 @@
         <v>1</v>
       </c>
       <c r="K93" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L93" s="10" t="s">
         <v>399</v>
@@ -11691,7 +11695,7 @@
         <v>314</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>156</v>
@@ -11709,7 +11713,7 @@
         <v>1</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L94" s="10" t="s">
         <v>399</v>
@@ -11734,7 +11738,7 @@
         <v>161</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>156</v>
@@ -11752,7 +11756,7 @@
         <v>1</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L95" s="10" t="s">
         <v>399</v>
@@ -11777,7 +11781,7 @@
         <v>314</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F96" s="10" t="s">
         <v>156</v>
@@ -11792,7 +11796,7 @@
         <v>30</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L96" s="10" t="s">
         <v>15</v>
@@ -11817,7 +11821,7 @@
         <v>163</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>156</v>
@@ -11832,7 +11836,7 @@
         <v>30</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>101</v>
@@ -11860,7 +11864,7 @@
         <v>163</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>171</v>
@@ -11872,7 +11876,7 @@
         <v>30</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>16</v>
@@ -11887,7 +11891,7 @@
         <v>1</v>
       </c>
       <c r="V98" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W98" s="11"/>
       <c r="X98" s="12"/>
@@ -11903,7 +11907,7 @@
         <v>238</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F99" s="10" t="s">
         <v>250</v>
@@ -11921,7 +11925,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L99" s="10" t="s">
         <v>15</v>
@@ -11933,7 +11937,7 @@
         <v>16</v>
       </c>
       <c r="V99" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W99" s="11">
         <v>1</v>
@@ -11953,7 +11957,7 @@
         <v>238</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F100" s="10" t="s">
         <v>250</v>
@@ -11971,7 +11975,7 @@
         <v>1</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>16</v>
@@ -12000,7 +12004,7 @@
         <v>161</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F101" s="10" t="s">
         <v>171</v>
@@ -12012,7 +12016,7 @@
         <v>30</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>399</v>
@@ -12024,7 +12028,7 @@
         <v>283</v>
       </c>
       <c r="V101" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W101" s="11"/>
       <c r="X101" s="12"/>
@@ -12040,7 +12044,7 @@
         <v>161</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F102" s="10" t="s">
         <v>171</v>
@@ -12052,7 +12056,7 @@
         <v>30</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L102" s="10" t="s">
         <v>399</v>
@@ -12064,7 +12068,7 @@
         <v>283</v>
       </c>
       <c r="V102" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W102" s="11"/>
       <c r="X102" s="12"/>
@@ -12080,7 +12084,7 @@
         <v>161</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>171</v>
@@ -12092,7 +12096,7 @@
         <v>30</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L103" s="10" t="s">
         <v>399</v>
@@ -12104,23 +12108,23 @@
         <v>283</v>
       </c>
       <c r="V103" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W103" s="11"/>
       <c r="X103" s="12"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>171</v>
@@ -12132,7 +12136,7 @@
         <v>30</v>
       </c>
       <c r="K104" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L104" s="10" t="s">
         <v>399</v>
@@ -12148,16 +12152,16 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F105" s="10" t="s">
         <v>171</v>
@@ -12169,7 +12173,7 @@
         <v>30</v>
       </c>
       <c r="K105" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L105" s="10" t="s">
         <v>399</v>
@@ -12185,16 +12189,16 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B106" s="9" t="s">
         <v>422</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>425</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>314</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F106" s="10" t="s">
         <v>171</v>
@@ -12206,7 +12210,7 @@
         <v>30</v>
       </c>
       <c r="K106" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L106" s="10" t="s">
         <v>399</v>
@@ -12222,16 +12226,16 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>314</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>171</v>
@@ -12243,7 +12247,7 @@
         <v>30</v>
       </c>
       <c r="K107" s="10" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="L107" s="10" t="s">
         <v>399</v>
@@ -12286,7 +12290,7 @@
         <v>30</v>
       </c>
       <c r="K108" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L108" s="10" t="s">
         <v>15</v>
@@ -12304,12 +12308,12 @@
         <v>0</v>
       </c>
       <c r="X108" s="11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>222</v>
@@ -12336,7 +12340,7 @@
         <v>30</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>15</v>
@@ -12348,13 +12352,13 @@
         <v>283</v>
       </c>
       <c r="V109" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W109" s="11">
         <v>1</v>
       </c>
       <c r="X109" s="11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
@@ -12368,7 +12372,7 @@
         <v>253</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="F110" s="10" t="s">
         <v>156</v>
@@ -12383,7 +12387,7 @@
         <v>30</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>15</v>
@@ -12401,54 +12405,54 @@
         <v>1</v>
       </c>
       <c r="V110" s="10" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="W110" s="11">
         <v>1</v>
       </c>
       <c r="X110" s="11" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I1:J110">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W111:W10020">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="33" priority="6">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G110">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="32" priority="5">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V110">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J110">
-    <cfRule type="expression" dxfId="1" priority="15">
+    <cfRule type="expression" dxfId="28" priority="15">
       <formula>OR($I2="q", $I2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12465,7 +12469,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W110">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>AND($I2&lt;&gt;"d", $I2 &lt;&gt; "w", $I2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12504,7 +12508,7 @@
         <v>56</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="E1" t="s">
         <v>355</v>
@@ -12677,7 +12681,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -12694,7 +12698,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -12711,7 +12715,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -12726,8 +12730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E828C45D-CF7B-424F-B36C-220BE51A990F}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12738,668 +12742,638 @@
     <col min="14" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>446</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>447</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>450</v>
+      <c r="H1" s="15" t="s">
+        <v>470</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>39</v>
+        <v>471</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>31</v>
+        <v>471</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>400</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="G2" s="16"/>
+        <v>467</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K2" s="15">
-        <v>1</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I2" s="17"/>
+      <c r="K2" s="15" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>401</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="G3" s="16"/>
+        <v>467</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K3" s="15">
-        <v>1</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>402</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="G4" s="16"/>
+        <v>467</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K4" s="15">
-        <v>1</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>403</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="G5" s="16"/>
+        <v>467</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>404</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="G6" s="16"/>
+        <v>468</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>405</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="G7" s="16"/>
+        <v>468</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>406</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>471</v>
-      </c>
-      <c r="G8" s="16"/>
+        <v>468</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>407</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E9" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F9" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>408</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E10" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F10" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>409</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E11" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F11" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G11" s="16"/>
       <c r="H11" s="16"/>
-      <c r="I11" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>410</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E12" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F12" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G12" s="16"/>
       <c r="H12" s="16"/>
-      <c r="I12" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>411</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E13" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F13" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G13" s="16"/>
       <c r="H13" s="16"/>
-      <c r="I13" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>412</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E14" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F14" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G14" s="16"/>
       <c r="H14" s="16"/>
-      <c r="I14" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>413</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E15" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F15" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G15" s="16"/>
       <c r="H15" s="16"/>
-      <c r="I15" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>414</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="E16" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="F16" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="G16" s="16"/>
       <c r="H16" s="16"/>
-      <c r="I16" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C17" s="16" t="s">
+      <c r="B20" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F17" s="16" t="s">
+      <c r="E20" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C18" s="16" t="s">
+      <c r="B22" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="E22" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C19" s="16" t="s">
+      <c r="B23" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F19" s="16" t="s">
+      <c r="E23" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C20" s="16" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F20" s="16" t="s">
+      <c r="E24" s="16" t="s">
+        <v>467</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>466</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>469</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>455</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>469</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
-        <v>456</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>469</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>469</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>470</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
         <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
-        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -13407,4 +13381,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624AEEDB-BBA7-44A6-A6FF-0B28C3344004}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added external forecasts for Diebold-Li factors (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FF14CB-D9F2-43A8-91AB-3917F1885A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA63D056-6B40-4870-9062-EC8F7419AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="473">
   <si>
     <t>gdp</t>
   </si>
@@ -1241,51 +1241,6 @@
     <t>diff1</t>
   </si>
   <si>
-    <t>2021Q2</t>
-  </si>
-  <si>
-    <t>2021Q3</t>
-  </si>
-  <si>
-    <t>2021Q4</t>
-  </si>
-  <si>
-    <t>2022Q1</t>
-  </si>
-  <si>
-    <t>2022Q2</t>
-  </si>
-  <si>
-    <t>2022Q3</t>
-  </si>
-  <si>
-    <t>2022Q4</t>
-  </si>
-  <si>
-    <t>2023Q1</t>
-  </si>
-  <si>
-    <t>2023Q2</t>
-  </si>
-  <si>
-    <t>2023Q3</t>
-  </si>
-  <si>
-    <t>2023Q4</t>
-  </si>
-  <si>
-    <t>2024Q1</t>
-  </si>
-  <si>
-    <t>2024Q2</t>
-  </si>
-  <si>
-    <t>2024Q3</t>
-  </si>
-  <si>
-    <t>2024Q4</t>
-  </si>
-  <si>
     <t>Treasury Bill - FFR Spread</t>
   </si>
   <si>
@@ -1385,54 +1340,6 @@
     <t>sofr.d1_weak</t>
   </si>
   <si>
-    <t>2025Q1</t>
-  </si>
-  <si>
-    <t>2025Q2</t>
-  </si>
-  <si>
-    <t>2025Q3</t>
-  </si>
-  <si>
-    <t>2025Q4</t>
-  </si>
-  <si>
-    <t>2026Q2</t>
-  </si>
-  <si>
-    <t>2026Q3</t>
-  </si>
-  <si>
-    <t>2026Q1</t>
-  </si>
-  <si>
-    <t>2026Q4</t>
-  </si>
-  <si>
-    <t>2027Q1</t>
-  </si>
-  <si>
-    <t>2027Q2</t>
-  </si>
-  <si>
-    <t>2027Q3</t>
-  </si>
-  <si>
-    <t>2027Q4</t>
-  </si>
-  <si>
-    <t>2028Q1</t>
-  </si>
-  <si>
-    <t>2028Q2</t>
-  </si>
-  <si>
-    <t>2028Q3</t>
-  </si>
-  <si>
-    <t>2028Q4</t>
-  </si>
-  <si>
     <t>market</t>
   </si>
   <si>
@@ -1457,10 +1364,100 @@
     <t>inf.d1_strong</t>
   </si>
   <si>
-    <t>tdns1.d1_baseline</t>
-  </si>
-  <si>
-    <t>[cmef.tdns1]</t>
+    <t>tdns.d1.baseline</t>
+  </si>
+  <si>
+    <t>2021-06</t>
+  </si>
+  <si>
+    <t>2021-07</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2021-09</t>
+  </si>
+  <si>
+    <t>2021-10</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2021-12</t>
+  </si>
+  <si>
+    <t>2022-01</t>
+  </si>
+  <si>
+    <t>2022-02</t>
+  </si>
+  <si>
+    <t>2022-03</t>
+  </si>
+  <si>
+    <t>2022-04</t>
+  </si>
+  <si>
+    <t>2022-05</t>
+  </si>
+  <si>
+    <t>2022-06</t>
+  </si>
+  <si>
+    <t>2022-07</t>
+  </si>
+  <si>
+    <t>2022-08</t>
+  </si>
+  <si>
+    <t>2022-09</t>
+  </si>
+  <si>
+    <t>2022-10</t>
+  </si>
+  <si>
+    <t>2022-11</t>
+  </si>
+  <si>
+    <t>2022-12</t>
+  </si>
+  <si>
+    <t>2023-01</t>
+  </si>
+  <si>
+    <t>2023-02</t>
+  </si>
+  <si>
+    <t>2023-03</t>
+  </si>
+  <si>
+    <t>2023-04</t>
+  </si>
+  <si>
+    <t>2023-05</t>
+  </si>
+  <si>
+    <t>2023-06</t>
+  </si>
+  <si>
+    <t>2023-07</t>
+  </si>
+  <si>
+    <t>2023-08</t>
+  </si>
+  <si>
+    <t>2023-09</t>
+  </si>
+  <si>
+    <t>2023-10</t>
+  </si>
+  <si>
+    <t>2023-11</t>
+  </si>
+  <si>
+    <t>2023-12</t>
   </si>
 </sst>
 </file>
@@ -1583,6 +1580,102 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2037,83 +2130,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2379,25 +2395,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2418,23 +2415,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="50"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="45"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="46"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2447,7 +2444,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="41"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2455,33 +2452,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X110" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X110" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:X110" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="21"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="5"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="35"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="26"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="25"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="24"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="23"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="22"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="21"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="20"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="19"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="18"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2494,7 +2491,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="14"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5611,7 +5608,7 @@
         <v>156</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>89</v>
@@ -7092,17 +7089,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="57" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="56" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7380,8 +7377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="S103" sqref="S103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7418,7 +7415,7 @@
         <v>286</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>155</v>
@@ -7448,34 +7445,34 @@
         <v>289</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="U1" s="8" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -7507,7 +7504,7 @@
         <v>18</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>15</v>
@@ -7546,7 +7543,7 @@
         <v>85</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>159</v>
@@ -7570,7 +7567,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>15</v>
@@ -7621,7 +7618,7 @@
         <v>18</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>15</v>
@@ -7666,7 +7663,7 @@
         <v>18</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>15</v>
@@ -7711,7 +7708,7 @@
         <v>18</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>15</v>
@@ -7756,7 +7753,7 @@
         <v>18</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>15</v>
@@ -7801,7 +7798,7 @@
         <v>18</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>15</v>
@@ -7846,7 +7843,7 @@
         <v>18</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>15</v>
@@ -7891,7 +7888,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>15</v>
@@ -7936,7 +7933,7 @@
         <v>18</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>15</v>
@@ -7981,7 +7978,7 @@
         <v>18</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>15</v>
@@ -8026,7 +8023,7 @@
         <v>18</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>15</v>
@@ -8071,7 +8068,7 @@
         <v>18</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>15</v>
@@ -8116,7 +8113,7 @@
         <v>18</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>15</v>
@@ -8161,7 +8158,7 @@
         <v>18</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>15</v>
@@ -8206,7 +8203,7 @@
         <v>18</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>15</v>
@@ -8251,7 +8248,7 @@
         <v>18</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>15</v>
@@ -8296,7 +8293,7 @@
         <v>18</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>15</v>
@@ -8341,7 +8338,7 @@
         <v>18</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>15</v>
@@ -8386,7 +8383,7 @@
         <v>18</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>15</v>
@@ -8431,7 +8428,7 @@
         <v>18</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>15</v>
@@ -8476,7 +8473,7 @@
         <v>18</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>15</v>
@@ -8521,7 +8518,7 @@
         <v>18</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>15</v>
@@ -8566,7 +8563,7 @@
         <v>18</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>15</v>
@@ -8611,7 +8608,7 @@
         <v>18</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L26" s="10" t="s">
         <v>15</v>
@@ -8656,7 +8653,7 @@
         <v>18</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>15</v>
@@ -8701,7 +8698,7 @@
         <v>18</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>15</v>
@@ -8746,7 +8743,7 @@
         <v>18</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>15</v>
@@ -8791,7 +8788,7 @@
         <v>18</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>16</v>
@@ -8836,7 +8833,7 @@
         <v>18</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>16</v>
@@ -8881,7 +8878,7 @@
         <v>18</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>15</v>
@@ -8926,7 +8923,7 @@
         <v>18</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L33" s="10" t="s">
         <v>15</v>
@@ -8971,7 +8968,7 @@
         <v>18</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L34" s="10" t="s">
         <v>15</v>
@@ -9016,7 +9013,7 @@
         <v>18</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L35" s="10" t="s">
         <v>15</v>
@@ -9061,7 +9058,7 @@
         <v>18</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L36" s="10" t="s">
         <v>15</v>
@@ -9106,7 +9103,7 @@
         <v>18</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L37" s="10" t="s">
         <v>15</v>
@@ -9151,7 +9148,7 @@
         <v>18</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>15</v>
@@ -9196,7 +9193,7 @@
         <v>18</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>15</v>
@@ -9241,7 +9238,7 @@
         <v>18</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>15</v>
@@ -9268,7 +9265,7 @@
         <v>162</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>156</v>
@@ -9283,7 +9280,7 @@
         <v>30</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>15</v>
@@ -9312,7 +9309,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F42" s="10" t="s">
         <v>156</v>
@@ -9327,7 +9324,7 @@
         <v>30</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>15</v>
@@ -9356,7 +9353,7 @@
         <v>162</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>156</v>
@@ -9371,7 +9368,7 @@
         <v>30</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>15</v>
@@ -9400,7 +9397,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>156</v>
@@ -9415,7 +9412,7 @@
         <v>30</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>15</v>
@@ -9444,7 +9441,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>156</v>
@@ -9459,7 +9456,7 @@
         <v>30</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>15</v>
@@ -9506,7 +9503,7 @@
         <v>30</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>15</v>
@@ -9553,7 +9550,7 @@
         <v>30</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>15</v>
@@ -9600,7 +9597,7 @@
         <v>30</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>16</v>
@@ -9644,7 +9641,7 @@
         <v>30</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>15</v>
@@ -9688,7 +9685,7 @@
         <v>30</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>15</v>
@@ -9732,7 +9729,7 @@
         <v>30</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>15</v>
@@ -9776,7 +9773,7 @@
         <v>30</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>15</v>
@@ -9805,7 +9802,7 @@
         <v>309</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>156</v>
@@ -9820,7 +9817,7 @@
         <v>30</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>15</v>
@@ -9849,7 +9846,7 @@
         <v>309</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>156</v>
@@ -9864,7 +9861,7 @@
         <v>30</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>15</v>
@@ -9893,7 +9890,7 @@
         <v>309</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>156</v>
@@ -9908,7 +9905,7 @@
         <v>30</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>15</v>
@@ -9937,7 +9934,7 @@
         <v>162</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>156</v>
@@ -9952,7 +9949,7 @@
         <v>30</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>16</v>
@@ -9981,7 +9978,7 @@
         <v>253</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>156</v>
@@ -9996,7 +9993,7 @@
         <v>30</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>15</v>
@@ -10025,7 +10022,7 @@
         <v>253</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>156</v>
@@ -10040,7 +10037,7 @@
         <v>30</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>15</v>
@@ -10069,7 +10066,7 @@
         <v>253</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>156</v>
@@ -10084,7 +10081,7 @@
         <v>30</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L59" s="10" t="s">
         <v>15</v>
@@ -10113,7 +10110,7 @@
         <v>159</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>156</v>
@@ -10128,7 +10125,7 @@
         <v>30</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>16</v>
@@ -10157,7 +10154,7 @@
         <v>238</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>156</v>
@@ -10172,7 +10169,7 @@
         <v>30</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>16</v>
@@ -10201,7 +10198,7 @@
         <v>160</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>156</v>
@@ -10216,7 +10213,7 @@
         <v>30</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>15</v>
@@ -10245,7 +10242,7 @@
         <v>162</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>156</v>
@@ -10260,7 +10257,7 @@
         <v>30</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>15</v>
@@ -10289,7 +10286,7 @@
         <v>238</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>156</v>
@@ -10304,7 +10301,7 @@
         <v>30</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>16</v>
@@ -10333,7 +10330,7 @@
         <v>238</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>156</v>
@@ -10348,7 +10345,7 @@
         <v>30</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>16</v>
@@ -10377,7 +10374,7 @@
         <v>253</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F66" s="10" t="s">
         <v>156</v>
@@ -10392,7 +10389,7 @@
         <v>30</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>16</v>
@@ -10421,7 +10418,7 @@
         <v>162</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>156</v>
@@ -10436,7 +10433,7 @@
         <v>30</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>15</v>
@@ -10465,7 +10462,7 @@
         <v>253</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>156</v>
@@ -10480,7 +10477,7 @@
         <v>30</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>16</v>
@@ -10509,7 +10506,7 @@
         <v>162</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F69" s="10" t="s">
         <v>156</v>
@@ -10524,7 +10521,7 @@
         <v>30</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L69" s="10" t="s">
         <v>16</v>
@@ -10553,7 +10550,7 @@
         <v>159</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>156</v>
@@ -10568,7 +10565,7 @@
         <v>30</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>15</v>
@@ -10597,7 +10594,7 @@
         <v>163</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F71" s="10" t="s">
         <v>156</v>
@@ -10612,7 +10609,7 @@
         <v>30</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>15</v>
@@ -10641,7 +10638,7 @@
         <v>238</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F72" s="10" t="s">
         <v>156</v>
@@ -10656,7 +10653,7 @@
         <v>18</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>16</v>
@@ -10683,7 +10680,7 @@
         <v>238</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F73" s="10" t="s">
         <v>156</v>
@@ -10698,7 +10695,7 @@
         <v>18</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>16</v>
@@ -10725,7 +10722,7 @@
         <v>238</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>156</v>
@@ -10740,7 +10737,7 @@
         <v>18</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>16</v>
@@ -10767,7 +10764,7 @@
         <v>242</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F75" s="10" t="s">
         <v>156</v>
@@ -10782,7 +10779,7 @@
         <v>30</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L75" s="10" t="s">
         <v>16</v>
@@ -10811,7 +10808,7 @@
         <v>242</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>156</v>
@@ -10826,7 +10823,7 @@
         <v>30</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L76" s="10" t="s">
         <v>16</v>
@@ -10855,7 +10852,7 @@
         <v>242</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>156</v>
@@ -10870,7 +10867,7 @@
         <v>30</v>
       </c>
       <c r="K77" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L77" s="10" t="s">
         <v>16</v>
@@ -10899,7 +10896,7 @@
         <v>159</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F78" s="10" t="s">
         <v>156</v>
@@ -10914,7 +10911,7 @@
         <v>30</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L78" s="10" t="s">
         <v>16</v>
@@ -10943,7 +10940,7 @@
         <v>161</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>156</v>
@@ -10958,7 +10955,7 @@
         <v>30</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L79" s="10" t="s">
         <v>16</v>
@@ -10987,7 +10984,7 @@
         <v>253</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>156</v>
@@ -11002,7 +10999,7 @@
         <v>30</v>
       </c>
       <c r="K80" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L80" s="10" t="s">
         <v>16</v>
@@ -11031,7 +11028,7 @@
         <v>161</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F81" s="10" t="s">
         <v>156</v>
@@ -11049,7 +11046,7 @@
         <v>1</v>
       </c>
       <c r="K81" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>399</v>
@@ -11067,13 +11064,13 @@
         <v>1</v>
       </c>
       <c r="V81" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W81" s="11">
         <v>1</v>
       </c>
       <c r="X81" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
@@ -11087,7 +11084,7 @@
         <v>161</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>156</v>
@@ -11105,7 +11102,7 @@
         <v>1</v>
       </c>
       <c r="K82" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L82" s="10" t="s">
         <v>399</v>
@@ -11120,13 +11117,13 @@
         <v>1</v>
       </c>
       <c r="V82" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W82" s="11">
         <v>0</v>
       </c>
       <c r="X82" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
@@ -11140,7 +11137,7 @@
         <v>161</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F83" s="10" t="s">
         <v>156</v>
@@ -11158,7 +11155,7 @@
         <v>1</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L83" s="10" t="s">
         <v>399</v>
@@ -11182,7 +11179,7 @@
         <v>1</v>
       </c>
       <c r="X83" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
@@ -11196,7 +11193,7 @@
         <v>161</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F84" s="10" t="s">
         <v>156</v>
@@ -11214,7 +11211,7 @@
         <v>1</v>
       </c>
       <c r="K84" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L84" s="10" t="s">
         <v>399</v>
@@ -11232,7 +11229,7 @@
         <v>0</v>
       </c>
       <c r="X84" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -11246,7 +11243,7 @@
         <v>161</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>156</v>
@@ -11264,7 +11261,7 @@
         <v>1</v>
       </c>
       <c r="K85" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L85" s="10" t="s">
         <v>399</v>
@@ -11282,7 +11279,7 @@
         <v>0</v>
       </c>
       <c r="X85" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
@@ -11296,7 +11293,7 @@
         <v>161</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>156</v>
@@ -11314,7 +11311,7 @@
         <v>1</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L86" s="10" t="s">
         <v>399</v>
@@ -11332,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="X86" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
@@ -11346,13 +11343,13 @@
         <v>161</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>89</v>
@@ -11364,7 +11361,7 @@
         <v>1</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L87" s="10" t="s">
         <v>399</v>
@@ -11385,7 +11382,7 @@
         <v>1</v>
       </c>
       <c r="X87" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
@@ -11399,7 +11396,7 @@
         <v>161</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>156</v>
@@ -11417,7 +11414,7 @@
         <v>1</v>
       </c>
       <c r="K88" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L88" s="10" t="s">
         <v>399</v>
@@ -11435,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="X88" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
@@ -11449,7 +11446,7 @@
         <v>161</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F89" s="10" t="s">
         <v>156</v>
@@ -11467,7 +11464,7 @@
         <v>1</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L89" s="10" t="s">
         <v>399</v>
@@ -11488,7 +11485,7 @@
         <v>0</v>
       </c>
       <c r="X89" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
@@ -11502,7 +11499,7 @@
         <v>161</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>156</v>
@@ -11520,7 +11517,7 @@
         <v>1</v>
       </c>
       <c r="K90" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L90" s="10" t="s">
         <v>399</v>
@@ -11538,7 +11535,7 @@
         <v>0</v>
       </c>
       <c r="X90" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
@@ -11552,7 +11549,7 @@
         <v>161</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>156</v>
@@ -11570,7 +11567,7 @@
         <v>1</v>
       </c>
       <c r="K91" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L91" s="10" t="s">
         <v>399</v>
@@ -11588,7 +11585,7 @@
         <v>0</v>
       </c>
       <c r="X91" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
@@ -11602,7 +11599,7 @@
         <v>161</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F92" s="10" t="s">
         <v>156</v>
@@ -11620,7 +11617,7 @@
         <v>1</v>
       </c>
       <c r="K92" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L92" s="10" t="s">
         <v>399</v>
@@ -11638,7 +11635,7 @@
         <v>0</v>
       </c>
       <c r="X92" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
@@ -11652,7 +11649,7 @@
         <v>314</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>156</v>
@@ -11670,7 +11667,7 @@
         <v>1</v>
       </c>
       <c r="K93" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L93" s="10" t="s">
         <v>399</v>
@@ -11695,7 +11692,7 @@
         <v>314</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>156</v>
@@ -11713,7 +11710,7 @@
         <v>1</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L94" s="10" t="s">
         <v>399</v>
@@ -11738,7 +11735,7 @@
         <v>161</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F95" s="10" t="s">
         <v>156</v>
@@ -11756,7 +11753,7 @@
         <v>1</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L95" s="10" t="s">
         <v>399</v>
@@ -11781,7 +11778,7 @@
         <v>314</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F96" s="10" t="s">
         <v>156</v>
@@ -11796,7 +11793,7 @@
         <v>30</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L96" s="10" t="s">
         <v>15</v>
@@ -11821,7 +11818,7 @@
         <v>163</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F97" s="10" t="s">
         <v>156</v>
@@ -11836,7 +11833,7 @@
         <v>30</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>101</v>
@@ -11864,7 +11861,7 @@
         <v>163</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>171</v>
@@ -11876,7 +11873,7 @@
         <v>30</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>16</v>
@@ -11891,7 +11888,7 @@
         <v>1</v>
       </c>
       <c r="V98" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W98" s="11"/>
       <c r="X98" s="12"/>
@@ -11907,7 +11904,7 @@
         <v>238</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F99" s="10" t="s">
         <v>250</v>
@@ -11925,7 +11922,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L99" s="10" t="s">
         <v>15</v>
@@ -11937,7 +11934,7 @@
         <v>16</v>
       </c>
       <c r="V99" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W99" s="11">
         <v>1</v>
@@ -11957,7 +11954,7 @@
         <v>238</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F100" s="10" t="s">
         <v>250</v>
@@ -11975,7 +11972,7 @@
         <v>1</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>16</v>
@@ -12004,7 +12001,7 @@
         <v>161</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F101" s="10" t="s">
         <v>171</v>
@@ -12016,7 +12013,7 @@
         <v>30</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>399</v>
@@ -12028,7 +12025,7 @@
         <v>283</v>
       </c>
       <c r="V101" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W101" s="11"/>
       <c r="X101" s="12"/>
@@ -12044,7 +12041,7 @@
         <v>161</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F102" s="10" t="s">
         <v>171</v>
@@ -12056,7 +12053,7 @@
         <v>30</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L102" s="10" t="s">
         <v>399</v>
@@ -12068,7 +12065,7 @@
         <v>283</v>
       </c>
       <c r="V102" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W102" s="11"/>
       <c r="X102" s="12"/>
@@ -12084,7 +12081,7 @@
         <v>161</v>
       </c>
       <c r="D103" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>171</v>
@@ -12096,7 +12093,7 @@
         <v>30</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L103" s="10" t="s">
         <v>399</v>
@@ -12108,23 +12105,23 @@
         <v>283</v>
       </c>
       <c r="V103" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W103" s="11"/>
       <c r="X103" s="12"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>171</v>
@@ -12136,7 +12133,7 @@
         <v>30</v>
       </c>
       <c r="K104" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L104" s="10" t="s">
         <v>399</v>
@@ -12152,16 +12149,16 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F105" s="10" t="s">
         <v>171</v>
@@ -12173,7 +12170,7 @@
         <v>30</v>
       </c>
       <c r="K105" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L105" s="10" t="s">
         <v>399</v>
@@ -12189,16 +12186,16 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>314</v>
       </c>
       <c r="D106" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F106" s="10" t="s">
         <v>171</v>
@@ -12210,7 +12207,7 @@
         <v>30</v>
       </c>
       <c r="K106" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L106" s="10" t="s">
         <v>399</v>
@@ -12226,16 +12223,16 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>314</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>171</v>
@@ -12247,7 +12244,7 @@
         <v>30</v>
       </c>
       <c r="K107" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="L107" s="10" t="s">
         <v>399</v>
@@ -12290,7 +12287,7 @@
         <v>30</v>
       </c>
       <c r="K108" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L108" s="10" t="s">
         <v>15</v>
@@ -12308,12 +12305,12 @@
         <v>0</v>
       </c>
       <c r="X108" s="11" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>222</v>
@@ -12340,7 +12337,7 @@
         <v>30</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>15</v>
@@ -12352,13 +12349,13 @@
         <v>283</v>
       </c>
       <c r="V109" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W109" s="11">
         <v>1</v>
       </c>
       <c r="X109" s="11" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
@@ -12372,7 +12369,7 @@
         <v>253</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F110" s="10" t="s">
         <v>156</v>
@@ -12387,7 +12384,7 @@
         <v>30</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>15</v>
@@ -12405,54 +12402,54 @@
         <v>1</v>
       </c>
       <c r="V110" s="10" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="W110" s="11">
         <v>1</v>
       </c>
       <c r="X110" s="11" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I1:J110">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W111:W10020">
-    <cfRule type="expression" dxfId="33" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G110">
-    <cfRule type="expression" dxfId="32" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V110">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J110">
-    <cfRule type="expression" dxfId="28" priority="15">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>OR($I2="q", $I2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12469,7 +12466,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W110">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($I2&lt;&gt;"d", $I2 &lt;&gt; "w", $I2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12486,7 +12483,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12508,7 +12505,7 @@
         <v>56</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>464</v>
+        <v>433</v>
       </c>
       <c r="E1" t="s">
         <v>355</v>
@@ -12681,7 +12678,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -12698,7 +12695,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -12715,7 +12712,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>465</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -12728,652 +12725,793 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E828C45D-CF7B-424F-B36C-220BE51A990F}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="13"/>
     <col min="2" max="3" width="10.7109375" style="14"/>
-    <col min="4" max="13" width="10.7109375" style="15"/>
-    <col min="14" max="16384" width="10.7109375" style="13"/>
+    <col min="4" max="15" width="10.7109375" style="15"/>
+    <col min="16" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="14" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>470</v>
+        <v>439</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>471</v>
+        <v>440</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>471</v>
+        <v>440</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>472</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>400</v>
+        <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H2" s="16"/>
       <c r="I2" s="17"/>
-      <c r="K2" s="15" t="s">
-        <v>473</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>401</v>
+        <v>443</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>402</v>
+        <v>444</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>403</v>
+        <v>445</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>404</v>
+        <v>446</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>405</v>
+        <v>447</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>406</v>
+        <v>448</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>407</v>
+        <v>449</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>408</v>
+        <v>450</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>409</v>
+        <v>451</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>410</v>
+        <v>452</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>411</v>
+        <v>453</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>412</v>
+        <v>454</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>413</v>
+        <v>455</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>414</v>
+        <v>456</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>467</v>
+        <v>436</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>466</v>
+        <v>435</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>469</v>
+        <v>438</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>456</v>
+        <v>465</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>457</v>
+        <v>466</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>458</v>
+        <v>467</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>459</v>
+        <v>468</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>460</v>
+        <v>469</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>461</v>
+        <v>470</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>462</v>
+        <v>471</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>463</v>
+        <v>472</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>438</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>435</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -13387,7 +13525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624AEEDB-BBA7-44A6-A6FF-0B28C3344004}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Split baseline initial forecasts from other scenario initial forecasts (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A89E46-CC09-4603-8E37-254E8160CB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CD30D-534C-4AC0-A7E0-6745FD58B720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3431" uniqueCount="493">
   <si>
     <t>gdp</t>
   </si>
@@ -1361,9 +1361,6 @@
     <t>inf.d1_strong</t>
   </si>
   <si>
-    <t>tdns.d1.baseline</t>
-  </si>
-  <si>
     <t>2021-06</t>
   </si>
   <si>
@@ -1455,6 +1452,72 @@
   </si>
   <si>
     <t>2023-12</t>
+  </si>
+  <si>
+    <t>spy.d1_strong</t>
+  </si>
+  <si>
+    <t>spy.d1_baseline</t>
+  </si>
+  <si>
+    <t>spy.d1_weak</t>
+  </si>
+  <si>
+    <t>tdns1.d1_baseline</t>
+  </si>
+  <si>
+    <t>tdns1.d1_strong</t>
+  </si>
+  <si>
+    <t>tdns1.d1_weak</t>
+  </si>
+  <si>
+    <t>tdns2.d1_baseline</t>
+  </si>
+  <si>
+    <t>tdns2.d1_strong</t>
+  </si>
+  <si>
+    <t>tdns2.d1_weak</t>
+  </si>
+  <si>
+    <t>tdns3.d1_baseline</t>
+  </si>
+  <si>
+    <t>tdns3.d1_strong</t>
+  </si>
+  <si>
+    <t>tdns3.d1_weak</t>
+  </si>
+  <si>
+    <t>ue.d1_baseline</t>
+  </si>
+  <si>
+    <t>ue.d1_strong</t>
+  </si>
+  <si>
+    <t>ue.d1_weak</t>
+  </si>
+  <si>
+    <t>[cle]</t>
+  </si>
+  <si>
+    <t>[dns]</t>
+  </si>
+  <si>
+    <t>[.003]</t>
+  </si>
+  <si>
+    <t>dpi.st_baseline</t>
+  </si>
+  <si>
+    <t>dpi.st_strong</t>
+  </si>
+  <si>
+    <t>dpi.st_weak</t>
+  </si>
+  <si>
+    <t>[cbo]</t>
   </si>
 </sst>
 </file>
@@ -1576,7 +1639,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="68">
     <dxf>
       <fill>
         <patternFill>
@@ -1670,6 +1733,76 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2412,23 +2545,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="54"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="65"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="63"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="58"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2441,7 +2574,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="51"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2449,33 +2582,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X108" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X108" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:X108" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="38"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="35"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="25"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="24"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="23"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="22"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="21"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="20"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="19"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="18"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="45"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="35"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="34"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="33"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="30"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="28"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2488,7 +2621,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="24"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2794,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41:M57"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6104,10 +6237,10 @@
         <v>15</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>16</v>
+        <v>391</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>283</v>
+        <v>16</v>
       </c>
       <c r="M75" s="3" t="b">
         <v>1</v>
@@ -7374,8 +7507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:X108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="X91" sqref="X91:X92"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12340,7 +12473,7 @@
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W109:W10018">
+  <conditionalFormatting sqref="W109:W10017">
     <cfRule type="expression" dxfId="6" priority="6">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
@@ -12396,7 +12529,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12613,7 +12746,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -12638,10 +12771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E828C45D-CF7B-424F-B36C-220BE51A990F}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G33" sqref="G33:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12649,10 +12782,12 @@
     <col min="1" max="1" width="10.7109375" style="13"/>
     <col min="2" max="3" width="10.7109375" style="14"/>
     <col min="4" max="15" width="10.7109375" style="15"/>
-    <col min="16" max="16384" width="10.7109375" style="13"/>
+    <col min="16" max="25" width="10.7109375" style="13"/>
+    <col min="26" max="26" width="10.7109375" style="15"/>
+    <col min="27" max="16384" width="10.7109375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B1" s="14" t="s">
         <v>426</v>
       </c>
@@ -12681,12 +12816,63 @@
         <v>439</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>473</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>440</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>441</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>435</v>
@@ -12706,12 +12892,67 @@
       <c r="G2" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K2" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L2" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M2" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>435</v>
@@ -12731,12 +12972,67 @@
       <c r="G3" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H3" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K3" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L3" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M3" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>435</v>
@@ -12756,12 +13052,67 @@
       <c r="G4" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K4" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L4" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M4" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X4" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>435</v>
@@ -12781,12 +13132,67 @@
       <c r="G5" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K5" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L5" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M5" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X5" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z5" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>435</v>
@@ -12806,12 +13212,67 @@
       <c r="G6" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K6" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L6" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M6" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W6" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>435</v>
@@ -12831,12 +13292,67 @@
       <c r="G7" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K7" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L7" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M7" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V7" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>435</v>
@@ -12856,12 +13372,67 @@
       <c r="G8" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H8" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K8" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L8" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M8" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V8" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W8" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y8" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z8" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>435</v>
@@ -12881,12 +13452,67 @@
       <c r="G9" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H9" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K9" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L9" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M9" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V9" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W9" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X9" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y9" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z9" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>435</v>
@@ -12906,12 +13532,67 @@
       <c r="G10" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H10" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K10" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M10" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y10" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z10" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>435</v>
@@ -12931,12 +13612,67 @@
       <c r="G11" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K11" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L11" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M11" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V11" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W11" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X11" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z11" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>435</v>
@@ -12956,12 +13692,67 @@
       <c r="G12" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H12" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K12" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L12" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M12" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z12" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>435</v>
@@ -12981,12 +13772,67 @@
       <c r="G13" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K13" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L13" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M13" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W13" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X13" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y13" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>435</v>
@@ -13006,12 +13852,67 @@
       <c r="G14" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H14" s="16"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K14" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L14" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M14" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V14" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W14" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X14" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>435</v>
@@ -13031,12 +13932,67 @@
       <c r="G15" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K15" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L15" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M15" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W15" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X15" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y15" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z15" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>435</v>
@@ -13056,12 +14012,67 @@
       <c r="G16" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K16" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L16" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M16" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V16" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W16" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X16" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y16" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z16" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>435</v>
@@ -13081,10 +14092,67 @@
       <c r="G17" s="17" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V17" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W17" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X17" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y17" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z17" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>435</v>
@@ -13104,10 +14172,67 @@
       <c r="G18" s="17" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K18" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L18" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M18" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V18" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W18" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X18" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y18" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>435</v>
@@ -13127,10 +14252,67 @@
       <c r="G19" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K19" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L19" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M19" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V19" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W19" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X19" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y19" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z19" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>435</v>
@@ -13150,10 +14332,67 @@
       <c r="G20" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K20" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L20" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M20" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V20" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W20" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X20" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y20" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z20" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>435</v>
@@ -13173,10 +14412,67 @@
       <c r="G21" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K21" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L21" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M21" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V21" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W21" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X21" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y21" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z21" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>435</v>
@@ -13196,10 +14492,67 @@
       <c r="G22" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K22" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L22" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M22" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W22" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X22" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>435</v>
@@ -13219,10 +14572,67 @@
       <c r="G23" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K23" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L23" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M23" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V23" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W23" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X23" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y23" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z23" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>435</v>
@@ -13242,10 +14652,67 @@
       <c r="G24" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K24" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L24" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M24" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V24" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W24" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X24" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y24" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z24" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>435</v>
@@ -13265,10 +14732,67 @@
       <c r="G25" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K25" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L25" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M25" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V25" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W25" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X25" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y25" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z25" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>435</v>
@@ -13288,10 +14812,67 @@
       <c r="G26" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K26" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L26" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M26" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V26" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W26" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X26" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y26" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z26" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>435</v>
@@ -13311,10 +14892,67 @@
       <c r="G27" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K27" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L27" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M27" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V27" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W27" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X27" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y27" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z27" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>435</v>
@@ -13334,10 +14972,67 @@
       <c r="G28" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K28" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L28" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M28" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V28" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W28" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X28" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y28" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z28" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>435</v>
@@ -13357,10 +15052,67 @@
       <c r="G29" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K29" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L29" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M29" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V29" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W29" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X29" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y29" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z29" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B30" s="16" t="s">
         <v>435</v>
@@ -13380,10 +15132,67 @@
       <c r="G30" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K30" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L30" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M30" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V30" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W30" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X30" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y30" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z30" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>435</v>
@@ -13403,10 +15212,67 @@
       <c r="G31" s="17" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K31" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L31" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M31" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V31" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W31" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X31" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y31" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z31" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B32" s="16" t="s">
         <v>435</v>
@@ -13425,6 +15291,63 @@
       </c>
       <c r="G32" s="17" t="s">
         <v>437</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>486</v>
+      </c>
+      <c r="K32" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L32" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M32" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="P32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="S32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="T32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="U32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V32" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="W32" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="X32" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y32" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z32" s="15" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update docs location to website via SFTP instead of Github Pages (v0.14)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1CD30D-534C-4AC0-A7E0-6745FD58B720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D04C43-403B-4298-9D14-F32CC49BE61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -1639,173 +1639,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2260,6 +2094,83 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2525,6 +2436,25 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2545,23 +2475,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="45"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="43"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2574,7 +2504,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="38"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2582,33 +2512,33 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X108" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:X108" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:X108" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="46"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="45"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="35"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="34"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="33"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="31"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="30"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="29"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="28"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="21"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2621,7 +2551,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7219,17 +7149,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="57" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="56" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7508,7 +7438,7 @@
   <dimension ref="A1:X108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+      <selection activeCell="V106" sqref="V106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12460,42 +12390,42 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I1:J108">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W109:W10017">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="33" priority="6">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G108">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="32" priority="5">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V108">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J108">
-    <cfRule type="expression" dxfId="1" priority="15">
+    <cfRule type="expression" dxfId="28" priority="15">
       <formula>OR($I2="q", $I2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12512,7 +12442,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W108">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>AND($I2&lt;&gt;"d", $I2 &lt;&gt; "w", $I2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added refactoring of FRED releases pulling (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB34BBE-A07A-4CE4-8143-52882F57E6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B15243-0AE6-4317-B68D-AB60F696B00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="646">
   <si>
     <t>gdp</t>
   </si>
@@ -1675,9 +1675,6 @@
   </si>
   <si>
     <t>post.exog</t>
-  </si>
-  <si>
-    <t>release</t>
   </si>
   <si>
     <t>BEA.GDP</t>
@@ -2114,7 +2111,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="77">
     <dxf>
       <fill>
         <patternFill>
@@ -2233,23 +2230,102 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2560,6 +2636,25 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -3010,23 +3105,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="72"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="65"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3039,7 +3134,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="60"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3047,35 +3142,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z106" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z106" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:Z106" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="40"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="release" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="30"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="29"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="28"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="27"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="26"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="25"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="24"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="23"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="22"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="55"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="54"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="41"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="39"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="37"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="36"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3103,7 +3198,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="31"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7989,8 +8084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H107" sqref="H107"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8038,7 +8133,7 @@
         <v>164</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>88</v>
@@ -8118,7 +8213,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>284</v>
@@ -8187,7 +8282,7 @@
         <v>106</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>284</v>
@@ -8244,7 +8339,7 @@
         <v>107</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>284</v>
@@ -8295,7 +8390,7 @@
         <v>108</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>284</v>
@@ -8346,7 +8441,7 @@
         <v>172</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>284</v>
@@ -8397,7 +8492,7 @@
         <v>173</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>284</v>
@@ -8448,7 +8543,7 @@
         <v>174</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>284</v>
@@ -8499,7 +8594,7 @@
         <v>175</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>284</v>
@@ -8550,7 +8645,7 @@
         <v>109</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>284</v>
@@ -8601,7 +8696,7 @@
         <v>110</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>284</v>
@@ -8652,7 +8747,7 @@
         <v>180</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>284</v>
@@ -8703,7 +8798,7 @@
         <v>181</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>284</v>
@@ -8754,7 +8849,7 @@
         <v>182</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>284</v>
@@ -8805,7 +8900,7 @@
         <v>111</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>284</v>
@@ -8856,7 +8951,7 @@
         <v>112</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>284</v>
@@ -8907,7 +9002,7 @@
         <v>113</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>284</v>
@@ -8958,7 +9053,7 @@
         <v>114</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>284</v>
@@ -9009,7 +9104,7 @@
         <v>115</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>284</v>
@@ -9060,7 +9155,7 @@
         <v>116</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>284</v>
@@ -9111,7 +9206,7 @@
         <v>117</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>284</v>
@@ -9162,7 +9257,7 @@
         <v>118</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>284</v>
@@ -9213,7 +9308,7 @@
         <v>119</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>284</v>
@@ -9264,7 +9359,7 @@
         <v>102</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>284</v>
@@ -9315,7 +9410,7 @@
         <v>120</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>284</v>
@@ -9366,7 +9461,7 @@
         <v>206</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>284</v>
@@ -9417,7 +9512,7 @@
         <v>207</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>284</v>
@@ -9468,7 +9563,7 @@
         <v>208</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>284</v>
@@ -9519,7 +9614,7 @@
         <v>121</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>284</v>
@@ -9570,7 +9665,7 @@
         <v>122</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>284</v>
@@ -9621,7 +9716,7 @@
         <v>123</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>284</v>
@@ -9672,7 +9767,7 @@
         <v>170</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>284</v>
@@ -9723,7 +9818,7 @@
         <v>213</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>284</v>
@@ -9774,7 +9869,7 @@
         <v>214</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>284</v>
@@ -9825,7 +9920,7 @@
         <v>169</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>284</v>
@@ -9876,7 +9971,7 @@
         <v>215</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>284</v>
@@ -9927,7 +10022,7 @@
         <v>216</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>284</v>
@@ -9978,7 +10073,7 @@
         <v>124</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>284</v>
@@ -10029,7 +10124,7 @@
         <v>125</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>284</v>
@@ -10080,7 +10175,7 @@
         <v>126</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>284</v>
@@ -10128,7 +10223,7 @@
         <v>100</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>284</v>
@@ -10178,7 +10273,7 @@
         <v>195</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>284</v>
@@ -10228,7 +10323,7 @@
         <v>192</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>284</v>
@@ -10278,7 +10373,7 @@
         <v>193</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I44" s="10" t="s">
         <v>284</v>
@@ -10328,7 +10423,7 @@
         <v>194</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I45" s="10" t="s">
         <v>284</v>
@@ -10381,7 +10476,7 @@
         <v>220</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>284</v>
@@ -10434,7 +10529,7 @@
         <v>230</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I47" s="10" t="s">
         <v>284</v>
@@ -10487,7 +10582,7 @@
         <v>229</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I48" s="10" t="s">
         <v>284</v>
@@ -10537,7 +10632,7 @@
         <v>32</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I49" s="10" t="s">
         <v>94</v>
@@ -10590,7 +10685,7 @@
         <v>300</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I50" s="10" t="s">
         <v>301</v>
@@ -10640,7 +10735,7 @@
         <v>315</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I51" s="10" t="s">
         <v>316</v>
@@ -10690,7 +10785,7 @@
         <v>325</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I52" s="10" t="s">
         <v>316</v>
@@ -10740,7 +10835,7 @@
         <v>318</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I53" s="10" t="s">
         <v>311</v>
@@ -10790,7 +10885,7 @@
         <v>321</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I54" s="10" t="s">
         <v>322</v>
@@ -10840,7 +10935,7 @@
         <v>310</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I55" s="10" t="s">
         <v>311</v>
@@ -10890,7 +10985,7 @@
         <v>33</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I56" s="10" t="s">
         <v>196</v>
@@ -10940,7 +11035,7 @@
         <v>305</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I57" s="10" t="s">
         <v>306</v>
@@ -10990,7 +11085,7 @@
         <v>329</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I58" s="10" t="s">
         <v>316</v>
@@ -11040,7 +11135,7 @@
         <v>38</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I59" s="10" t="s">
         <v>94</v>
@@ -11090,7 +11185,7 @@
         <v>332</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I60" s="10" t="s">
         <v>333</v>
@@ -11140,7 +11235,7 @@
         <v>42</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I61" s="10" t="s">
         <v>285</v>
@@ -11190,7 +11285,7 @@
         <v>44</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I62" s="10" t="s">
         <v>285</v>
@@ -11240,7 +11335,7 @@
         <v>48</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I63" s="10" t="s">
         <v>94</v>
@@ -11290,7 +11385,7 @@
         <v>50</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I64" s="10" t="s">
         <v>94</v>
@@ -11340,7 +11435,7 @@
         <v>52</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I65" s="10" t="s">
         <v>165</v>
@@ -11390,7 +11485,7 @@
         <v>91</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I66" s="10" t="s">
         <v>95</v>
@@ -11440,7 +11535,7 @@
         <v>55</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I67" s="10" t="s">
         <v>94</v>
@@ -11490,7 +11585,7 @@
         <v>82</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I68" s="10" t="s">
         <v>166</v>
@@ -11540,7 +11635,7 @@
         <v>84</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I69" s="10" t="s">
         <v>94</v>
@@ -11590,7 +11685,7 @@
         <v>97</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>99</v>
@@ -11640,7 +11735,7 @@
         <v>239</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I71" s="10" t="s">
         <v>89</v>
@@ -11688,7 +11783,7 @@
         <v>240</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I72" s="10" t="s">
         <v>89</v>
@@ -11736,7 +11831,7 @@
         <v>241</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>89</v>
@@ -11784,7 +11879,7 @@
         <v>244</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I74" s="10" t="s">
         <v>94</v>
@@ -11834,7 +11929,7 @@
         <v>245</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I75" s="10" t="s">
         <v>94</v>
@@ -11884,7 +11979,7 @@
         <v>296</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>94</v>
@@ -11934,7 +12029,7 @@
         <v>254</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I77" s="10" t="s">
         <v>94</v>
@@ -11984,7 +12079,7 @@
         <v>336</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I78" s="10" t="s">
         <v>89</v>
@@ -12034,7 +12129,7 @@
         <v>339</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>89</v>
@@ -12084,7 +12179,7 @@
         <v>28</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>89</v>
@@ -12146,7 +12241,7 @@
         <v>29</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I81" s="10" t="s">
         <v>89</v>
@@ -12205,7 +12300,7 @@
         <v>19</v>
       </c>
       <c r="H82" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>89</v>
@@ -12267,7 +12362,7 @@
         <v>21</v>
       </c>
       <c r="H83" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I83" s="10" t="s">
         <v>89</v>
@@ -12323,7 +12418,7 @@
         <v>22</v>
       </c>
       <c r="H84" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I84" s="10" t="s">
         <v>89</v>
@@ -12379,7 +12474,7 @@
         <v>23</v>
       </c>
       <c r="H85" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I85" s="10" t="s">
         <v>89</v>
@@ -12435,7 +12530,7 @@
         <v>402</v>
       </c>
       <c r="H86" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I86" s="10" t="s">
         <v>89</v>
@@ -12494,7 +12589,7 @@
         <v>24</v>
       </c>
       <c r="H87" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I87" s="10" t="s">
         <v>89</v>
@@ -12550,7 +12645,7 @@
         <v>25</v>
       </c>
       <c r="H88" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I88" s="10" t="s">
         <v>89</v>
@@ -12609,7 +12704,7 @@
         <v>26</v>
       </c>
       <c r="H89" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I89" s="10" t="s">
         <v>89</v>
@@ -12665,7 +12760,7 @@
         <v>20</v>
       </c>
       <c r="H90" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I90" s="10" t="s">
         <v>89</v>
@@ -12721,7 +12816,7 @@
         <v>27</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>89</v>
@@ -12777,7 +12872,7 @@
         <v>349</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I92" s="10" t="s">
         <v>89</v>
@@ -12830,7 +12925,7 @@
         <v>350</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I93" s="10" t="s">
         <v>89</v>
@@ -12883,7 +12978,7 @@
         <v>351</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I94" s="10" t="s">
         <v>89</v>
@@ -12936,7 +13031,7 @@
         <v>352</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I95" s="10" t="s">
         <v>94</v>
@@ -12985,6 +13080,9 @@
       <c r="F96" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H96" s="10" t="s">
+        <v>627</v>
+      </c>
       <c r="I96" s="10" t="s">
         <v>89</v>
       </c>
@@ -13039,7 +13137,7 @@
         <v>290</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I97" s="10" t="s">
         <v>94</v>
@@ -13095,7 +13193,7 @@
         <v>291</v>
       </c>
       <c r="H98" s="10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I98" s="10" t="s">
         <v>94</v>
@@ -13144,6 +13242,9 @@
       <c r="F99" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H99" s="10" t="s">
+        <v>616</v>
+      </c>
       <c r="I99" s="10" t="s">
         <v>89</v>
       </c>
@@ -13191,6 +13292,9 @@
       <c r="F100" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H100" s="10" t="s">
+        <v>616</v>
+      </c>
       <c r="I100" s="10" t="s">
         <v>89</v>
       </c>
@@ -13238,6 +13342,9 @@
       <c r="F101" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H101" s="10" t="s">
+        <v>616</v>
+      </c>
       <c r="I101" s="10" t="s">
         <v>89</v>
       </c>
@@ -13285,6 +13392,9 @@
       <c r="F102" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H102" s="10" t="s">
+        <v>642</v>
+      </c>
       <c r="I102" s="10" t="s">
         <v>89</v>
       </c>
@@ -13329,6 +13439,9 @@
       <c r="F103" s="10" t="s">
         <v>171</v>
       </c>
+      <c r="H103" s="10" t="s">
+        <v>642</v>
+      </c>
       <c r="I103" s="10" t="s">
         <v>89</v>
       </c>
@@ -13380,7 +13493,7 @@
         <v>221</v>
       </c>
       <c r="H104" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I104" s="10" t="s">
         <v>284</v>
@@ -13436,7 +13549,7 @@
         <v>87</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I105" s="10" t="s">
         <v>284</v>
@@ -13489,7 +13602,7 @@
         <v>36</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I106" s="10" t="s">
         <v>89</v>
@@ -13549,7 +13662,7 @@
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H106">
+  <conditionalFormatting sqref="G2:G106">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>$F2="calc"</formula>
     </cfRule>
@@ -13610,8 +13723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624AEEDB-BBA7-44A6-A6FF-0B28C3344004}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13625,33 +13738,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" t="s">
         <v>548</v>
       </c>
-      <c r="B1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>549</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>550</v>
       </c>
-      <c r="E1" t="s">
-        <v>551</v>
-      </c>
       <c r="F1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C2" t="s">
         <v>552</v>
-      </c>
-      <c r="C2" t="s">
-        <v>553</v>
       </c>
       <c r="D2" t="s">
         <v>156</v>
@@ -13662,13 +13775,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D3" t="s">
         <v>156</v>
@@ -13679,13 +13792,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D4" t="s">
         <v>156</v>
@@ -13696,13 +13809,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D5" t="s">
         <v>156</v>
@@ -13713,13 +13826,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C6" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D6" t="s">
         <v>156</v>
@@ -13730,13 +13843,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B7" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D7" t="s">
         <v>156</v>
@@ -13747,13 +13860,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D8" t="s">
         <v>156</v>
@@ -13764,13 +13877,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D9" t="s">
         <v>156</v>
@@ -13781,13 +13894,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B10" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C10" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D10" t="s">
         <v>156</v>
@@ -13798,13 +13911,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B11" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D11" t="s">
         <v>156</v>
@@ -13815,13 +13928,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B12" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C12" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D12" t="s">
         <v>156</v>
@@ -13832,13 +13945,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B13" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D13" t="s">
         <v>156</v>
@@ -13847,18 +13960,18 @@
         <v>465</v>
       </c>
       <c r="F13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D14" t="s">
         <v>156</v>
@@ -13869,13 +13982,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B15" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D15" t="s">
         <v>156</v>
@@ -13886,7 +13999,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
@@ -13898,18 +14011,18 @@
         <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D17" t="s">
         <v>156</v>
@@ -13920,13 +14033,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B18" t="s">
+        <v>636</v>
+      </c>
+      <c r="C18" t="s">
         <v>637</v>
-      </c>
-      <c r="C18" t="s">
-        <v>638</v>
       </c>
       <c r="D18" t="s">
         <v>156</v>
@@ -13937,13 +14050,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C19" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D19" t="s">
         <v>156</v>
@@ -13952,18 +14065,18 @@
         <v>341</v>
       </c>
       <c r="F19" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D20" t="s">
         <v>156</v>
@@ -13974,13 +14087,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C21" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D21" t="s">
         <v>156</v>
@@ -13991,13 +14104,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B22" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -14006,18 +14119,18 @@
         <v>321</v>
       </c>
       <c r="F22" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B23" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D23" t="s">
         <v>156</v>
@@ -14026,18 +14139,18 @@
         <v>374</v>
       </c>
       <c r="F23" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B24" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C24" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D24" t="s">
         <v>156</v>
@@ -14046,18 +14159,18 @@
         <v>351</v>
       </c>
       <c r="F24" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B25" t="s">
         <v>252</v>
       </c>
       <c r="C25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
@@ -14068,10 +14181,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B26" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D26" t="s">
         <v>156</v>
@@ -14082,13 +14195,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B27" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C27" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -14099,13 +14212,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D28" t="s">
         <v>156</v>
@@ -14116,13 +14229,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B29" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D29" t="s">
         <v>156</v>
@@ -14133,13 +14246,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D30" t="s">
         <v>156</v>
@@ -14150,13 +14263,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D31" t="s">
         <v>156</v>
@@ -14167,13 +14280,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>643</v>
+      </c>
+      <c r="B32" t="s">
         <v>644</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>645</v>
-      </c>
-      <c r="C32" t="s">
-        <v>646</v>
       </c>
       <c r="D32" t="s">
         <v>250</v>

</xml_diff>

<commit_message>
Working nowcast version (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17C92C3-5D4D-4C76-8C11-4E51B38EB444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E41B16-F5F0-46E6-BFAA-8642695FD62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -7983,8 +7983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="Y105" sqref="Y105"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13045,7 +13045,7 @@
         <v>341</v>
       </c>
       <c r="K97" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>410</v>
@@ -13101,7 +13101,7 @@
         <v>341</v>
       </c>
       <c r="K98" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Fixed bug with NA-only obs related to new WSJ data release (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E41B16-F5F0-46E6-BFAA-8642695FD62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A3F332-3478-4253-9988-990F14CA95E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -7984,7 +7984,7 @@
   <dimension ref="A1:Z106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13045,7 +13045,7 @@
         <v>341</v>
       </c>
       <c r="K97" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>410</v>
@@ -13101,7 +13101,7 @@
         <v>341</v>
       </c>
       <c r="K98" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>410</v>

</xml_diff>

<commit_message>
Refactored some nowcast code and added d2 transformation (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3940A633-61D8-422B-9731-4662181FE5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8284812F-6B10-49C4-B455-FCA1AD6670A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2105,7 +2105,224 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="80">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2599,104 +2816,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3001,23 +3120,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="52"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="50"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="48"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="72"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="65"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3030,7 +3149,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="60"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3038,35 +3157,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z106" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z106" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A1:Z106" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="55"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="54"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="51"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="43"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="41"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="39"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="37"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="36"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3094,7 +3213,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="31"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7692,17 +7811,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="62" priority="3">
+    <cfRule type="expression" dxfId="79" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="61" priority="2">
+    <cfRule type="expression" dxfId="78" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7980,8 +8099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="X93" sqref="X93"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="X101" sqref="X101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13540,47 +13659,47 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K106">
-    <cfRule type="cellIs" dxfId="42" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X107:X10015">
-    <cfRule type="expression" dxfId="38" priority="9">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G106">
-    <cfRule type="expression" dxfId="37" priority="8">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W106">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K106">
-    <cfRule type="expression" dxfId="33" priority="18">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X107:X1048576">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -13592,19 +13711,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X106">
-    <cfRule type="expression" dxfId="32" priority="4">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z106">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"core.exog"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y2:Y106">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"calc"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"dfm.m"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"dfm.q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added mroe financial indices to import (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335EB0E0-A71B-4AD6-B3E2-04D0F790DFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FFE9F3-A53B-4D1A-BD53-84FBACC361B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3633" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="654">
   <si>
     <t>gdp</t>
   </si>
@@ -1988,6 +1988,33 @@
   </si>
   <si>
     <t>New York Fed: Future Capex Manufacturing Survey</t>
+  </si>
+  <si>
+    <t>moo</t>
+  </si>
+  <si>
+    <t>DBA</t>
+  </si>
+  <si>
+    <t>metals</t>
+  </si>
+  <si>
+    <t>DBB</t>
+  </si>
+  <si>
+    <t>spdw</t>
+  </si>
+  <si>
+    <t>SPDW</t>
+  </si>
+  <si>
+    <t>Ex-US Equities (SPDW)</t>
+  </si>
+  <si>
+    <t>Metal Commodities (DBB)</t>
+  </si>
+  <si>
+    <t>Agricultural Commodities (DBA)</t>
   </si>
 </sst>
 </file>
@@ -2109,6 +2136,144 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="66">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2602,125 +2767,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2986,25 +3032,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3025,23 +3052,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3054,7 +3081,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="49"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3062,35 +3089,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z106" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:Z106" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:Z109" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="44"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="43"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="32"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="31"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="30"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="28"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="27"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="26"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="25"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3118,7 +3145,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="20"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3424,8 +3451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7716,17 +7743,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="64" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8002,10 +8029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
-  <dimension ref="A1:Z106"/>
+  <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10567,7 +10594,7 @@
         <v>15</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="O49" s="10" t="s">
         <v>282</v>
@@ -13148,163 +13175,172 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>391</v>
+        <v>645</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>394</v>
+        <v>653</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>409</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>646</v>
       </c>
       <c r="H99" s="10" t="s">
-        <v>613</v>
+        <v>640</v>
       </c>
       <c r="I99" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="K99" s="10">
+        <v>1</v>
       </c>
       <c r="L99" s="10" t="s">
         <v>408</v>
       </c>
       <c r="M99" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N99" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O99" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="W99" s="10" t="s">
-        <v>416</v>
+        <v>16</v>
       </c>
       <c r="X99" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y99" s="11" t="s">
         <v>154</v>
       </c>
       <c r="Z99" s="11" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>392</v>
+        <v>647</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>395</v>
+        <v>652</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>409</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>648</v>
       </c>
       <c r="H100" s="10" t="s">
-        <v>613</v>
+        <v>640</v>
       </c>
       <c r="I100" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="K100" s="10">
+        <v>1</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>408</v>
       </c>
       <c r="M100" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N100" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O100" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="W100" s="10" t="s">
-        <v>416</v>
+        <v>16</v>
       </c>
       <c r="X100" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y100" s="11" t="s">
         <v>154</v>
       </c>
       <c r="Z100" s="11" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>393</v>
+        <v>649</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>396</v>
+        <v>651</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>409</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>650</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>613</v>
+        <v>640</v>
       </c>
       <c r="I101" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="K101" s="10">
+        <v>1</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>408</v>
       </c>
       <c r="M101" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N101" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O101" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="W101" s="10" t="s">
-        <v>416</v>
+        <v>16</v>
       </c>
       <c r="X101" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y101" s="11" t="s">
         <v>154</v>
       </c>
       <c r="Z101" s="11" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>313</v>
+        <v>161</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>409</v>
@@ -13313,7 +13349,7 @@
         <v>171</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>639</v>
+        <v>613</v>
       </c>
       <c r="I102" s="10" t="s">
         <v>89</v>
@@ -13333,25 +13369,28 @@
       <c r="O102" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="W102" s="10" t="s">
+        <v>416</v>
+      </c>
       <c r="X102" s="11">
         <v>0</v>
       </c>
       <c r="Y102" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z102" s="11" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>313</v>
+        <v>161</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>409</v>
@@ -13360,7 +13399,7 @@
         <v>171</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>639</v>
+        <v>613</v>
       </c>
       <c r="I103" s="10" t="s">
         <v>89</v>
@@ -13380,61 +13419,58 @@
       <c r="O103" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="W103" s="10" t="s">
+        <v>416</v>
+      </c>
       <c r="X103" s="11">
         <v>0</v>
       </c>
       <c r="Y103" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z103" s="11" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>217</v>
+        <v>393</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>218</v>
+        <v>396</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="E104" s="10">
-        <v>1</v>
+        <v>409</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G104" s="10" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="H104" s="10" t="s">
-        <v>637</v>
+        <v>613</v>
       </c>
       <c r="I104" s="10" t="s">
-        <v>283</v>
+        <v>89</v>
       </c>
       <c r="J104" s="10" t="s">
         <v>30</v>
       </c>
       <c r="L104" s="10" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M104" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N104" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="O104" s="10" t="s">
         <v>282</v>
       </c>
       <c r="W104" s="10" t="s">
-        <v>171</v>
+        <v>416</v>
       </c>
       <c r="X104" s="11">
         <v>0</v>
@@ -13443,86 +13479,74 @@
         <v>154</v>
       </c>
       <c r="Z104" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>225</v>
+        <v>397</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>222</v>
+        <v>400</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="E105" s="10">
-        <v>2</v>
+        <v>409</v>
       </c>
       <c r="F105" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="I105" s="10" t="s">
-        <v>283</v>
+        <v>89</v>
       </c>
       <c r="J105" s="10" t="s">
         <v>30</v>
       </c>
       <c r="L105" s="10" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M105" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N105" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="O105" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="W105" s="10" t="s">
-        <v>416</v>
-      </c>
       <c r="X105" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y105" s="11" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="Z105" s="11" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>35</v>
+        <v>398</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>303</v>
+        <v>399</v>
       </c>
       <c r="C106" s="10" t="s">
-        <v>252</v>
+        <v>313</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>409</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G106" s="10" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>618</v>
+        <v>639</v>
       </c>
       <c r="I106" s="10" t="s">
         <v>89</v>
@@ -13531,79 +13555,241 @@
         <v>30</v>
       </c>
       <c r="L106" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="M106" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N106" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O106" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="X106" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y106" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z106" s="11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1</v>
+      </c>
+      <c r="F107" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H107" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="I107" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L107" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="M106" s="10" t="s">
+      <c r="M107" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N106" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O106" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="S106" s="10">
+      <c r="N107" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O107" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W107" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="X107" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y107" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z107" s="11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E108" s="10">
+        <v>2</v>
+      </c>
+      <c r="F108" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G108" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>637</v>
+      </c>
+      <c r="I108" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="J108" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L108" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="M108" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N108" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O108" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="W108" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="X108" s="11">
         <v>1</v>
       </c>
-      <c r="U106" s="10">
+      <c r="Y108" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z108" s="11" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="F109" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G109" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>618</v>
+      </c>
+      <c r="I109" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L109" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="M109" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N109" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O109" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="S109" s="10">
         <v>1</v>
       </c>
-      <c r="W106" s="10" t="s">
+      <c r="U109" s="10">
+        <v>1</v>
+      </c>
+      <c r="W109" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="X106" s="11">
+      <c r="X109" s="11">
         <v>1</v>
       </c>
-      <c r="Y106" s="11" t="s">
+      <c r="Y109" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="Z106" s="11" t="s">
+      <c r="Z109" s="11" t="s">
         <v>540</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="J1:K106">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
+  <conditionalFormatting sqref="J1:K109">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X107:X10015">
-    <cfRule type="expression" dxfId="41" priority="12">
+  <conditionalFormatting sqref="X110:X10018">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G106">
-    <cfRule type="expression" dxfId="40" priority="11">
+  <conditionalFormatting sqref="G2:G109">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W106">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+  <conditionalFormatting sqref="W2:W109">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K106">
-    <cfRule type="expression" dxfId="36" priority="21">
+  <conditionalFormatting sqref="K2:K109">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X107:X1048576">
+  <conditionalFormatting sqref="X110:X1048576">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -13615,31 +13801,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X106">
-    <cfRule type="expression" dxfId="35" priority="7">
+  <conditionalFormatting sqref="X2:X109">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z106">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+  <conditionalFormatting sqref="Z2:Z109">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y106">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
-      <formula>"calc"</formula>
+  <conditionalFormatting sqref="Y2:Y109">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
-      <formula>"dfm.q"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added retransformation of qualitative forecasts to d1 and st forms (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4485476-3FD9-45AE-A282-8E3B7BF0A47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB77392-850F-4776-9FF1-3FD50CDD0080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="654">
   <si>
     <t>gdp</t>
   </si>
@@ -8031,8 +8031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12224,7 +12224,7 @@
         <v>154</v>
       </c>
       <c r="Z81" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
@@ -12454,7 +12454,7 @@
         <v>154</v>
       </c>
       <c r="Z85" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.25">
@@ -12569,7 +12569,7 @@
         <v>154</v>
       </c>
       <c r="Z87" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
@@ -12796,7 +12796,7 @@
         <v>154</v>
       </c>
       <c r="Z91" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.25">
@@ -13618,9 +13618,6 @@
       </c>
       <c r="O107" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="W107" s="10" t="s">
-        <v>171</v>
       </c>
       <c r="X107" s="11">
         <v>0</v>

</xml_diff>

<commit_message>
Added S&P 500 qualitative forecasts & CSM forecast date calculations (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9F0FD-0269-48A2-AA5E-F2A2DA01875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D63E0D-6761-4DE1-824E-914D4F4C5281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2135,7 +2135,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="72">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2687,27 +2750,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
@@ -3052,23 +3094,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="64"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3081,7 +3123,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="52"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3089,35 +3131,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:Z109" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="32"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="20"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="18"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="17"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="16"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="15"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="14"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3145,7 +3187,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7743,17 +7785,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="71" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="64" priority="2">
+    <cfRule type="expression" dxfId="70" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8031,8 +8073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13747,42 +13789,42 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K109">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="15" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X110:X10018">
-    <cfRule type="expression" dxfId="41" priority="12">
+    <cfRule type="expression" dxfId="47" priority="12">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G109">
-    <cfRule type="expression" dxfId="40" priority="11">
+    <cfRule type="expression" dxfId="46" priority="11">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W109">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K109">
-    <cfRule type="expression" dxfId="36" priority="21">
+    <cfRule type="expression" dxfId="45" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13799,29 +13841,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X109">
-    <cfRule type="expression" dxfId="35" priority="7">
+    <cfRule type="expression" dxfId="44" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z109">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y109">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated CSM forecasting for new inputs (v0.15)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D63E0D-6761-4DE1-824E-914D4F4C5281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1906C653-ADC5-4C7E-883E-D8CF3A3A3EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2135,49 +2135,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="66">
     <dxf>
       <fill>
         <patternFill>
@@ -3094,23 +3052,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="64"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="61"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="57"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="56"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3123,7 +3081,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3131,35 +3089,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:Z109" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="33"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="32"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="21"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="17"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="16"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="15"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="13"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="26"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="11"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="10"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="9"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3187,7 +3145,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7785,17 +7743,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="71" priority="3">
+    <cfRule type="expression" dxfId="65" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="64" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="69" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8073,8 +8031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9628,7 +9586,7 @@
         <v>153</v>
       </c>
       <c r="Z29" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
@@ -13789,42 +13747,42 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K109">
-    <cfRule type="cellIs" dxfId="51" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X110:X10018">
-    <cfRule type="expression" dxfId="47" priority="12">
+    <cfRule type="expression" dxfId="41" priority="12">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G109">
-    <cfRule type="expression" dxfId="46" priority="11">
+    <cfRule type="expression" dxfId="40" priority="11">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W109">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K109">
-    <cfRule type="expression" dxfId="45" priority="21">
+    <cfRule type="expression" dxfId="39" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13841,29 +13799,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X109">
-    <cfRule type="expression" dxfId="44" priority="7">
+    <cfRule type="expression" dxfId="38" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z109">
-    <cfRule type="cellIs" dxfId="43" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y109">
-    <cfRule type="cellIs" dxfId="40" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added new CSM equations (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1906C653-ADC5-4C7E-883E-D8CF3A3A3EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C57276C-A15C-43BB-BCEB-E3FFA722A181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="653">
   <si>
     <t>gdp</t>
   </si>
@@ -1663,9 +1663,6 @@
   </si>
   <si>
     <t>core.exog</t>
-  </si>
-  <si>
-    <t>post.exog</t>
   </si>
   <si>
     <t>BEA.GDP</t>
@@ -2136,27 +2133,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="66">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2708,6 +2684,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
@@ -3089,35 +3086,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:Z109" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="26"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="15"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="14"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="13"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="12"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="11"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="10"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="9"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="8"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3145,7 +3142,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7494,7 +7491,7 @@
         <v>156</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>94</v>
@@ -8031,8 +8028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="W94" sqref="W94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8080,7 +8077,7 @@
         <v>164</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>88</v>
@@ -8160,7 +8157,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>283</v>
@@ -8229,7 +8226,7 @@
         <v>106</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>283</v>
@@ -8286,7 +8283,7 @@
         <v>107</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>283</v>
@@ -8311,7 +8308,7 @@
         <v>171</v>
       </c>
       <c r="Z4" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -8337,7 +8334,7 @@
         <v>108</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>283</v>
@@ -8388,7 +8385,7 @@
         <v>172</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>283</v>
@@ -8439,7 +8436,7 @@
         <v>173</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>283</v>
@@ -8490,7 +8487,7 @@
         <v>174</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>283</v>
@@ -8541,7 +8538,7 @@
         <v>175</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>283</v>
@@ -8592,7 +8589,7 @@
         <v>109</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>283</v>
@@ -8643,7 +8640,7 @@
         <v>110</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>283</v>
@@ -8694,7 +8691,7 @@
         <v>180</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>283</v>
@@ -8745,7 +8742,7 @@
         <v>181</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>283</v>
@@ -8796,7 +8793,7 @@
         <v>182</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>283</v>
@@ -8847,7 +8844,7 @@
         <v>111</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>283</v>
@@ -8872,7 +8869,7 @@
         <v>171</v>
       </c>
       <c r="Z15" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -8898,7 +8895,7 @@
         <v>112</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>283</v>
@@ -8949,7 +8946,7 @@
         <v>113</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>283</v>
@@ -9000,7 +8997,7 @@
         <v>114</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>283</v>
@@ -9051,7 +9048,7 @@
         <v>115</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>283</v>
@@ -9102,7 +9099,7 @@
         <v>116</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>283</v>
@@ -9153,7 +9150,7 @@
         <v>117</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>283</v>
@@ -9204,7 +9201,7 @@
         <v>118</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>283</v>
@@ -9255,7 +9252,7 @@
         <v>119</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>283</v>
@@ -9306,7 +9303,7 @@
         <v>102</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>283</v>
@@ -9357,7 +9354,7 @@
         <v>120</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>283</v>
@@ -9408,7 +9405,7 @@
         <v>206</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>283</v>
@@ -9459,7 +9456,7 @@
         <v>207</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>283</v>
@@ -9510,7 +9507,7 @@
         <v>208</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>283</v>
@@ -9561,7 +9558,7 @@
         <v>121</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>283</v>
@@ -9612,7 +9609,7 @@
         <v>122</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>283</v>
@@ -9663,7 +9660,7 @@
         <v>123</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>283</v>
@@ -9714,7 +9711,7 @@
         <v>170</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>283</v>
@@ -9765,7 +9762,7 @@
         <v>213</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>283</v>
@@ -9816,7 +9813,7 @@
         <v>214</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>283</v>
@@ -9867,7 +9864,7 @@
         <v>169</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>283</v>
@@ -9918,7 +9915,7 @@
         <v>215</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>283</v>
@@ -9969,7 +9966,7 @@
         <v>216</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>283</v>
@@ -10020,7 +10017,7 @@
         <v>124</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>283</v>
@@ -10071,7 +10068,7 @@
         <v>125</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>283</v>
@@ -10096,7 +10093,7 @@
         <v>153</v>
       </c>
       <c r="Z39" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
@@ -10122,7 +10119,7 @@
         <v>126</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>283</v>
@@ -10147,7 +10144,7 @@
         <v>153</v>
       </c>
       <c r="Z40" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
@@ -10170,7 +10167,7 @@
         <v>100</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>283</v>
@@ -10220,7 +10217,7 @@
         <v>195</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>283</v>
@@ -10270,7 +10267,7 @@
         <v>192</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>283</v>
@@ -10320,7 +10317,7 @@
         <v>193</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I44" s="10" t="s">
         <v>283</v>
@@ -10370,7 +10367,7 @@
         <v>194</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I45" s="10" t="s">
         <v>283</v>
@@ -10423,7 +10420,7 @@
         <v>220</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>283</v>
@@ -10476,7 +10473,7 @@
         <v>230</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I47" s="10" t="s">
         <v>283</v>
@@ -10529,7 +10526,7 @@
         <v>229</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I48" s="10" t="s">
         <v>283</v>
@@ -10579,7 +10576,7 @@
         <v>32</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I49" s="10" t="s">
         <v>94</v>
@@ -10632,7 +10629,7 @@
         <v>299</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I50" s="10" t="s">
         <v>300</v>
@@ -10659,7 +10656,7 @@
         <v>154</v>
       </c>
       <c r="Z50" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
@@ -10682,7 +10679,7 @@
         <v>314</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I51" s="10" t="s">
         <v>315</v>
@@ -10709,7 +10706,7 @@
         <v>154</v>
       </c>
       <c r="Z51" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
@@ -10732,7 +10729,7 @@
         <v>324</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I52" s="10" t="s">
         <v>315</v>
@@ -10782,7 +10779,7 @@
         <v>317</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I53" s="10" t="s">
         <v>310</v>
@@ -10832,7 +10829,7 @@
         <v>320</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I54" s="10" t="s">
         <v>321</v>
@@ -10882,7 +10879,7 @@
         <v>309</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I55" s="10" t="s">
         <v>310</v>
@@ -10932,7 +10929,7 @@
         <v>33</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I56" s="10" t="s">
         <v>196</v>
@@ -10982,7 +10979,7 @@
         <v>304</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I57" s="10" t="s">
         <v>305</v>
@@ -11032,7 +11029,7 @@
         <v>328</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I58" s="10" t="s">
         <v>315</v>
@@ -11082,7 +11079,7 @@
         <v>38</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I59" s="10" t="s">
         <v>94</v>
@@ -11132,7 +11129,7 @@
         <v>331</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I60" s="10" t="s">
         <v>332</v>
@@ -11182,7 +11179,7 @@
         <v>42</v>
       </c>
       <c r="H61" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I61" s="10" t="s">
         <v>284</v>
@@ -11232,7 +11229,7 @@
         <v>44</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I62" s="10" t="s">
         <v>284</v>
@@ -11282,7 +11279,7 @@
         <v>48</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I63" s="10" t="s">
         <v>94</v>
@@ -11332,7 +11329,7 @@
         <v>50</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I64" s="10" t="s">
         <v>94</v>
@@ -11382,7 +11379,7 @@
         <v>52</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I65" s="10" t="s">
         <v>165</v>
@@ -11432,7 +11429,7 @@
         <v>91</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I66" s="10" t="s">
         <v>95</v>
@@ -11482,7 +11479,7 @@
         <v>55</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I67" s="10" t="s">
         <v>94</v>
@@ -11532,7 +11529,7 @@
         <v>82</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I68" s="10" t="s">
         <v>166</v>
@@ -11582,7 +11579,7 @@
         <v>84</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I69" s="10" t="s">
         <v>94</v>
@@ -11632,7 +11629,7 @@
         <v>97</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>99</v>
@@ -11682,7 +11679,7 @@
         <v>239</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I71" s="10" t="s">
         <v>89</v>
@@ -11730,7 +11727,7 @@
         <v>240</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I72" s="10" t="s">
         <v>89</v>
@@ -11778,7 +11775,7 @@
         <v>241</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>89</v>
@@ -11811,7 +11808,7 @@
         <v>291</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>242</v>
@@ -11823,10 +11820,10 @@
         <v>156</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I74" s="10" t="s">
         <v>94</v>
@@ -11876,7 +11873,7 @@
         <v>244</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I75" s="10" t="s">
         <v>94</v>
@@ -11926,7 +11923,7 @@
         <v>295</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>94</v>
@@ -11976,7 +11973,7 @@
         <v>253</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I77" s="10" t="s">
         <v>94</v>
@@ -12026,7 +12023,7 @@
         <v>335</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I78" s="10" t="s">
         <v>89</v>
@@ -12076,7 +12073,7 @@
         <v>338</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>89</v>
@@ -12126,7 +12123,7 @@
         <v>28</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>89</v>
@@ -12188,7 +12185,7 @@
         <v>29</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I81" s="10" t="s">
         <v>89</v>
@@ -12247,7 +12244,7 @@
         <v>19</v>
       </c>
       <c r="H82" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>89</v>
@@ -12309,7 +12306,7 @@
         <v>21</v>
       </c>
       <c r="H83" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I83" s="10" t="s">
         <v>89</v>
@@ -12365,7 +12362,7 @@
         <v>22</v>
       </c>
       <c r="H84" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I84" s="10" t="s">
         <v>89</v>
@@ -12421,7 +12418,7 @@
         <v>23</v>
       </c>
       <c r="H85" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I85" s="10" t="s">
         <v>89</v>
@@ -12477,7 +12474,7 @@
         <v>401</v>
       </c>
       <c r="H86" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I86" s="10" t="s">
         <v>89</v>
@@ -12536,7 +12533,7 @@
         <v>24</v>
       </c>
       <c r="H87" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I87" s="10" t="s">
         <v>89</v>
@@ -12592,7 +12589,7 @@
         <v>25</v>
       </c>
       <c r="H88" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I88" s="10" t="s">
         <v>89</v>
@@ -12651,7 +12648,7 @@
         <v>26</v>
       </c>
       <c r="H89" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I89" s="10" t="s">
         <v>89</v>
@@ -12707,7 +12704,7 @@
         <v>20</v>
       </c>
       <c r="H90" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I90" s="10" t="s">
         <v>89</v>
@@ -12763,7 +12760,7 @@
         <v>27</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I91" s="10" t="s">
         <v>89</v>
@@ -12819,7 +12816,7 @@
         <v>348</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I92" s="10" t="s">
         <v>89</v>
@@ -12841,6 +12838,9 @@
       </c>
       <c r="O92" s="10" t="s">
         <v>282</v>
+      </c>
+      <c r="W92" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="X92" s="11">
         <v>0</v>
@@ -12872,7 +12872,7 @@
         <v>349</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I93" s="10" t="s">
         <v>89</v>
@@ -12894,6 +12894,9 @@
       </c>
       <c r="O93" s="10" t="s">
         <v>282</v>
+      </c>
+      <c r="W93" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="X93" s="11">
         <v>0</v>
@@ -12925,7 +12928,7 @@
         <v>350</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I94" s="10" t="s">
         <v>89</v>
@@ -12978,7 +12981,7 @@
         <v>351</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I95" s="10" t="s">
         <v>94</v>
@@ -13028,7 +13031,7 @@
         <v>171</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I96" s="10" t="s">
         <v>89</v>
@@ -13084,7 +13087,7 @@
         <v>289</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I97" s="10" t="s">
         <v>94</v>
@@ -13140,7 +13143,7 @@
         <v>290</v>
       </c>
       <c r="H98" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I98" s="10" t="s">
         <v>94</v>
@@ -13170,15 +13173,15 @@
         <v>154</v>
       </c>
       <c r="Z98" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>238</v>
@@ -13190,10 +13193,10 @@
         <v>249</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H99" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I99" s="10" t="s">
         <v>94</v>
@@ -13223,15 +13226,15 @@
         <v>154</v>
       </c>
       <c r="Z99" s="11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>238</v>
@@ -13243,10 +13246,10 @@
         <v>249</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H100" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I100" s="10" t="s">
         <v>94</v>
@@ -13276,15 +13279,15 @@
         <v>154</v>
       </c>
       <c r="Z100" s="11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>238</v>
@@ -13296,10 +13299,10 @@
         <v>249</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I101" s="10" t="s">
         <v>94</v>
@@ -13329,7 +13332,7 @@
         <v>154</v>
       </c>
       <c r="Z101" s="11" t="s">
-        <v>541</v>
+        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
@@ -13349,7 +13352,7 @@
         <v>171</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I102" s="10" t="s">
         <v>89</v>
@@ -13399,7 +13402,7 @@
         <v>171</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I103" s="10" t="s">
         <v>89</v>
@@ -13449,7 +13452,7 @@
         <v>171</v>
       </c>
       <c r="H104" s="10" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I104" s="10" t="s">
         <v>89</v>
@@ -13499,7 +13502,7 @@
         <v>171</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I105" s="10" t="s">
         <v>89</v>
@@ -13518,6 +13521,9 @@
       </c>
       <c r="O105" s="10" t="s">
         <v>282</v>
+      </c>
+      <c r="W105" s="10" t="s">
+        <v>416</v>
       </c>
       <c r="X105" s="11">
         <v>0</v>
@@ -13546,7 +13552,7 @@
         <v>171</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I106" s="10" t="s">
         <v>89</v>
@@ -13565,6 +13571,9 @@
       </c>
       <c r="O106" s="10" t="s">
         <v>282</v>
+      </c>
+      <c r="W106" s="10" t="s">
+        <v>416</v>
       </c>
       <c r="X106" s="11">
         <v>0</v>
@@ -13599,7 +13608,7 @@
         <v>221</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I107" s="10" t="s">
         <v>283</v>
@@ -13626,7 +13635,7 @@
         <v>154</v>
       </c>
       <c r="Z107" s="11" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.25">
@@ -13652,7 +13661,7 @@
         <v>87</v>
       </c>
       <c r="H108" s="10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I108" s="10" t="s">
         <v>283</v>
@@ -13705,7 +13714,7 @@
         <v>36</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I109" s="10" t="s">
         <v>89</v>
@@ -13771,18 +13780,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W109">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K109">
-    <cfRule type="expression" dxfId="39" priority="21">
+    <cfRule type="expression" dxfId="36" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13799,29 +13808,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X109">
-    <cfRule type="expression" dxfId="38" priority="7">
+    <cfRule type="expression" dxfId="35" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z109">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y109">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13852,33 +13861,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1" t="s">
         <v>544</v>
       </c>
-      <c r="B1" t="s">
-        <v>543</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>545</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>546</v>
       </c>
-      <c r="E1" t="s">
-        <v>547</v>
-      </c>
       <c r="F1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C2" t="s">
         <v>548</v>
-      </c>
-      <c r="C2" t="s">
-        <v>549</v>
       </c>
       <c r="D2" t="s">
         <v>156</v>
@@ -13889,13 +13898,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
         <v>156</v>
@@ -13906,13 +13915,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D4" t="s">
         <v>156</v>
@@ -13923,13 +13932,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D5" t="s">
         <v>156</v>
@@ -13940,13 +13949,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B6" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C6" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D6" t="s">
         <v>156</v>
@@ -13957,13 +13966,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B7" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D7" t="s">
         <v>156</v>
@@ -13974,13 +13983,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B8" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D8" t="s">
         <v>156</v>
@@ -13991,13 +14000,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D9" t="s">
         <v>156</v>
@@ -14008,13 +14017,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D10" t="s">
         <v>156</v>
@@ -14025,13 +14034,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D11" t="s">
         <v>156</v>
@@ -14042,13 +14051,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C12" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D12" t="s">
         <v>156</v>
@@ -14059,13 +14068,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C13" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D13" t="s">
         <v>156</v>
@@ -14074,18 +14083,18 @@
         <v>465</v>
       </c>
       <c r="F13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D14" t="s">
         <v>156</v>
@@ -14096,13 +14105,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B15" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D15" t="s">
         <v>156</v>
@@ -14113,7 +14122,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
@@ -14125,18 +14134,18 @@
         <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C17" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D17" t="s">
         <v>156</v>
@@ -14147,13 +14156,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B18" t="s">
+        <v>632</v>
+      </c>
+      <c r="C18" t="s">
         <v>633</v>
-      </c>
-      <c r="C18" t="s">
-        <v>634</v>
       </c>
       <c r="D18" t="s">
         <v>156</v>
@@ -14164,13 +14173,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C19" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D19" t="s">
         <v>156</v>
@@ -14179,18 +14188,18 @@
         <v>341</v>
       </c>
       <c r="F19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B20" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D20" t="s">
         <v>156</v>
@@ -14201,13 +14210,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B21" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C21" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D21" t="s">
         <v>156</v>
@@ -14218,13 +14227,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B22" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D22" t="s">
         <v>156</v>
@@ -14233,18 +14242,18 @@
         <v>321</v>
       </c>
       <c r="F22" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B23" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D23" t="s">
         <v>156</v>
@@ -14253,18 +14262,18 @@
         <v>374</v>
       </c>
       <c r="F23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C24" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D24" t="s">
         <v>156</v>
@@ -14273,18 +14282,18 @@
         <v>351</v>
       </c>
       <c r="F24" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B25" t="s">
         <v>251</v>
       </c>
       <c r="C25" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
@@ -14295,10 +14304,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B26" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D26" t="s">
         <v>156</v>
@@ -14309,13 +14318,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B27" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C27" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D27" t="s">
         <v>156</v>
@@ -14326,13 +14335,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B28" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C28" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D28" t="s">
         <v>156</v>
@@ -14343,13 +14352,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B29" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C29" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D29" t="s">
         <v>156</v>
@@ -14360,13 +14369,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B30" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C30" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D30" t="s">
         <v>156</v>
@@ -14377,13 +14386,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B31" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D31" t="s">
         <v>156</v>
@@ -14394,13 +14403,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>639</v>
+      </c>
+      <c r="B32" t="s">
         <v>640</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>641</v>
-      </c>
-      <c r="C32" t="s">
-        <v>642</v>
       </c>
       <c r="D32" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
Added qual.calc forecasts of mort30y and mort15y (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004E3D97-5E89-4246-95F4-156A4D74F34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B041887B-097A-45CB-865A-A27E765E5968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8028,8 +8028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="Y104" sqref="Y104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12846,10 +12846,10 @@
         <v>0</v>
       </c>
       <c r="Y92" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z92" s="11" t="s">
-        <v>282</v>
+        <v>538</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.25">
@@ -12902,10 +12902,10 @@
         <v>0</v>
       </c>
       <c r="Y93" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z93" s="11" t="s">
-        <v>282</v>
+        <v>538</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Split CSM forecasting by scenario (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B041887B-097A-45CB-865A-A27E765E5968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CB2100-9AFA-43AA-A451-F011490CA2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <sheet name="initial-forecasts-qual" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -8028,8 +8029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="Y104" sqref="Y104"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="P105" sqref="P105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tested different parameters for fitting quarterly nowcast variables (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CB2100-9AFA-43AA-A451-F011490CA2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72F36F2-45C9-4B21-A948-012524198552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8030,7 +8030,7 @@
   <dimension ref="A1:Z109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="P105" sqref="P105"/>
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Got rid of some poorly predictive external indices (CFNAI & WEI), replaced with JOLTS and FRB.H8 predictors (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72F36F2-45C9-4B21-A948-012524198552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F1E378-25F2-4356-AAE3-329BC35B4062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3711" uniqueCount="666">
   <si>
     <t>gdp</t>
   </si>
@@ -2013,6 +2013,45 @@
   </si>
   <si>
     <t>Mortgage 30Y - Treasury 30Y Spread</t>
+  </si>
+  <si>
+    <t>bankcredit</t>
+  </si>
+  <si>
+    <t>Total Bank Credit</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>TOTBKCR</t>
+  </si>
+  <si>
+    <t>$bn</t>
+  </si>
+  <si>
+    <t>bankre</t>
+  </si>
+  <si>
+    <t>bankdeposits</t>
+  </si>
+  <si>
+    <t>Bank Deposits</t>
+  </si>
+  <si>
+    <t>DPSACBW027SBOG</t>
+  </si>
+  <si>
+    <t>bankci</t>
+  </si>
+  <si>
+    <t>Bank Commercial &amp; Industrial Loans</t>
+  </si>
+  <si>
+    <t>TOTCI</t>
+  </si>
+  <si>
+    <t>Bank Real Estate Loans</t>
   </si>
 </sst>
 </file>
@@ -2133,7 +2172,376 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="99">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2627,125 +3035,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3011,25 +3300,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3050,23 +3320,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="95"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="94"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="91"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="86"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3079,7 +3349,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="82"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3087,35 +3357,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z109" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:Z109" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z111" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:Z111" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="78"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="77"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="76"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="73"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="72"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="65"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="64"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="63"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="62"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="61"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="60"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="59"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="58"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="57"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="56"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3143,7 +3413,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="53"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3450,7 +3720,7 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7741,17 +8011,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="64" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8027,10 +8297,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
-  <dimension ref="A1:Z109"/>
+  <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G109" sqref="G109"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="X58" sqref="X58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11042,7 +11312,7 @@
         <v>405</v>
       </c>
       <c r="M58" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N58" s="10" t="s">
         <v>16</v>
@@ -11051,7 +11321,7 @@
         <v>282</v>
       </c>
       <c r="X58" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y58" s="11" t="s">
         <v>154</v>
@@ -11101,7 +11371,7 @@
         <v>282</v>
       </c>
       <c r="X59" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y59" s="11" t="s">
         <v>154</v>
@@ -11162,22 +11432,22 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>41</v>
+        <v>662</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>75</v>
+        <v>663</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>407</v>
+        <v>655</v>
       </c>
       <c r="F61" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>42</v>
+        <v>664</v>
       </c>
       <c r="H61" s="10" t="s">
         <v>608</v>
@@ -11186,7 +11456,10 @@
         <v>284</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="K61" s="10">
+        <v>1</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>405</v>
@@ -11195,7 +11468,7 @@
         <v>15</v>
       </c>
       <c r="N61" s="10" t="s">
-        <v>101</v>
+        <v>390</v>
       </c>
       <c r="O61" s="10" t="s">
         <v>282</v>
@@ -11212,22 +11485,22 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>43</v>
+        <v>659</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>76</v>
+        <v>660</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>162</v>
+        <v>238</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>407</v>
+        <v>655</v>
       </c>
       <c r="F62" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>44</v>
+        <v>661</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>608</v>
@@ -11236,7 +11509,10 @@
         <v>284</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="K62" s="10">
+        <v>1</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>405</v>
@@ -11245,7 +11521,7 @@
         <v>15</v>
       </c>
       <c r="N62" s="10" t="s">
-        <v>101</v>
+        <v>390</v>
       </c>
       <c r="O62" s="10" t="s">
         <v>282</v>
@@ -11262,40 +11538,43 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>47</v>
+        <v>658</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>78</v>
+        <v>665</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>238</v>
+        <v>160</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>407</v>
+        <v>655</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>94</v>
+        <v>284</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="K63" s="10">
+        <v>1</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>405</v>
       </c>
       <c r="M63" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N63" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O63" s="10" t="s">
         <v>282</v>
@@ -11312,10 +11591,10 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>238</v>
@@ -11327,10 +11606,10 @@
         <v>156</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>609</v>
+        <v>618</v>
       </c>
       <c r="I64" s="10" t="s">
         <v>94</v>
@@ -11362,13 +11641,13 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>407</v>
@@ -11377,13 +11656,13 @@
         <v>156</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="J65" s="10" t="s">
         <v>30</v>
@@ -11412,13 +11691,13 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>407</v>
@@ -11427,13 +11706,13 @@
         <v>156</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="J66" s="10" t="s">
         <v>30</v>
@@ -11442,10 +11721,10 @@
         <v>405</v>
       </c>
       <c r="M66" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="O66" s="10" t="s">
         <v>282</v>
@@ -11462,13 +11741,13 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>407</v>
@@ -11477,13 +11756,13 @@
         <v>156</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J67" s="10" t="s">
         <v>30</v>
@@ -11492,10 +11771,10 @@
         <v>405</v>
       </c>
       <c r="M67" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N67" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="O67" s="10" t="s">
         <v>282</v>
@@ -11512,13 +11791,13 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>407</v>
@@ -11527,13 +11806,13 @@
         <v>156</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>30</v>
@@ -11562,13 +11841,13 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>231</v>
+        <v>80</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>407</v>
@@ -11577,13 +11856,13 @@
         <v>156</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>607</v>
+        <v>627</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="J69" s="10" t="s">
         <v>30</v>
@@ -11592,10 +11871,10 @@
         <v>405</v>
       </c>
       <c r="M69" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N69" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="O69" s="10" t="s">
         <v>282</v>
@@ -11612,13 +11891,13 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>96</v>
+        <v>231</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>407</v>
@@ -11627,13 +11906,13 @@
         <v>156</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>634</v>
+        <v>607</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J70" s="10" t="s">
         <v>30</v>
@@ -11662,13 +11941,13 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>232</v>
+        <v>96</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>233</v>
+        <v>98</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>238</v>
+        <v>163</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>407</v>
@@ -11677,43 +11956,45 @@
         <v>156</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>239</v>
+        <v>97</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>405</v>
       </c>
       <c r="M71" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N71" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="O71" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="X71" s="11"/>
+      <c r="X71" s="11">
+        <v>1</v>
+      </c>
       <c r="Y71" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Z71" s="11" t="s">
-        <v>536</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>238</v>
@@ -11725,7 +12006,7 @@
         <v>156</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H72" s="10" t="s">
         <v>635</v>
@@ -11758,10 +12039,10 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>238</v>
@@ -11773,7 +12054,7 @@
         <v>156</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H73" s="10" t="s">
         <v>635</v>
@@ -11806,13 +12087,13 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>291</v>
+        <v>236</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>641</v>
+        <v>237</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>407</v>
@@ -11821,16 +12102,16 @@
         <v>156</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>640</v>
+        <v>241</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>405</v>
@@ -11844,22 +12125,20 @@
       <c r="O74" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="X74" s="11">
-        <v>1</v>
-      </c>
+      <c r="X74" s="11"/>
       <c r="Y74" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z74" s="11" t="s">
-        <v>282</v>
+        <v>536</v>
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>296</v>
+        <v>641</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>242</v>
@@ -11871,10 +12150,10 @@
         <v>156</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>244</v>
+        <v>640</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="I75" s="10" t="s">
         <v>94</v>
@@ -11906,10 +12185,10 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>242</v>
@@ -11921,10 +12200,10 @@
         <v>156</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>295</v>
+        <v>244</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I76" s="10" t="s">
         <v>94</v>
@@ -11956,13 +12235,13 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>250</v>
+        <v>293</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>251</v>
+        <v>294</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>407</v>
@@ -11971,10 +12250,10 @@
         <v>156</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="I77" s="10" t="s">
         <v>94</v>
@@ -12006,13 +12285,13 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>333</v>
+        <v>250</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>334</v>
+        <v>251</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>407</v>
@@ -12021,13 +12300,13 @@
         <v>156</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>335</v>
+        <v>253</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J78" s="10" t="s">
         <v>30</v>
@@ -12045,7 +12324,7 @@
         <v>282</v>
       </c>
       <c r="X78" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y78" s="11" t="s">
         <v>154</v>
@@ -12056,13 +12335,13 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>252</v>
+        <v>161</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>407</v>
@@ -12071,10 +12350,10 @@
         <v>156</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="I79" s="10" t="s">
         <v>89</v>
@@ -12106,13 +12385,13 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>2</v>
+        <v>336</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>60</v>
+        <v>337</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>407</v>
@@ -12121,22 +12400,19 @@
         <v>156</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>28</v>
+        <v>338</v>
       </c>
       <c r="H80" s="10" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="I80" s="10" t="s">
         <v>89</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="K80" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L80" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M80" s="10" t="s">
         <v>16</v>
@@ -12146,15 +12422,6 @@
       </c>
       <c r="O80" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="U80" s="10">
-        <v>1</v>
-      </c>
-      <c r="V80" s="10">
-        <v>1</v>
-      </c>
-      <c r="W80" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="X80" s="11">
         <v>1</v>
@@ -12163,15 +12430,15 @@
         <v>154</v>
       </c>
       <c r="Z80" s="11" t="s">
-        <v>538</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>161</v>
@@ -12183,10 +12450,10 @@
         <v>156</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I81" s="10" t="s">
         <v>89</v>
@@ -12209,6 +12476,9 @@
       <c r="O81" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="U81" s="10">
+        <v>1</v>
+      </c>
       <c r="V81" s="10">
         <v>1</v>
       </c>
@@ -12216,7 +12486,7 @@
         <v>414</v>
       </c>
       <c r="X81" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y81" s="11" t="s">
         <v>154</v>
@@ -12227,10 +12497,10 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>161</v>
@@ -12242,10 +12512,10 @@
         <v>156</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H82" s="10" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="I82" s="10" t="s">
         <v>89</v>
@@ -12268,17 +12538,14 @@
       <c r="O82" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="S82" s="10">
-        <v>1</v>
-      </c>
       <c r="V82" s="10">
         <v>1</v>
       </c>
       <c r="W82" s="10" t="s">
-        <v>171</v>
+        <v>414</v>
       </c>
       <c r="X82" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y82" s="11" t="s">
         <v>154</v>
@@ -12289,10 +12556,10 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>161</v>
@@ -12304,7 +12571,7 @@
         <v>156</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H83" s="10" t="s">
         <v>610</v>
@@ -12330,11 +12597,17 @@
       <c r="O83" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="S83" s="10">
+        <v>1</v>
+      </c>
+      <c r="V83" s="10">
+        <v>1</v>
+      </c>
       <c r="W83" s="10" t="s">
         <v>171</v>
       </c>
       <c r="X83" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y83" s="11" t="s">
         <v>154</v>
@@ -12345,10 +12618,10 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>161</v>
@@ -12360,7 +12633,7 @@
         <v>156</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H84" s="10" t="s">
         <v>610</v>
@@ -12401,10 +12674,10 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>161</v>
@@ -12416,7 +12689,7 @@
         <v>156</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H85" s="10" t="s">
         <v>610</v>
@@ -12457,10 +12730,10 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>161</v>
@@ -12472,7 +12745,7 @@
         <v>156</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>399</v>
+        <v>23</v>
       </c>
       <c r="H86" s="10" t="s">
         <v>610</v>
@@ -12498,14 +12771,11 @@
       <c r="O86" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="V86" s="10">
-        <v>1</v>
-      </c>
       <c r="W86" s="10" t="s">
         <v>171</v>
       </c>
       <c r="X86" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y86" s="11" t="s">
         <v>154</v>
@@ -12516,10 +12786,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>161</v>
@@ -12531,7 +12801,7 @@
         <v>156</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>24</v>
+        <v>399</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>610</v>
@@ -12557,11 +12827,14 @@
       <c r="O87" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="V87" s="10">
+        <v>1</v>
+      </c>
       <c r="W87" s="10" t="s">
         <v>171</v>
       </c>
       <c r="X87" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y87" s="11" t="s">
         <v>154</v>
@@ -12572,10 +12845,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>161</v>
@@ -12587,7 +12860,7 @@
         <v>156</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H88" s="10" t="s">
         <v>610</v>
@@ -12613,9 +12886,6 @@
       <c r="O88" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="S88" s="10">
-        <v>1</v>
-      </c>
       <c r="W88" s="10" t="s">
         <v>171</v>
       </c>
@@ -12631,10 +12901,10 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>161</v>
@@ -12646,7 +12916,7 @@
         <v>156</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H89" s="10" t="s">
         <v>610</v>
@@ -12672,6 +12942,9 @@
       <c r="O89" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="S89" s="10">
+        <v>1</v>
+      </c>
       <c r="W89" s="10" t="s">
         <v>171</v>
       </c>
@@ -12687,10 +12960,10 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>161</v>
@@ -12702,7 +12975,7 @@
         <v>156</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H90" s="10" t="s">
         <v>610</v>
@@ -12743,10 +13016,10 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>161</v>
@@ -12758,7 +13031,7 @@
         <v>156</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>610</v>
@@ -12799,13 +13072,13 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>341</v>
+        <v>13</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>344</v>
+        <v>67</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>313</v>
+        <v>161</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>407</v>
@@ -12814,16 +13087,16 @@
         <v>156</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>348</v>
+        <v>27</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>636</v>
+        <v>610</v>
       </c>
       <c r="I92" s="10" t="s">
         <v>89</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>388</v>
+        <v>340</v>
       </c>
       <c r="K92" s="10">
         <v>1</v>
@@ -12855,10 +13128,10 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>313</v>
@@ -12870,7 +13143,7 @@
         <v>156</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H93" s="10" t="s">
         <v>636</v>
@@ -12911,13 +13184,13 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>161</v>
+        <v>313</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>407</v>
@@ -12926,7 +13199,7 @@
         <v>156</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H94" s="10" t="s">
         <v>636</v>
@@ -12952,25 +13225,28 @@
       <c r="O94" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="W94" s="10" t="s">
+        <v>171</v>
+      </c>
       <c r="X94" s="11">
         <v>0</v>
       </c>
       <c r="Y94" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z94" s="11" t="s">
-        <v>282</v>
+        <v>538</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>343</v>
+        <v>385</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>407</v>
@@ -12979,22 +13255,25 @@
         <v>156</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>621</v>
+        <v>636</v>
       </c>
       <c r="I95" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="K95" s="10">
+        <v>1</v>
       </c>
       <c r="L95" s="10" t="s">
         <v>406</v>
       </c>
       <c r="M95" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="N95" s="10" t="s">
         <v>16</v>
@@ -13002,14 +13281,11 @@
       <c r="O95" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="U95" s="10">
-        <v>1</v>
-      </c>
       <c r="X95" s="11">
         <v>0</v>
       </c>
       <c r="Y95" s="11" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="Z95" s="11" t="s">
         <v>282</v>
@@ -13017,10 +13293,10 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>386</v>
+        <v>343</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>163</v>
@@ -13029,13 +13305,16 @@
         <v>407</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>171</v>
+        <v>156</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>351</v>
       </c>
       <c r="H96" s="10" t="s">
         <v>621</v>
       </c>
       <c r="I96" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J96" s="10" t="s">
         <v>30</v>
@@ -13044,7 +13323,7 @@
         <v>406</v>
       </c>
       <c r="M96" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="N96" s="10" t="s">
         <v>16</v>
@@ -13052,11 +13331,8 @@
       <c r="O96" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="V96" s="10">
+      <c r="U96" s="10">
         <v>1</v>
-      </c>
-      <c r="W96" s="10" t="s">
-        <v>414</v>
       </c>
       <c r="X96" s="11">
         <v>0</v>
@@ -13065,57 +13341,54 @@
         <v>154</v>
       </c>
       <c r="Z96" s="11" t="s">
-        <v>538</v>
+        <v>282</v>
       </c>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>39</v>
+        <v>386</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>74</v>
+        <v>387</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>238</v>
+        <v>163</v>
       </c>
       <c r="D97" s="10" t="s">
         <v>407</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>289</v>
+        <v>171</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="I97" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="K97" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>406</v>
       </c>
       <c r="M97" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N97" s="10" t="s">
-        <v>390</v>
+        <v>16</v>
       </c>
       <c r="O97" s="10" t="s">
-        <v>16</v>
+        <v>282</v>
+      </c>
+      <c r="V97" s="10">
+        <v>1</v>
       </c>
       <c r="W97" s="10" t="s">
         <v>414</v>
       </c>
       <c r="X97" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y97" s="11" t="s">
         <v>154</v>
@@ -13126,10 +13399,10 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>238</v>
@@ -13141,7 +13414,7 @@
         <v>249</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H98" s="10" t="s">
         <v>637</v>
@@ -13159,13 +13432,16 @@
         <v>406</v>
       </c>
       <c r="M98" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N98" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O98" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
+      </c>
+      <c r="W98" s="10" t="s">
+        <v>414</v>
       </c>
       <c r="X98" s="11">
         <v>1</v>
@@ -13174,15 +13450,15 @@
         <v>154</v>
       </c>
       <c r="Z98" s="11" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>642</v>
+        <v>40</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>650</v>
+        <v>58</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>238</v>
@@ -13194,7 +13470,7 @@
         <v>249</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>643</v>
+        <v>290</v>
       </c>
       <c r="H99" s="10" t="s">
         <v>637</v>
@@ -13212,13 +13488,13 @@
         <v>406</v>
       </c>
       <c r="M99" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N99" s="10" t="s">
-        <v>390</v>
+        <v>16</v>
       </c>
       <c r="O99" s="10" t="s">
-        <v>16</v>
+        <v>282</v>
       </c>
       <c r="X99" s="11">
         <v>1</v>
@@ -13227,15 +13503,15 @@
         <v>154</v>
       </c>
       <c r="Z99" s="11" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>238</v>
@@ -13247,7 +13523,7 @@
         <v>249</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="H100" s="10" t="s">
         <v>637</v>
@@ -13285,10 +13561,10 @@
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>238</v>
@@ -13300,7 +13576,7 @@
         <v>249</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="H101" s="10" t="s">
         <v>637</v>
@@ -13333,65 +13609,68 @@
         <v>154</v>
       </c>
       <c r="Z101" s="11" t="s">
-        <v>282</v>
+        <v>536</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>391</v>
+        <v>646</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>394</v>
+        <v>648</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>161</v>
+        <v>238</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>407</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>647</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>610</v>
+        <v>637</v>
       </c>
       <c r="I102" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="K102" s="10">
+        <v>1</v>
       </c>
       <c r="L102" s="10" t="s">
         <v>406</v>
       </c>
       <c r="M102" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N102" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="O102" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="W102" s="10" t="s">
-        <v>414</v>
+        <v>16</v>
       </c>
       <c r="X102" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y102" s="11" t="s">
         <v>154</v>
       </c>
       <c r="Z102" s="11" t="s">
-        <v>538</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>161</v>
@@ -13438,10 +13717,10 @@
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>161</v>
@@ -13488,13 +13767,13 @@
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>651</v>
+        <v>393</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>652</v>
+        <v>396</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>313</v>
+        <v>161</v>
       </c>
       <c r="D105" s="10" t="s">
         <v>407</v>
@@ -13503,7 +13782,7 @@
         <v>171</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>636</v>
+        <v>610</v>
       </c>
       <c r="I105" s="10" t="s">
         <v>89</v>
@@ -13530,18 +13809,18 @@
         <v>0</v>
       </c>
       <c r="Y105" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z105" s="11" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>397</v>
+        <v>651</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>398</v>
+        <v>652</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>313</v>
@@ -13588,52 +13867,49 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>217</v>
+        <v>397</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>218</v>
+        <v>398</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="E107" s="10">
-        <v>1</v>
+        <v>407</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="G107" s="10" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="I107" s="10" t="s">
-        <v>283</v>
+        <v>89</v>
       </c>
       <c r="J107" s="10" t="s">
         <v>30</v>
       </c>
       <c r="L107" s="10" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M107" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N107" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="O107" s="10" t="s">
         <v>282</v>
       </c>
+      <c r="W107" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="X107" s="11">
         <v>0</v>
       </c>
       <c r="Y107" s="11" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="Z107" s="11" t="s">
         <v>536</v>
@@ -13641,10 +13917,10 @@
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>162</v>
@@ -13653,13 +13929,13 @@
         <v>218</v>
       </c>
       <c r="E108" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F108" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>87</v>
+        <v>221</v>
       </c>
       <c r="H108" s="10" t="s">
         <v>634</v>
@@ -13682,43 +13958,43 @@
       <c r="O108" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="W108" s="10" t="s">
-        <v>414</v>
-      </c>
       <c r="X108" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y108" s="11" t="s">
         <v>154</v>
       </c>
       <c r="Z108" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>407</v>
+        <v>218</v>
+      </c>
+      <c r="E109" s="10">
+        <v>2</v>
       </c>
       <c r="F109" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>615</v>
+        <v>634</v>
       </c>
       <c r="I109" s="10" t="s">
-        <v>89</v>
+        <v>283</v>
       </c>
       <c r="J109" s="10" t="s">
         <v>30</v>
@@ -13730,16 +14006,10 @@
         <v>15</v>
       </c>
       <c r="N109" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="O109" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="S109" s="10">
-        <v>1</v>
-      </c>
-      <c r="U109" s="10">
-        <v>1</v>
       </c>
       <c r="W109" s="10" t="s">
         <v>414</v>
@@ -13754,84 +14024,184 @@
         <v>538</v>
       </c>
     </row>
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D110" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="F110" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G110" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>615</v>
+      </c>
+      <c r="I110" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L110" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="M110" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N110" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O110" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="S110" s="10">
+        <v>1</v>
+      </c>
+      <c r="U110" s="10">
+        <v>1</v>
+      </c>
+      <c r="W110" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="X110" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y110" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z110" s="11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>655</v>
+      </c>
+      <c r="F111" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G111" s="10" t="s">
+        <v>656</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="I111" s="10" t="s">
+        <v>657</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="K111" s="10">
+        <v>1</v>
+      </c>
+      <c r="L111" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="M111" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N111" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="O111" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="X111" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y111" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z111" s="11" t="s">
+        <v>282</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="J1:K109">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
+  <conditionalFormatting sqref="J1:K111">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X110:X10018">
-    <cfRule type="expression" dxfId="41" priority="12">
+  <conditionalFormatting sqref="X111:X10019">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G109">
-    <cfRule type="expression" dxfId="40" priority="11">
+  <conditionalFormatting sqref="G2:G111">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W109">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+  <conditionalFormatting sqref="W2:W111">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K109">
-    <cfRule type="expression" dxfId="36" priority="21">
+  <conditionalFormatting sqref="K2:K111">
+    <cfRule type="expression" dxfId="7" priority="21">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X110:X1048576">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X109">
-    <cfRule type="expression" dxfId="35" priority="7">
+  <conditionalFormatting sqref="X2:X111">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z109">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+  <conditionalFormatting sqref="Z2:Z111">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y109">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+  <conditionalFormatting sqref="Y2:Y111">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13848,7 +14218,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added quarterly re-aggregation of monthly variables (v0.16)"
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1F76DF-23A1-4353-8B24-31F6C7A22A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9F350-010A-44EC-94EA-F176B8943D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2175,7 +2175,252 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="84">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2669,125 +2914,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3092,23 +3218,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="58"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="77"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="76"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="73"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="69"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3121,7 +3247,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="64"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3129,35 +3255,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z111" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z111" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:Z111" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="59"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="58"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="48"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="47"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="46"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="45"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="44"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="43"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="42"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="41"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="39"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="38"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3185,7 +3311,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="35"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7783,17 +7909,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="65" priority="3">
+    <cfRule type="expression" dxfId="83" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="64" priority="2">
+    <cfRule type="expression" dxfId="82" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8071,17 +8197,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" style="9" customWidth="1"/>
-    <col min="3" max="5" width="15.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="10" customWidth="1"/>
     <col min="6" max="6" width="5.140625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="10" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="10" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="6.85546875" style="10" customWidth="1"/>
@@ -13911,69 +14039,72 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K111">
-    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="15" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="18" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X111:X10019">
-    <cfRule type="expression" dxfId="41" priority="12">
+    <cfRule type="expression" dxfId="30" priority="13">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G111">
-    <cfRule type="expression" dxfId="40" priority="11">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W111">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K111">
-    <cfRule type="expression" dxfId="36" priority="21">
+    <cfRule type="expression" dxfId="25" priority="22">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X111">
-    <cfRule type="expression" dxfId="35" priority="7">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z111">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"core.exog"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+      <formula>"post.endog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y111">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Improved some of the core structural equations (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D9F350-010A-44EC-94EA-F176B8943D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB86129-926A-4F34-BE05-2969898F0630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -22,7 +22,6 @@
     <sheet name="initial-forecasts-qual" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2175,252 +2173,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="67">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2914,6 +2667,132 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3218,23 +3097,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="76"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="69"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="68"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="67"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="52"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3247,7 +3126,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="47"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3255,35 +3134,35 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z111" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:Z111" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:Z111" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="61"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="59"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="58"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="49"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="47"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="46"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="45"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="44"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="43"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="42"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="41"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="40"/>
-    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="39"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="38"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="23"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
+    <tableColumn id="24" xr3:uid="{27D73877-E00B-4043-B0F4-C927FE5C7382}" name="initial_forecast" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3311,7 +3190,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7909,17 +7788,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="83" priority="3">
+    <cfRule type="expression" dxfId="66" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="82" priority="2">
+    <cfRule type="expression" dxfId="65" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8197,8 +8076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="Y97" sqref="Y97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10581,9 +10460,6 @@
       <c r="D46" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E46" s="10">
-        <v>3</v>
-      </c>
       <c r="F46" s="10" t="s">
         <v>156</v>
       </c>
@@ -10618,7 +10494,7 @@
         <v>154</v>
       </c>
       <c r="Z46" s="11" t="s">
-        <v>537</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
@@ -10634,9 +10510,6 @@
       <c r="D47" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E47" s="10">
-        <v>4</v>
-      </c>
       <c r="F47" s="10" t="s">
         <v>156</v>
       </c>
@@ -10671,7 +10544,7 @@
         <v>154</v>
       </c>
       <c r="Z47" s="11" t="s">
-        <v>666</v>
+        <v>282</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
@@ -10687,9 +10560,6 @@
       <c r="D48" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E48" s="10">
-        <v>5</v>
-      </c>
       <c r="F48" s="10" t="s">
         <v>156</v>
       </c>
@@ -10724,7 +10594,7 @@
         <v>171</v>
       </c>
       <c r="Z48" s="11" t="s">
-        <v>666</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
@@ -13185,7 +13055,7 @@
         <v>0</v>
       </c>
       <c r="Y95" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="Z95" s="11" t="s">
         <v>282</v>
@@ -13456,7 +13326,7 @@
         <v>154</v>
       </c>
       <c r="Z100" s="11" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.25">
@@ -13509,7 +13379,7 @@
         <v>154</v>
       </c>
       <c r="Z101" s="11" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.25">
@@ -13828,9 +13698,6 @@
       <c r="D108" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E108" s="10">
-        <v>1</v>
-      </c>
       <c r="F108" s="10" t="s">
         <v>156</v>
       </c>
@@ -13865,7 +13732,7 @@
         <v>154</v>
       </c>
       <c r="Z108" s="11" t="s">
-        <v>536</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.25">
@@ -13881,9 +13748,6 @@
       <c r="D109" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="E109" s="10">
-        <v>2</v>
-      </c>
       <c r="F109" s="10" t="s">
         <v>156</v>
       </c>
@@ -14039,72 +13903,72 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K111">
-    <cfRule type="cellIs" dxfId="34" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="17" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="18" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X111:X10019">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="42" priority="13">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G111">
-    <cfRule type="expression" dxfId="29" priority="12">
+    <cfRule type="expression" dxfId="41" priority="12">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W111">
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K111">
-    <cfRule type="expression" dxfId="25" priority="22">
+    <cfRule type="expression" dxfId="37" priority="22">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X111">
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="36" priority="8">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z111">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y111">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added GDP nowcasts as CSM exogenous variables (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E63D1C6-76E9-4297-B6F0-9DBF107ED076}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C89CE61-0DA9-49C1-8FC8-7AD6E49D1AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8076,8 +8076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="X45" sqref="X45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added split of mandatory exogenous variables versus variables which can be on/off endogenous and exogenous (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB273F0-367E-4695-B76A-F73761604082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB71923-3E22-4EBD-918D-AFE09D18047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3763" uniqueCount="670">
   <si>
     <t>gdp</t>
   </si>
@@ -2061,7 +2061,7 @@
     <t>estimated</t>
   </si>
   <si>
-    <t>identity</t>
+    <t>core.exog.p</t>
   </si>
 </sst>
 </file>
@@ -2182,7 +2182,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="172">
+  <dxfs count="117">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2242,7 +2277,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF41DFDB"/>
+          <bgColor rgb="FF6BF9F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2326,7 +2368,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
+          <bgColor rgb="FFA7FBF9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2383,6 +2425,13 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2494,7 +2543,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2522,7 +2571,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF41DFDB"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2604,475 +2653,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF41DFDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF41DFDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3110,6 +2690,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3829,10 +3425,32 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA7FBF9"/>
+      <color rgb="FF6BF9F6"/>
+      <color rgb="FF9ED2E4"/>
       <color rgb="FF41DFDB"/>
       <color rgb="FFFF9393"/>
       <color rgb="FFFF7D7D"/>
@@ -3850,23 +3468,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="171" dataDxfId="170">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="169"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="168"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="167"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="166"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="164"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="163"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="162"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="161"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="160"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="159"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="158"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="157"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="111"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="109"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="106"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="102"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="101"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3879,7 +3497,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="97"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3887,36 +3505,36 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AA111" totalsRowShown="0" headerRowDxfId="154" dataDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AA111" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
   <autoFilter ref="A1:AA111" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="152"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="151"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="150"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="149"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="147"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="146"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="145"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="144"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="143"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="142"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="141"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="140"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="138"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="137"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="136"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="135"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="134"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="133"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="132"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="131"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="130"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="129"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="127"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="92"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="91"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="88"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="81"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="80"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="79"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="78"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="77"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="76"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="75"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="74"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="73"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="72"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="71"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3944,7 +3562,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="67"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -8542,17 +8160,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="124" priority="3">
+    <cfRule type="expression" dxfId="116" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="123" priority="2">
+    <cfRule type="expression" dxfId="115" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="122" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8831,7 +8449,7 @@
   <dimension ref="A1:AA111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9232,7 +8850,7 @@
         <v>414</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA6" s="11"/>
     </row>
@@ -9287,7 +8905,7 @@
         <v>414</v>
       </c>
       <c r="Z7" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA7" s="11"/>
     </row>
@@ -9342,7 +8960,7 @@
         <v>414</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA8" s="11"/>
     </row>
@@ -9397,7 +9015,7 @@
         <v>414</v>
       </c>
       <c r="Z9" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA9" s="11"/>
     </row>
@@ -9506,7 +9124,7 @@
         <v>414</v>
       </c>
       <c r="Z11" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA11" s="11"/>
     </row>
@@ -9561,7 +9179,7 @@
         <v>414</v>
       </c>
       <c r="Z12" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA12" s="11"/>
     </row>
@@ -9616,7 +9234,7 @@
         <v>414</v>
       </c>
       <c r="Z13" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA13" s="11"/>
     </row>
@@ -9671,7 +9289,7 @@
         <v>414</v>
       </c>
       <c r="Z14" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA14" s="11"/>
     </row>
@@ -9780,7 +9398,7 @@
         <v>414</v>
       </c>
       <c r="Z16" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA16" s="11"/>
     </row>
@@ -9835,7 +9453,7 @@
         <v>414</v>
       </c>
       <c r="Z17" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA17" s="11"/>
     </row>
@@ -9890,7 +9508,7 @@
         <v>414</v>
       </c>
       <c r="Z18" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA18" s="11"/>
     </row>
@@ -9945,7 +9563,7 @@
         <v>414</v>
       </c>
       <c r="Z19" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA19" s="11"/>
     </row>
@@ -10000,7 +9618,7 @@
         <v>414</v>
       </c>
       <c r="Z20" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA20" s="11"/>
     </row>
@@ -10055,7 +9673,7 @@
         <v>414</v>
       </c>
       <c r="Z21" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA21" s="11"/>
     </row>
@@ -10110,7 +9728,7 @@
         <v>414</v>
       </c>
       <c r="Z22" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA22" s="11"/>
     </row>
@@ -10165,7 +9783,7 @@
         <v>414</v>
       </c>
       <c r="Z23" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA23" s="11"/>
     </row>
@@ -10328,7 +9946,7 @@
         <v>414</v>
       </c>
       <c r="Z26" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA26" s="11"/>
     </row>
@@ -10383,7 +10001,7 @@
         <v>414</v>
       </c>
       <c r="Z27" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA27" s="11"/>
     </row>
@@ -10438,7 +10056,7 @@
         <v>414</v>
       </c>
       <c r="Z28" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA28" s="11"/>
     </row>
@@ -10489,8 +10107,11 @@
       <c r="X29" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y29" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z29" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA29" s="11"/>
     </row>
@@ -10699,8 +10320,11 @@
       <c r="X33" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y33" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z33" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA33" s="11"/>
     </row>
@@ -10751,8 +10375,11 @@
       <c r="X34" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y34" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z34" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA34" s="11"/>
     </row>
@@ -10857,8 +10484,11 @@
       <c r="X36" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y36" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z36" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA36" s="11"/>
     </row>
@@ -10909,8 +10539,11 @@
       <c r="X37" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y37" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z37" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA37" s="11"/>
     </row>
@@ -11015,8 +10648,11 @@
       <c r="X39" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y39" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z39" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA39" s="11"/>
     </row>
@@ -11067,8 +10703,11 @@
       <c r="X40" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="Y40" s="10" t="s">
+        <v>414</v>
+      </c>
       <c r="Z40" s="11" t="s">
-        <v>537</v>
+        <v>669</v>
       </c>
       <c r="AA40" s="11"/>
     </row>
@@ -14010,7 +13649,7 @@
         <v>536</v>
       </c>
       <c r="AA95" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
@@ -14063,11 +13702,9 @@
         <v>154</v>
       </c>
       <c r="Z96" s="11" t="s">
-        <v>536</v>
-      </c>
-      <c r="AA96" s="11" t="s">
-        <v>669</v>
-      </c>
+        <v>665</v>
+      </c>
+      <c r="AA96" s="11"/>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
@@ -14602,7 +14239,7 @@
         <v>414</v>
       </c>
       <c r="Z106" s="11" t="s">
-        <v>537</v>
+        <v>282</v>
       </c>
       <c r="AA106" s="11"/>
     </row>
@@ -14653,7 +14290,7 @@
         <v>414</v>
       </c>
       <c r="Z107" s="11" t="s">
-        <v>537</v>
+        <v>282</v>
       </c>
       <c r="AA107" s="11"/>
     </row>
@@ -14879,80 +14516,83 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K111">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="25" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W111:W10019">
-    <cfRule type="expression" dxfId="35" priority="19">
+    <cfRule type="expression" dxfId="42" priority="20">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G111">
-    <cfRule type="expression" dxfId="34" priority="18">
+    <cfRule type="expression" dxfId="41" priority="19">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K111">
-    <cfRule type="expression" dxfId="33" priority="28">
+    <cfRule type="expression" dxfId="40" priority="29">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W111">
-    <cfRule type="expression" dxfId="32" priority="14">
+    <cfRule type="expression" dxfId="39" priority="15">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z111">
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
       <formula>"core.exog"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"core.exog.p"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X111">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>"none"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA111">
-    <cfRule type="expression" dxfId="24" priority="6">
+    <cfRule type="expression" dxfId="30" priority="7">
       <formula>$Z2 &lt;&gt; "core.endog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y111">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed some inputs from nowcasts due to collinearity issues (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EA4EDA-C197-4262-AA63-382F87A7ECCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCBC7F7-0BA0-47A7-9D72-748BCEBB77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2189,205 +2189,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="74">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2629,6 +2430,25 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2896,6 +2716,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3161,6 +3142,25 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3186,23 +3186,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="69"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="66"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="62"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="68"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="66"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="58"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3215,7 +3215,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="54"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3223,37 +3223,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AB111" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AB111" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:AB111" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="51"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="48"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="40"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="39"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="38"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="37"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="36"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="34"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="33"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="32"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="31"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="29"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="25"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3281,7 +3281,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7879,17 +7879,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="26" priority="3">
+    <cfRule type="expression" dxfId="73" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="72" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8167,8 +8167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="X63" sqref="X63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11803,7 +11803,7 @@
         <v>282</v>
       </c>
       <c r="X62" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y62" s="11" t="s">
         <v>154</v>
@@ -13213,7 +13213,7 @@
         <v>1</v>
       </c>
       <c r="X87" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y87" s="11" t="s">
         <v>154</v>
@@ -13636,7 +13636,7 @@
         <v>282</v>
       </c>
       <c r="X94" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y94" s="11" t="s">
         <v>154</v>
@@ -13929,7 +13929,7 @@
         <v>282</v>
       </c>
       <c r="X99" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y99" s="11" t="s">
         <v>154</v>
@@ -13988,7 +13988,7 @@
         <v>16</v>
       </c>
       <c r="X100" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y100" s="11" t="s">
         <v>154</v>
@@ -14620,89 +14620,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="J1:K111">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X111:X10019">
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="49" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G111">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="48" priority="21">
       <formula>$F2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K111">
-    <cfRule type="expression" dxfId="17" priority="31">
+    <cfRule type="expression" dxfId="47" priority="31">
       <formula>OR($J2="q", $J2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X111">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="46" priority="17">
       <formula>AND($J2&lt;&gt;"d", $J2 &lt;&gt; "w", $J2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA111">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y111">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB111">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="34" priority="9">
       <formula>AND($AA2 &lt;&gt; "core.endog",$AA2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z111">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed SPDW from nowcast calculation - causing collinearity issues, chol decomposition fails due to matrix singularity (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCBC7F7-0BA0-47A7-9D72-748BCEBB77C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91613AB-C584-492C-B03B-44B41D9A1181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8167,8 +8167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="X63" sqref="X63"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="AA100" sqref="AA100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13929,7 +13929,7 @@
         <v>282</v>
       </c>
       <c r="X99" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y99" s="11" t="s">
         <v>154</v>
@@ -13988,7 +13988,7 @@
         <v>16</v>
       </c>
       <c r="X100" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y100" s="11" t="s">
         <v>154</v>
@@ -14106,7 +14106,7 @@
         <v>16</v>
       </c>
       <c r="X102" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y102" s="11" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
Switched to Moore-Penrose inverse due to singularity issues (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91613AB-C584-492C-B03B-44B41D9A1181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE454ECC-96BD-4812-BC31-4E87FF1B1B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8167,8 +8167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="AA100" sqref="AA100"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="X88" sqref="X88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11191,7 +11191,7 @@
         <v>282</v>
       </c>
       <c r="X51" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y51" s="11" t="s">
         <v>154</v>
@@ -11247,7 +11247,7 @@
         <v>282</v>
       </c>
       <c r="X52" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y52" s="11" t="s">
         <v>154</v>
@@ -11357,7 +11357,7 @@
         <v>282</v>
       </c>
       <c r="X54" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y54" s="11" t="s">
         <v>154</v>
@@ -11675,7 +11675,7 @@
         <v>405</v>
       </c>
       <c r="M60" s="10" t="s">
-        <v>671</v>
+        <v>15</v>
       </c>
       <c r="N60" s="10" t="s">
         <v>16</v>
@@ -11687,7 +11687,7 @@
         <v>282</v>
       </c>
       <c r="X60" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y60" s="11" t="s">
         <v>154</v>
@@ -11956,7 +11956,7 @@
         <v>405</v>
       </c>
       <c r="M65" s="10" t="s">
-        <v>15</v>
+        <v>671</v>
       </c>
       <c r="N65" s="10" t="s">
         <v>16</v>
@@ -13213,7 +13213,7 @@
         <v>1</v>
       </c>
       <c r="X87" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y87" s="11" t="s">
         <v>154</v>
@@ -13929,7 +13929,7 @@
         <v>282</v>
       </c>
       <c r="X99" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y99" s="11" t="s">
         <v>154</v>
@@ -13988,7 +13988,7 @@
         <v>16</v>
       </c>
       <c r="X100" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y100" s="11" t="s">
         <v>154</v>
@@ -14047,7 +14047,7 @@
         <v>16</v>
       </c>
       <c r="X101" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y101" s="11" t="s">
         <v>154</v>
@@ -14607,7 +14607,7 @@
         <v>16</v>
       </c>
       <c r="X111" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y111" s="11" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
Added pred charts and some bug fixes for CSM forecasts (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE454ECC-96BD-4812-BC31-4E87FF1B1B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898E209-B5EB-43BE-B37E-207534974DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8167,8 +8167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="X88" sqref="X88"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="P109" sqref="P109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14481,7 +14481,7 @@
         <v>101</v>
       </c>
       <c r="P109" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="X109" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Added SQL inserts (v0.16)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CBE231-DA10-45CF-9A57-14E687FD72A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49825E1F-A3B0-4E01-84AC-10A250E4E240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -8167,8 +8167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="AA110" sqref="AA110"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14718,15 +14718,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624AEEDB-BBA7-44A6-A6FF-0B28C3344004}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" customWidth="1"/>
     <col min="6" max="6" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Added some SQL productionalization for model-sentiments (v0.17)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4127C9-BC4E-40BF-BD75-5D2D82605879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971DBD69-59DF-4187-9BEC-31B6B58D5AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="679">
   <si>
     <t>gdp</t>
   </si>
@@ -2086,6 +2086,9 @@
   </si>
   <si>
     <t>hpi20</t>
+  </si>
+  <si>
+    <t>Total Nonfarm Job Openings</t>
   </si>
 </sst>
 </file>
@@ -8185,8 +8188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AB112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11601,7 +11604,7 @@
         <v>326</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>327</v>
+        <v>678</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
Changed input dispgroups to remove spaces; needed to fix HTML parsing errors in CSS selectors for website (v0.17)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA78771F-19C4-4962-B58C-03B6B7030234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB33D3-5121-443D-841B-48582FA2F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="726">
   <si>
     <t>gdp</t>
   </si>
@@ -2064,12 +2064,6 @@
     <t>diff1</t>
   </si>
   <si>
-    <t>Stocks &amp; Commodities</t>
-  </si>
-  <si>
-    <t>Benchmark Rates</t>
-  </si>
-  <si>
     <t>Credit</t>
   </si>
   <si>
@@ -2097,12 +2091,6 @@
     <t>Currencies</t>
   </si>
   <si>
-    <t>Consumer Sales</t>
-  </si>
-  <si>
-    <t>Consumer Wealth</t>
-  </si>
-  <si>
     <t>advsalesmotor</t>
   </si>
   <si>
@@ -2227,6 +2215,21 @@
   </si>
   <si>
     <t>$millions</t>
+  </si>
+  <si>
+    <t>Labor_Market</t>
+  </si>
+  <si>
+    <t>Consumer_Sales</t>
+  </si>
+  <si>
+    <t>Stocks_and_Commodities</t>
+  </si>
+  <si>
+    <t>Benchmark_Rates</t>
+  </si>
+  <si>
+    <t>Consumer_Wealth</t>
   </si>
 </sst>
 </file>
@@ -2348,224 +2351,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="76">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3033,6 +2818,44 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3091,6 +2914,167 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3358,6 +3342,25 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3383,23 +3386,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="71"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="62"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3412,7 +3415,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="56"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3420,39 +3423,39 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="56"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="53"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="27"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="26"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="50"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="49"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="44"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="41"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="38"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="37"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="36"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="35"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="34"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="32"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="25"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3480,7 +3483,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -8078,17 +8081,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="75" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="74" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8366,8 +8369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G35" workbookViewId="0">
-      <selection activeCell="O69" sqref="O69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8408,10 +8411,10 @@
         <v>285</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>414</v>
@@ -10409,7 +10412,7 @@
         <v>57</v>
       </c>
       <c r="E31" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F31" s="10">
         <v>2</v>
@@ -11052,7 +11055,7 @@
         <v>162</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>156</v>
@@ -11106,7 +11109,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>156</v>
@@ -11160,7 +11163,7 @@
         <v>162</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>156</v>
@@ -11214,7 +11217,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>156</v>
@@ -11268,7 +11271,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>156</v>
@@ -11469,7 +11472,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>160</v>
@@ -11532,10 +11535,10 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>160</v>
@@ -11556,7 +11559,7 @@
         <v>156</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J50" s="10" t="s">
         <v>604</v>
@@ -11955,7 +11958,7 @@
         <v>162</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E57" s="10">
         <v>1</v>
@@ -12020,7 +12023,7 @@
         <v>252</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>252</v>
+        <v>721</v>
       </c>
       <c r="E58" s="10">
         <v>3</v>
@@ -12079,13 +12082,13 @@
         <v>326</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>252</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>252</v>
+        <v>721</v>
       </c>
       <c r="E59" s="10">
         <v>3</v>
@@ -12201,7 +12204,7 @@
         <v>238</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="E61" s="10">
         <v>1</v>
@@ -12266,7 +12269,7 @@
         <v>238</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E62" s="10">
         <v>2</v>
@@ -12334,7 +12337,7 @@
         <v>238</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E63" s="10">
         <v>1</v>
@@ -12402,7 +12405,7 @@
         <v>160</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E64" s="10">
         <v>2</v>
@@ -12521,7 +12524,7 @@
         <v>238</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E66" s="10">
         <v>1</v>
@@ -12637,7 +12640,7 @@
         <v>162</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E68" s="10">
         <v>1</v>
@@ -12652,13 +12655,13 @@
         <v>156</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>30</v>
@@ -12906,7 +12909,7 @@
         <v>238</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E73" s="10">
         <v>1</v>
@@ -12969,7 +12972,7 @@
         <v>238</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E74" s="10">
         <v>1</v>
@@ -13032,7 +13035,7 @@
         <v>238</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="E75" s="10">
         <v>1</v>
@@ -13401,7 +13404,7 @@
         <v>161</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E82" s="10">
         <v>1</v>
@@ -13476,7 +13479,7 @@
         <v>161</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E83" s="10">
         <v>1</v>
@@ -13548,7 +13551,7 @@
         <v>161</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E84" s="10">
         <v>1</v>
@@ -13623,7 +13626,7 @@
         <v>161</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E85" s="10">
         <v>1</v>
@@ -13692,7 +13695,7 @@
         <v>161</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E86" s="10">
         <v>1</v>
@@ -13761,7 +13764,7 @@
         <v>161</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E87" s="10">
         <v>2</v>
@@ -13830,7 +13833,7 @@
         <v>161</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E88" s="10">
         <v>1</v>
@@ -13902,7 +13905,7 @@
         <v>161</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E89" s="10">
         <v>2</v>
@@ -13971,7 +13974,7 @@
         <v>161</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E90" s="10">
         <v>2</v>
@@ -14043,7 +14046,7 @@
         <v>161</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E91" s="10">
         <v>2</v>
@@ -14112,7 +14115,7 @@
         <v>161</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E92" s="10">
         <v>1</v>
@@ -14181,7 +14184,7 @@
         <v>161</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E93" s="10">
         <v>2</v>
@@ -14250,7 +14253,7 @@
         <v>313</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E94" s="10">
         <v>1</v>
@@ -14319,7 +14322,7 @@
         <v>313</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>671</v>
+        <v>724</v>
       </c>
       <c r="E95" s="10">
         <v>1</v>
@@ -14564,7 +14567,7 @@
         <v>238</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="E99" s="10">
         <v>1</v>
@@ -14633,7 +14636,7 @@
         <v>238</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="E100" s="10">
         <v>2</v>
@@ -14701,7 +14704,7 @@
         <v>238</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="E101" s="10">
         <v>2</v>
@@ -14769,7 +14772,7 @@
         <v>238</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>670</v>
+        <v>723</v>
       </c>
       <c r="E102" s="10">
         <v>2</v>
@@ -15197,7 +15200,7 @@
         <v>162</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>682</v>
+        <v>725</v>
       </c>
       <c r="E110" s="10">
         <v>1</v>
@@ -15263,7 +15266,7 @@
         <v>252</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>252</v>
+        <v>721</v>
       </c>
       <c r="E111" s="10">
         <v>1</v>
@@ -15380,16 +15383,16 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E113" s="10">
         <v>2</v>
@@ -15404,13 +15407,13 @@
         <v>156</v>
       </c>
       <c r="I113" s="10" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="J113" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L113" s="10" t="s">
         <v>30</v>
@@ -15446,16 +15449,16 @@
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E114" s="10">
         <v>2</v>
@@ -15470,13 +15473,13 @@
         <v>156</v>
       </c>
       <c r="I114" s="10" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="J114" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L114" s="10" t="s">
         <v>30</v>
@@ -15512,16 +15515,16 @@
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="C115" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E115" s="10">
         <v>2</v>
@@ -15536,13 +15539,13 @@
         <v>156</v>
       </c>
       <c r="I115" s="10" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="J115" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K115" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L115" s="10" t="s">
         <v>30</v>
@@ -15578,16 +15581,16 @@
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C116" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E116" s="10">
         <v>2</v>
@@ -15602,13 +15605,13 @@
         <v>156</v>
       </c>
       <c r="I116" s="10" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="J116" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K116" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L116" s="10" t="s">
         <v>30</v>
@@ -15644,16 +15647,16 @@
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E117" s="10">
         <v>2</v>
@@ -15668,13 +15671,13 @@
         <v>156</v>
       </c>
       <c r="I117" s="10" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="J117" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L117" s="10" t="s">
         <v>30</v>
@@ -15710,16 +15713,16 @@
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E118" s="10">
         <v>2</v>
@@ -15734,13 +15737,13 @@
         <v>156</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="J118" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K118" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L118" s="10" t="s">
         <v>30</v>
@@ -15776,16 +15779,16 @@
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E119" s="10">
         <v>2</v>
@@ -15800,13 +15803,13 @@
         <v>156</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="J119" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K119" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L119" s="10" t="s">
         <v>30</v>
@@ -15842,16 +15845,16 @@
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E120" s="10">
         <v>2</v>
@@ -15866,13 +15869,13 @@
         <v>156</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="J120" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K120" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L120" s="10" t="s">
         <v>30</v>
@@ -15908,16 +15911,16 @@
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="C121" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E121" s="10">
         <v>2</v>
@@ -15932,13 +15935,13 @@
         <v>156</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="J121" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K121" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L121" s="10" t="s">
         <v>30</v>
@@ -15974,16 +15977,16 @@
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="B122" s="9" t="s">
         <v>692</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>696</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E122" s="10">
         <v>2</v>
@@ -15998,13 +16001,13 @@
         <v>156</v>
       </c>
       <c r="I122" s="10" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="J122" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K122" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L122" s="10" t="s">
         <v>30</v>
@@ -16040,16 +16043,16 @@
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E123" s="10">
         <v>2</v>
@@ -16064,13 +16067,13 @@
         <v>156</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="J123" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K123" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L123" s="10" t="s">
         <v>30</v>
@@ -16106,16 +16109,16 @@
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C124" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E124" s="10">
         <v>2</v>
@@ -16130,13 +16133,13 @@
         <v>156</v>
       </c>
       <c r="I124" s="10" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="J124" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K124" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L124" s="10" t="s">
         <v>30</v>
@@ -16172,16 +16175,16 @@
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="C125" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>681</v>
+        <v>722</v>
       </c>
       <c r="E125" s="10">
         <v>2</v>
@@ -16196,13 +16199,13 @@
         <v>156</v>
       </c>
       <c r="I125" s="10" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="J125" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="L125" s="10" t="s">
         <v>30</v>
@@ -16239,89 +16242,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="51" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="50" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="49" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="48" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="36" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Changed dispranks such that disprank = 1 variables will be displayed on charts on forecasts table for website (v0.17)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB33D3-5121-443D-841B-48582FA2F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A62B25-44E3-4B46-9877-7239D2FB1F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -8369,8 +8369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9961,7 +9961,7 @@
         <v>57</v>
       </c>
       <c r="E24" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="10">
         <v>2</v>
@@ -10473,7 +10473,7 @@
         <v>57</v>
       </c>
       <c r="E32" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" s="10">
         <v>2</v>
@@ -10668,7 +10668,7 @@
         <v>57</v>
       </c>
       <c r="E35" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" s="10">
         <v>2</v>
@@ -10863,7 +10863,7 @@
         <v>57</v>
       </c>
       <c r="E38" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" s="10">
         <v>2</v>
@@ -11613,7 +11613,7 @@
         <v>313</v>
       </c>
       <c r="E51" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F51" s="10">
         <v>1</v>
@@ -11961,7 +11961,7 @@
         <v>722</v>
       </c>
       <c r="E57" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" s="10">
         <v>1</v>
@@ -12207,7 +12207,7 @@
         <v>723</v>
       </c>
       <c r="E61" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F61" s="10">
         <v>1</v>
@@ -12340,7 +12340,7 @@
         <v>670</v>
       </c>
       <c r="E63" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="10">
         <v>1</v>

</xml_diff>

<commit_message>
Added consistency to unit naming for web display (v0.17)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A62B25-44E3-4B46-9877-7239D2FB1F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4996663F-6F1B-4D16-AB4F-CCE2C2206DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="730">
   <si>
     <t>gdp</t>
   </si>
@@ -2016,9 +2016,6 @@
     <t>TOTBKCR</t>
   </si>
   <si>
-    <t>$bn</t>
-  </si>
-  <si>
     <t>bankre</t>
   </si>
   <si>
@@ -2214,9 +2211,6 @@
     <t>RSAFS</t>
   </si>
   <si>
-    <t>$millions</t>
-  </si>
-  <si>
     <t>Labor_Market</t>
   </si>
   <si>
@@ -2230,6 +2224,24 @@
   </si>
   <si>
     <t>Consumer_Wealth</t>
+  </si>
+  <si>
+    <t>billions $</t>
+  </si>
+  <si>
+    <t>millions $</t>
+  </si>
+  <si>
+    <t>index (2012 = 100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billions of 2012 $ </t>
+  </si>
+  <si>
+    <t>$ per barrel</t>
+  </si>
+  <si>
+    <t>millions</t>
   </si>
 </sst>
 </file>
@@ -8369,8 +8381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B50CF-603C-40CA-9342-7B13AD6F1231}">
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8411,10 +8423,10 @@
         <v>285</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>414</v>
@@ -8444,7 +8456,7 @@
         <v>286</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>287</v>
@@ -8486,7 +8498,7 @@
         <v>534</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -8521,7 +8533,7 @@
         <v>537</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>18</v>
@@ -8567,7 +8579,7 @@
         <v>535</v>
       </c>
       <c r="AD2" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
@@ -8602,7 +8614,7 @@
         <v>537</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>18</v>
@@ -8636,7 +8648,7 @@
         <v>535</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
@@ -8671,7 +8683,7 @@
         <v>537</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>18</v>
@@ -8699,7 +8711,7 @@
         <v>535</v>
       </c>
       <c r="AD4" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
@@ -8734,7 +8746,7 @@
         <v>537</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>18</v>
@@ -8762,7 +8774,7 @@
         <v>535</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
@@ -8797,7 +8809,7 @@
         <v>537</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>18</v>
@@ -8825,10 +8837,10 @@
         <v>413</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD6" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -8863,7 +8875,7 @@
         <v>537</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>18</v>
@@ -8891,10 +8903,10 @@
         <v>413</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD7" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -8929,7 +8941,7 @@
         <v>537</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>18</v>
@@ -8957,10 +8969,10 @@
         <v>413</v>
       </c>
       <c r="AC8" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD8" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -8995,7 +9007,7 @@
         <v>537</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>18</v>
@@ -9023,10 +9035,10 @@
         <v>413</v>
       </c>
       <c r="AC9" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD9" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -9061,7 +9073,7 @@
         <v>537</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>18</v>
@@ -9089,7 +9101,7 @@
         <v>535</v>
       </c>
       <c r="AD10" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -9124,7 +9136,7 @@
         <v>537</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>18</v>
@@ -9152,10 +9164,10 @@
         <v>413</v>
       </c>
       <c r="AC11" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD11" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -9190,7 +9202,7 @@
         <v>537</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>18</v>
@@ -9218,10 +9230,10 @@
         <v>413</v>
       </c>
       <c r="AC12" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD12" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -9256,7 +9268,7 @@
         <v>537</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>18</v>
@@ -9284,10 +9296,10 @@
         <v>413</v>
       </c>
       <c r="AC13" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD13" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -9322,7 +9334,7 @@
         <v>537</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>18</v>
@@ -9350,10 +9362,10 @@
         <v>413</v>
       </c>
       <c r="AC14" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD14" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -9388,7 +9400,7 @@
         <v>537</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>18</v>
@@ -9416,7 +9428,7 @@
         <v>535</v>
       </c>
       <c r="AD15" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -9451,7 +9463,7 @@
         <v>537</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>18</v>
@@ -9479,10 +9491,10 @@
         <v>413</v>
       </c>
       <c r="AC16" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD16" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
@@ -9517,7 +9529,7 @@
         <v>537</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>18</v>
@@ -9545,10 +9557,10 @@
         <v>413</v>
       </c>
       <c r="AC17" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD17" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
@@ -9583,7 +9595,7 @@
         <v>537</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>18</v>
@@ -9611,10 +9623,10 @@
         <v>413</v>
       </c>
       <c r="AC18" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD18" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -9649,7 +9661,7 @@
         <v>537</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>18</v>
@@ -9677,10 +9689,10 @@
         <v>413</v>
       </c>
       <c r="AC19" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD19" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -9715,7 +9727,7 @@
         <v>537</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>18</v>
@@ -9743,10 +9755,10 @@
         <v>413</v>
       </c>
       <c r="AC20" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD20" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
@@ -9781,7 +9793,7 @@
         <v>537</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>18</v>
@@ -9809,10 +9821,10 @@
         <v>413</v>
       </c>
       <c r="AC21" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD21" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -9847,7 +9859,7 @@
         <v>537</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>18</v>
@@ -9875,10 +9887,10 @@
         <v>413</v>
       </c>
       <c r="AC22" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD22" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
@@ -9913,7 +9925,7 @@
         <v>537</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>18</v>
@@ -9941,10 +9953,10 @@
         <v>413</v>
       </c>
       <c r="AC23" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD23" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
@@ -9979,7 +9991,7 @@
         <v>537</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>18</v>
@@ -10007,7 +10019,7 @@
         <v>535</v>
       </c>
       <c r="AD24" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
@@ -10042,7 +10054,7 @@
         <v>537</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>18</v>
@@ -10070,7 +10082,7 @@
         <v>535</v>
       </c>
       <c r="AD25" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.25">
@@ -10105,7 +10117,7 @@
         <v>537</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L26" s="10" t="s">
         <v>18</v>
@@ -10133,10 +10145,10 @@
         <v>413</v>
       </c>
       <c r="AC26" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD26" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.25">
@@ -10171,7 +10183,7 @@
         <v>537</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>18</v>
@@ -10199,10 +10211,10 @@
         <v>413</v>
       </c>
       <c r="AC27" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD27" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
@@ -10237,7 +10249,7 @@
         <v>537</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>18</v>
@@ -10265,10 +10277,10 @@
         <v>413</v>
       </c>
       <c r="AC28" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD28" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -10303,7 +10315,7 @@
         <v>537</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>18</v>
@@ -10331,10 +10343,10 @@
         <v>413</v>
       </c>
       <c r="AC29" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD29" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
@@ -10369,7 +10381,7 @@
         <v>537</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>18</v>
@@ -10394,7 +10406,7 @@
         <v>153</v>
       </c>
       <c r="AC30" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AD30" s="11"/>
     </row>
@@ -10430,7 +10442,7 @@
         <v>537</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>18</v>
@@ -10455,7 +10467,7 @@
         <v>171</v>
       </c>
       <c r="AC31" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AD31" s="11"/>
     </row>
@@ -10491,7 +10503,7 @@
         <v>537</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>18</v>
@@ -10519,7 +10531,7 @@
         <v>535</v>
       </c>
       <c r="AD32" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.25">
@@ -10554,7 +10566,7 @@
         <v>537</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L33" s="10" t="s">
         <v>18</v>
@@ -10582,10 +10594,10 @@
         <v>413</v>
       </c>
       <c r="AC33" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD33" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
@@ -10620,7 +10632,7 @@
         <v>537</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L34" s="10" t="s">
         <v>18</v>
@@ -10648,10 +10660,10 @@
         <v>413</v>
       </c>
       <c r="AC34" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD34" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.25">
@@ -10686,7 +10698,7 @@
         <v>537</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L35" s="10" t="s">
         <v>18</v>
@@ -10714,7 +10726,7 @@
         <v>535</v>
       </c>
       <c r="AD35" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
@@ -10749,7 +10761,7 @@
         <v>537</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L36" s="10" t="s">
         <v>18</v>
@@ -10777,10 +10789,10 @@
         <v>413</v>
       </c>
       <c r="AC36" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD36" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
@@ -10815,7 +10827,7 @@
         <v>537</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L37" s="10" t="s">
         <v>18</v>
@@ -10843,10 +10855,10 @@
         <v>413</v>
       </c>
       <c r="AC37" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD37" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.25">
@@ -10881,7 +10893,7 @@
         <v>537</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>18</v>
@@ -10909,7 +10921,7 @@
         <v>535</v>
       </c>
       <c r="AD38" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.25">
@@ -10944,7 +10956,7 @@
         <v>537</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>18</v>
@@ -10972,10 +10984,10 @@
         <v>413</v>
       </c>
       <c r="AC39" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD39" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.25">
@@ -11010,7 +11022,7 @@
         <v>537</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>18</v>
@@ -11038,10 +11050,10 @@
         <v>413</v>
       </c>
       <c r="AC40" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AD40" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
@@ -11055,7 +11067,7 @@
         <v>162</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>156</v>
@@ -11067,7 +11079,7 @@
         <v>632</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>30</v>
@@ -11109,7 +11121,7 @@
         <v>162</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>156</v>
@@ -11121,7 +11133,7 @@
         <v>632</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>30</v>
@@ -11163,7 +11175,7 @@
         <v>162</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>156</v>
@@ -11175,7 +11187,7 @@
         <v>632</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>30</v>
@@ -11217,7 +11229,7 @@
         <v>162</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>156</v>
@@ -11229,7 +11241,7 @@
         <v>632</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>30</v>
@@ -11271,7 +11283,7 @@
         <v>162</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>156</v>
@@ -11283,7 +11295,7 @@
         <v>632</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>30</v>
@@ -11334,7 +11346,7 @@
         <v>632</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>30</v>
@@ -11385,7 +11397,7 @@
         <v>632</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>30</v>
@@ -11436,7 +11448,7 @@
         <v>632</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>30</v>
@@ -11472,7 +11484,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>160</v>
@@ -11535,10 +11547,10 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>160</v>
@@ -11559,7 +11571,7 @@
         <v>156</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J50" s="10" t="s">
         <v>604</v>
@@ -11596,7 +11608,7 @@
         <v>535</v>
       </c>
       <c r="AD50" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
@@ -11631,7 +11643,7 @@
         <v>610</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>30</v>
@@ -11661,7 +11673,7 @@
         <v>535</v>
       </c>
       <c r="AD51" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
@@ -11726,7 +11738,7 @@
         <v>535</v>
       </c>
       <c r="AD52" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
@@ -11791,7 +11803,7 @@
         <v>535</v>
       </c>
       <c r="AD53" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
@@ -11814,7 +11826,7 @@
         <v>626</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>310</v>
+        <v>725</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>30</v>
@@ -11916,7 +11928,7 @@
         <v>609</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>310</v>
+        <v>725</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>30</v>
@@ -11958,7 +11970,7 @@
         <v>162</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E57" s="10">
         <v>2</v>
@@ -11979,7 +11991,7 @@
         <v>612</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>196</v>
+        <v>729</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>30</v>
@@ -12009,7 +12021,7 @@
         <v>535</v>
       </c>
       <c r="AD57" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.25">
@@ -12023,7 +12035,7 @@
         <v>252</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E58" s="10">
         <v>3</v>
@@ -12044,7 +12056,7 @@
         <v>613</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>30</v>
@@ -12074,7 +12086,7 @@
         <v>535</v>
       </c>
       <c r="AD58" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.25">
@@ -12082,13 +12094,13 @@
         <v>326</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>252</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E59" s="10">
         <v>3</v>
@@ -12139,7 +12151,7 @@
         <v>535</v>
       </c>
       <c r="AD59" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
@@ -12204,7 +12216,7 @@
         <v>238</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E61" s="10">
         <v>2</v>
@@ -12225,7 +12237,7 @@
         <v>627</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>332</v>
+        <v>728</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>30</v>
@@ -12255,21 +12267,21 @@
         <v>535</v>
       </c>
       <c r="AD61" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>659</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>660</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>238</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E62" s="10">
         <v>2</v>
@@ -12284,13 +12296,13 @@
         <v>156</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J62" s="10" t="s">
         <v>606</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>284</v>
+        <v>724</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>388</v>
@@ -12323,21 +12335,21 @@
         <v>535</v>
       </c>
       <c r="AD62" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>656</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>657</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>238</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E63" s="10">
         <v>2</v>
@@ -12352,13 +12364,13 @@
         <v>156</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J63" s="10" t="s">
         <v>606</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>284</v>
+        <v>724</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>388</v>
@@ -12391,21 +12403,21 @@
         <v>535</v>
       </c>
       <c r="AD63" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>160</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E64" s="10">
         <v>2</v>
@@ -12426,7 +12438,7 @@
         <v>606</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>284</v>
+        <v>724</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>388</v>
@@ -12459,7 +12471,7 @@
         <v>535</v>
       </c>
       <c r="AD64" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="65" spans="1:30" x14ac:dyDescent="0.25">
@@ -12524,7 +12536,7 @@
         <v>238</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E66" s="10">
         <v>1</v>
@@ -12554,7 +12566,7 @@
         <v>405</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P66" s="10" t="s">
         <v>16</v>
@@ -12575,7 +12587,7 @@
         <v>535</v>
       </c>
       <c r="AD66" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.25">
@@ -12607,7 +12619,7 @@
         <v>405</v>
       </c>
       <c r="O67" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P67" s="10" t="s">
         <v>16</v>
@@ -12640,7 +12652,7 @@
         <v>162</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E68" s="10">
         <v>1</v>
@@ -12655,13 +12667,13 @@
         <v>156</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>30</v>
@@ -12691,7 +12703,7 @@
         <v>535</v>
       </c>
       <c r="AD68" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="69" spans="1:30" x14ac:dyDescent="0.25">
@@ -12765,7 +12777,7 @@
         <v>625</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>30</v>
@@ -12867,7 +12879,7 @@
         <v>632</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>99</v>
+        <v>726</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>30</v>
@@ -12909,7 +12921,7 @@
         <v>238</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E73" s="10">
         <v>1</v>
@@ -12958,7 +12970,7 @@
         <v>535</v>
       </c>
       <c r="AD73" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="74" spans="1:30" x14ac:dyDescent="0.25">
@@ -12972,7 +12984,7 @@
         <v>238</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E74" s="10">
         <v>1</v>
@@ -13021,7 +13033,7 @@
         <v>535</v>
       </c>
       <c r="AD74" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="75" spans="1:30" x14ac:dyDescent="0.25">
@@ -13035,7 +13047,7 @@
         <v>238</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E75" s="10">
         <v>1</v>
@@ -13084,7 +13096,7 @@
         <v>535</v>
       </c>
       <c r="AD75" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="76" spans="1:30" x14ac:dyDescent="0.25">
@@ -13404,7 +13416,7 @@
         <v>161</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E82" s="10">
         <v>1</v>
@@ -13437,7 +13449,7 @@
         <v>406</v>
       </c>
       <c r="O82" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P82" s="10" t="s">
         <v>16</v>
@@ -13479,7 +13491,7 @@
         <v>161</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E83" s="10">
         <v>1</v>
@@ -13512,7 +13524,7 @@
         <v>406</v>
       </c>
       <c r="O83" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P83" s="10" t="s">
         <v>16</v>
@@ -13551,7 +13563,7 @@
         <v>161</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E84" s="10">
         <v>1</v>
@@ -13584,7 +13596,7 @@
         <v>406</v>
       </c>
       <c r="O84" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P84" s="10" t="s">
         <v>16</v>
@@ -13626,7 +13638,7 @@
         <v>161</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E85" s="10">
         <v>1</v>
@@ -13659,7 +13671,7 @@
         <v>406</v>
       </c>
       <c r="O85" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P85" s="10" t="s">
         <v>16</v>
@@ -13695,7 +13707,7 @@
         <v>161</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E86" s="10">
         <v>1</v>
@@ -13728,7 +13740,7 @@
         <v>406</v>
       </c>
       <c r="O86" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P86" s="10" t="s">
         <v>16</v>
@@ -13764,7 +13776,7 @@
         <v>161</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E87" s="10">
         <v>2</v>
@@ -13797,7 +13809,7 @@
         <v>406</v>
       </c>
       <c r="O87" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P87" s="10" t="s">
         <v>16</v>
@@ -13833,7 +13845,7 @@
         <v>161</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E88" s="10">
         <v>1</v>
@@ -13866,7 +13878,7 @@
         <v>406</v>
       </c>
       <c r="O88" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P88" s="10" t="s">
         <v>16</v>
@@ -13905,7 +13917,7 @@
         <v>161</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E89" s="10">
         <v>2</v>
@@ -13938,7 +13950,7 @@
         <v>406</v>
       </c>
       <c r="O89" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P89" s="10" t="s">
         <v>16</v>
@@ -13974,7 +13986,7 @@
         <v>161</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E90" s="10">
         <v>2</v>
@@ -14007,7 +14019,7 @@
         <v>406</v>
       </c>
       <c r="O90" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P90" s="10" t="s">
         <v>16</v>
@@ -14046,7 +14058,7 @@
         <v>161</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E91" s="10">
         <v>2</v>
@@ -14079,7 +14091,7 @@
         <v>406</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P91" s="10" t="s">
         <v>16</v>
@@ -14115,7 +14127,7 @@
         <v>161</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E92" s="10">
         <v>1</v>
@@ -14148,7 +14160,7 @@
         <v>406</v>
       </c>
       <c r="O92" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P92" s="10" t="s">
         <v>16</v>
@@ -14184,7 +14196,7 @@
         <v>161</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E93" s="10">
         <v>2</v>
@@ -14217,7 +14229,7 @@
         <v>406</v>
       </c>
       <c r="O93" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P93" s="10" t="s">
         <v>16</v>
@@ -14253,7 +14265,7 @@
         <v>313</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E94" s="10">
         <v>1</v>
@@ -14286,7 +14298,7 @@
         <v>406</v>
       </c>
       <c r="O94" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P94" s="10" t="s">
         <v>16</v>
@@ -14322,7 +14334,7 @@
         <v>313</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E95" s="10">
         <v>1</v>
@@ -14355,7 +14367,7 @@
         <v>406</v>
       </c>
       <c r="O95" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P95" s="10" t="s">
         <v>16</v>
@@ -14412,7 +14424,7 @@
         <v>406</v>
       </c>
       <c r="O96" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P96" s="10" t="s">
         <v>16</v>
@@ -14433,7 +14445,7 @@
         <v>535</v>
       </c>
       <c r="AD96" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="97" spans="1:30" x14ac:dyDescent="0.25">
@@ -14486,7 +14498,7 @@
         <v>154</v>
       </c>
       <c r="AC97" s="11" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AD97" s="11"/>
     </row>
@@ -14567,7 +14579,7 @@
         <v>238</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E99" s="10">
         <v>1</v>
@@ -14636,7 +14648,7 @@
         <v>238</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E100" s="10">
         <v>2</v>
@@ -14690,7 +14702,7 @@
         <v>535</v>
       </c>
       <c r="AD100" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="101" spans="1:30" x14ac:dyDescent="0.25">
@@ -14704,7 +14716,7 @@
         <v>238</v>
       </c>
       <c r="D101" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E101" s="10">
         <v>2</v>
@@ -14758,7 +14770,7 @@
         <v>535</v>
       </c>
       <c r="AD101" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="102" spans="1:30" x14ac:dyDescent="0.25">
@@ -14772,7 +14784,7 @@
         <v>238</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E102" s="10">
         <v>2</v>
@@ -14826,7 +14838,7 @@
         <v>535</v>
       </c>
       <c r="AD102" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="103" spans="1:30" x14ac:dyDescent="0.25">
@@ -14909,7 +14921,7 @@
         <v>406</v>
       </c>
       <c r="O104" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P104" s="10" t="s">
         <v>16</v>
@@ -14960,7 +14972,7 @@
         <v>406</v>
       </c>
       <c r="O105" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P105" s="10" t="s">
         <v>16</v>
@@ -15011,7 +15023,7 @@
         <v>406</v>
       </c>
       <c r="O106" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P106" s="10" t="s">
         <v>16</v>
@@ -15062,7 +15074,7 @@
         <v>406</v>
       </c>
       <c r="O107" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P107" s="10" t="s">
         <v>16</v>
@@ -15113,7 +15125,7 @@
         <v>406</v>
       </c>
       <c r="O108" s="10" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P108" s="10" t="s">
         <v>16</v>
@@ -15158,7 +15170,7 @@
         <v>632</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>30</v>
@@ -15200,7 +15212,7 @@
         <v>162</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E110" s="10">
         <v>1</v>
@@ -15221,7 +15233,7 @@
         <v>632</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>283</v>
+        <v>727</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>30</v>
@@ -15266,7 +15278,7 @@
         <v>252</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E111" s="10">
         <v>1</v>
@@ -15347,7 +15359,7 @@
         <v>606</v>
       </c>
       <c r="K112" s="10" t="s">
-        <v>654</v>
+        <v>724</v>
       </c>
       <c r="L112" s="10" t="s">
         <v>388</v>
@@ -15383,16 +15395,16 @@
     </row>
     <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E113" s="10">
         <v>2</v>
@@ -15407,13 +15419,13 @@
         <v>156</v>
       </c>
       <c r="I113" s="10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="J113" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K113" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L113" s="10" t="s">
         <v>30</v>
@@ -15444,21 +15456,21 @@
         <v>535</v>
       </c>
       <c r="AD113" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D114" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E114" s="10">
         <v>2</v>
@@ -15473,13 +15485,13 @@
         <v>156</v>
       </c>
       <c r="I114" s="10" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="J114" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K114" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L114" s="10" t="s">
         <v>30</v>
@@ -15510,21 +15522,21 @@
         <v>535</v>
       </c>
       <c r="AD114" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C115" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D115" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E115" s="10">
         <v>2</v>
@@ -15539,13 +15551,13 @@
         <v>156</v>
       </c>
       <c r="I115" s="10" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J115" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K115" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L115" s="10" t="s">
         <v>30</v>
@@ -15576,21 +15588,21 @@
         <v>535</v>
       </c>
       <c r="AD115" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C116" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E116" s="10">
         <v>2</v>
@@ -15605,13 +15617,13 @@
         <v>156</v>
       </c>
       <c r="I116" s="10" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="J116" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K116" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L116" s="10" t="s">
         <v>30</v>
@@ -15642,21 +15654,21 @@
         <v>535</v>
       </c>
       <c r="AD116" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D117" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E117" s="10">
         <v>2</v>
@@ -15671,13 +15683,13 @@
         <v>156</v>
       </c>
       <c r="I117" s="10" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J117" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K117" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L117" s="10" t="s">
         <v>30</v>
@@ -15708,21 +15720,21 @@
         <v>535</v>
       </c>
       <c r="AD117" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D118" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E118" s="10">
         <v>2</v>
@@ -15737,13 +15749,13 @@
         <v>156</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J118" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K118" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L118" s="10" t="s">
         <v>30</v>
@@ -15774,21 +15786,21 @@
         <v>535</v>
       </c>
       <c r="AD118" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D119" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E119" s="10">
         <v>2</v>
@@ -15803,13 +15815,13 @@
         <v>156</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J119" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K119" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L119" s="10" t="s">
         <v>30</v>
@@ -15840,21 +15852,21 @@
         <v>535</v>
       </c>
       <c r="AD119" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D120" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E120" s="10">
         <v>2</v>
@@ -15869,13 +15881,13 @@
         <v>156</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J120" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K120" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L120" s="10" t="s">
         <v>30</v>
@@ -15906,21 +15918,21 @@
         <v>535</v>
       </c>
       <c r="AD120" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="121" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C121" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D121" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E121" s="10">
         <v>2</v>
@@ -15935,13 +15947,13 @@
         <v>156</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="J121" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K121" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L121" s="10" t="s">
         <v>30</v>
@@ -15972,21 +15984,21 @@
         <v>535</v>
       </c>
       <c r="AD121" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D122" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E122" s="10">
         <v>2</v>
@@ -16001,13 +16013,13 @@
         <v>156</v>
       </c>
       <c r="I122" s="10" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J122" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K122" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L122" s="10" t="s">
         <v>30</v>
@@ -16038,21 +16050,21 @@
         <v>535</v>
       </c>
       <c r="AD122" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="B123" s="9" t="s">
         <v>714</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>715</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D123" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E123" s="10">
         <v>2</v>
@@ -16067,13 +16079,13 @@
         <v>156</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J123" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K123" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L123" s="10" t="s">
         <v>30</v>
@@ -16104,21 +16116,21 @@
         <v>535</v>
       </c>
       <c r="AD123" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="124" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C124" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D124" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E124" s="10">
         <v>2</v>
@@ -16133,13 +16145,13 @@
         <v>156</v>
       </c>
       <c r="I124" s="10" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J124" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K124" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L124" s="10" t="s">
         <v>30</v>
@@ -16170,21 +16182,21 @@
         <v>535</v>
       </c>
       <c r="AD124" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="125" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C125" s="10" t="s">
         <v>162</v>
       </c>
       <c r="D125" s="10" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E125" s="10">
         <v>2</v>
@@ -16199,13 +16211,13 @@
         <v>156</v>
       </c>
       <c r="I125" s="10" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J125" s="10" t="s">
         <v>630</v>
       </c>
       <c r="K125" s="10" t="s">
-        <v>720</v>
+        <v>725</v>
       </c>
       <c r="L125" s="10" t="s">
         <v>30</v>
@@ -16236,7 +16248,7 @@
         <v>535</v>
       </c>
       <c r="AD125" s="11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DB structure diagram (v0.18)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF94A9-EEE6-4BA8-B770-E4BF0E3DE6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E5A8C5-2243-4B5E-A9D0-1D49F0AEC206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6350" uniqueCount="735">
   <si>
     <t>gdp</t>
   </si>
@@ -2244,6 +2244,21 @@
   </si>
   <si>
     <t>millions</t>
+  </si>
+  <si>
+    <t>btc</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
+  </si>
+  <si>
+    <t>CBBTCUSD</t>
+  </si>
+  <si>
+    <t>COIN.CRYPT</t>
+  </si>
+  <si>
+    <t>$</t>
   </si>
 </sst>
 </file>
@@ -2364,7 +2379,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="153">
     <dxf>
       <fill>
         <patternFill>
@@ -2494,13 +2509,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -2525,747 +2533,6 @@
           <bgColor rgb="FFFF7D7D"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3832,6 +3099,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4097,6 +3525,747 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4122,39 +4291,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD124" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
-  <autoFilter ref="A1:AD124" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+  <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="77"/>
-    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="76"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="75"/>
-    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="74"/>
-    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="73"/>
-    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="70"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="69"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="61"/>
-    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="60"/>
-    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="59"/>
-    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="58"/>
-    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="57"/>
-    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="56"/>
-    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="55"/>
-    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="53"/>
-    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="52"/>
-    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="50"/>
-    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="127"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="125"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="124"/>
+    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="123"/>
+    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="122"/>
+    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="119"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="118"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="115"/>
+    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="113"/>
+    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="112"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="110"/>
+    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="109"/>
+    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="108"/>
+    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="107"/>
+    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="106"/>
+    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="105"/>
+    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="104"/>
+    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="103"/>
+    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="102"/>
+    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="101"/>
+    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="99"/>
+    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4176,23 +4345,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="128"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="126"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="125"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="123"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="121"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="120"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="119"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="118"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="117"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="115"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="92"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="90"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="87"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="83"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="82"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4205,7 +4374,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="78"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4213,39 +4382,39 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="111"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="110"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="109"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="108"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="107"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="106"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="104"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="103"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="102"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="101"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="99"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="97"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="96"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="95"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="94"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="93"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="92"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="91"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="90"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="89"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="88"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="87"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="86"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="85"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="50"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="49"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="48"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="47"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="35"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="34"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="33"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="30"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="29"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="26"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="24"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4273,7 +4442,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="22"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4580,10 +4749,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:AD124"/>
+  <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="C104" workbookViewId="0">
+      <selection activeCell="Z126" sqref="Z126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8390,7 +8559,7 @@
         <v>728</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
       </c>
       <c r="N60" s="10" t="s">
         <v>405</v>
@@ -8647,7 +8816,10 @@
         <v>94</v>
       </c>
       <c r="L64" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="M64" s="10">
+        <v>1</v>
       </c>
       <c r="N64" s="10" t="s">
         <v>405</v>
@@ -9476,7 +9648,10 @@
         <v>89</v>
       </c>
       <c r="L79" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="M79" s="10">
+        <v>1</v>
       </c>
       <c r="N79" s="10" t="s">
         <v>405</v>
@@ -12401,91 +12576,148 @@
         <v>665</v>
       </c>
     </row>
+    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A125" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>731</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H125" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I125" s="10" t="s">
+        <v>732</v>
+      </c>
+      <c r="J125" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="K125" s="10" t="s">
+        <v>734</v>
+      </c>
+      <c r="L125" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="M125" s="10">
+        <v>1</v>
+      </c>
+      <c r="N125" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="O125" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="P125" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q125" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R125" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="Z125" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA125" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB125" s="11"/>
+      <c r="AC125" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="AD125" s="11" t="s">
+        <v>665</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:M124">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
+  <conditionalFormatting sqref="L1:M125">
+    <cfRule type="cellIs" dxfId="152" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z111:Z10020">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="148" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I124">
-    <cfRule type="expression" dxfId="43" priority="17">
+  <conditionalFormatting sqref="I2:I125">
+    <cfRule type="expression" dxfId="147" priority="17">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M124">
-    <cfRule type="expression" dxfId="42" priority="23">
+  <conditionalFormatting sqref="M2:M125">
+    <cfRule type="expression" dxfId="146" priority="23">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:Z124">
-    <cfRule type="expression" dxfId="41" priority="16">
+  <conditionalFormatting sqref="Z2:Z125">
+    <cfRule type="expression" dxfId="145" priority="16">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC124">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+  <conditionalFormatting sqref="AC2:AC125">
+    <cfRule type="cellIs" dxfId="144" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA2:AA124">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+  <conditionalFormatting sqref="AA2:AA125">
+    <cfRule type="cellIs" dxfId="139" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD2:AD124">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+  <conditionalFormatting sqref="AD2:AD125">
+    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="133" priority="8">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB2:AB124">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+  <conditionalFormatting sqref="AB2:AB125">
+    <cfRule type="cellIs" dxfId="132" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12504,8 +12736,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17378,17 +17610,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="97" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="96" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25539,89 +25771,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="73" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="72" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="71" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="70" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="58" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added historical data import fixes and release data (v0.18)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E5A8C5-2243-4B5E-A9D0-1D49F0AEC206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1DF4C5-ACFD-4B82-9DFB-CDB6E2274A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6350" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6354" uniqueCount="737">
   <si>
     <t>gdp</t>
   </si>
@@ -2259,6 +2259,12 @@
   </si>
   <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>Coinbase CryptoCurrency</t>
+  </si>
+  <si>
+    <t>https://coinbase.com</t>
   </si>
 </sst>
 </file>
@@ -2379,161 +2385,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="153">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="131">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4291,39 +4143,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="127"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="126"/>
-    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="125"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="124"/>
-    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="123"/>
-    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="122"/>
-    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="119"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="118"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="115"/>
-    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="114"/>
-    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="113"/>
-    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="112"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="111"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="110"/>
-    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="109"/>
-    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="108"/>
-    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="107"/>
-    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="106"/>
-    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="105"/>
-    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="104"/>
-    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="103"/>
-    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="102"/>
-    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="101"/>
-    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="99"/>
-    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="105"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="104"/>
+    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="103"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="102"/>
+    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="101"/>
+    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="100"/>
+    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="97"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="96"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="91"/>
+    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="90"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="88"/>
+    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="87"/>
+    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="86"/>
+    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="85"/>
+    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="84"/>
+    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="83"/>
+    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="82"/>
+    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="79"/>
+    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4345,23 +4197,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="90"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="87"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="83"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="82"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4374,7 +4226,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="56"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4382,39 +4234,39 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="50"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="49"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="48"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="47"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="38"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="35"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="34"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="33"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="31"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="30"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="29"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="28"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="26"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="24"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="25"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4442,7 +4294,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4751,8 +4603,8 @@
   </sheetPr>
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C104" workbookViewId="0">
-      <selection activeCell="Z126" sqref="Z126"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="N126" sqref="N126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12635,89 +12487,89 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="152" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z111:Z10020">
-    <cfRule type="expression" dxfId="148" priority="18">
+    <cfRule type="expression" dxfId="126" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="147" priority="17">
+    <cfRule type="expression" dxfId="125" priority="17">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="146" priority="23">
+    <cfRule type="expression" dxfId="124" priority="23">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="145" priority="16">
+    <cfRule type="expression" dxfId="123" priority="16">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="144" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="139" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="135" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="8">
+    <cfRule type="expression" dxfId="111" priority="8">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="132" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12734,10 +12586,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13303,6 +13155,23 @@
       </c>
       <c r="D32" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>733</v>
+      </c>
+      <c r="B33" t="s">
+        <v>735</v>
+      </c>
+      <c r="C33" t="s">
+        <v>736</v>
+      </c>
+      <c r="D33" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -17610,17 +17479,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="97" priority="3">
+    <cfRule type="expression" dxfId="75" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="96" priority="2">
+    <cfRule type="expression" dxfId="74" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="95" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25771,89 +25640,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="77" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="73" priority="22">
+    <cfRule type="expression" dxfId="51" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="72" priority="21">
+    <cfRule type="expression" dxfId="50" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="71" priority="31">
+    <cfRule type="expression" dxfId="49" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="70" priority="17">
+    <cfRule type="expression" dxfId="48" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="64" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="9">
+    <cfRule type="expression" dxfId="36" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed data pulls (v0.18)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1DF4C5-ACFD-4B82-9DFB-CDB6E2274A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE42B4-0B71-4DDE-891B-2D11CB45E2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -12589,7 +12589,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated workflow and added DNS history values (v0.19)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307FA46-EF46-4262-BF3E-D957FBB35EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4B090A-8301-4766-94BF-2E0D42B1C6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="10" r:id="rId1"/>
@@ -2385,3428 +2385,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="571">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="131">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -6372,6 +2951,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6636,6 +3376,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7198,6 +3957,167 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7223,39 +4143,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="570" dataDxfId="569">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="568"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="567"/>
-    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="566"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="565"/>
-    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="564"/>
-    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="563"/>
-    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="562"/>
-    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="561"/>
-    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="560"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="559"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="558"/>
-    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="557"/>
-    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="556"/>
-    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="555"/>
-    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="554"/>
-    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="553"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="552"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="551"/>
-    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="550"/>
-    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="549"/>
-    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="548"/>
-    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="547"/>
-    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="546"/>
-    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="545"/>
-    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="544"/>
-    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="543"/>
-    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="542"/>
-    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="541"/>
-    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="540"/>
-    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="539"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="105"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="104"/>
+    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="103"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="102"/>
+    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="101"/>
+    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="100"/>
+    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="97"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="96"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="94"/>
+    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="91"/>
+    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="90"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="88"/>
+    <tableColumn id="20" xr3:uid="{BD9C003A-D74B-48E7-BFF6-EA60EEE6DB32}" name="ext_atl" dataDxfId="87"/>
+    <tableColumn id="21" xr3:uid="{4C8A45F1-F7C8-4B06-B2A5-D1374D172CEC}" name="ext_stl" dataDxfId="86"/>
+    <tableColumn id="22" xr3:uid="{3D074362-A1C7-4C20-9399-33B81AEFC5D3}" name="ext_nyf" dataDxfId="85"/>
+    <tableColumn id="23" xr3:uid="{98E4C166-4FD1-4121-9260-23A9A05F68C3}" name="ext_spf" dataDxfId="84"/>
+    <tableColumn id="26" xr3:uid="{B8BAA3DB-A9E6-4025-9EFA-A02508AD057F}" name="ext_wsj" dataDxfId="83"/>
+    <tableColumn id="27" xr3:uid="{ECEF868A-1F7A-48D6-A85C-BDB45DA4078E}" name="ext_cbo" dataDxfId="82"/>
+    <tableColumn id="28" xr3:uid="{653B0BB4-5F3E-4BF1-8BFD-C3BEF81611E4}" name="ext_mkt" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="79"/>
+    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7277,23 +4197,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="538" dataDxfId="537">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="536"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="535"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="534"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="533"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="532"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="531"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="530"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="529"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="528"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="527"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="526"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="525"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="524"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="523"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="69"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="68"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7306,7 +4226,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="522"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="56"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7314,39 +4234,39 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="521" dataDxfId="520">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="519"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="518"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="517"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="516"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="515"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="514"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="513"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="512"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="511"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="510"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="509"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="508"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="507"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="506"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="505"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="504"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="503"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="502"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="501"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="500"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="499"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="498"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="497"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="496"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="495"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="494"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="493"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="492"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="491"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="490"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="26"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="25"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="22"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="7"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7374,7 +4294,7 @@
     <tableColumn id="1" xr3:uid="{DE80604F-79B1-4324-817D-137A434345B1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{DD3F53BB-B835-4706-A86C-47DF4CCEB32C}" name="freq"/>
     <tableColumn id="3" xr3:uid="{79BD2DFD-DD4C-4E37-948A-F6F662388AB7}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="489"/>
+    <tableColumn id="4" xr3:uid="{747FA420-CE38-4715-8BA1-284F15A995E9}" name="market" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{E889BE1D-727B-4E74-8F79-F0DCBF6D400F}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7683,8 +4603,8 @@
   </sheetPr>
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15567,89 +12487,89 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z111:Z10000">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="126" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="43" priority="17">
+    <cfRule type="expression" dxfId="125" priority="17">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="42" priority="23">
+    <cfRule type="expression" dxfId="124" priority="23">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="41" priority="16">
+    <cfRule type="expression" dxfId="123" priority="16">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="111" priority="8">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20559,17 +17479,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="75" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="74" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28720,89 +25640,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="51" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="50" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="49" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="48" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="36" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Critical bugfix of nowcast model returning wrong dates for quarterly forecast (v0.20)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58C2CB4-106C-4E10-A31B-3BA4F0945851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A722DB-2531-4589-9928-67DF2267D8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="gdp-model-inputs" sheetId="12" r:id="rId1"/>
@@ -2450,501 +2450,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="167">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3507,6 +3012,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3771,6 +3437,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4201,6 +3886,167 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -4571,6 +4417,160 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4596,61 +4596,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:T108" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:T108" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
   <autoFilter ref="A1:T108" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="164"/>
-    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="163"/>
-    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="162"/>
-    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="161"/>
-    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="160"/>
-    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="159"/>
-    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="157"/>
-    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="156"/>
-    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="155"/>
-    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="154"/>
-    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="152"/>
-    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="151"/>
-    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="150"/>
-    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="149"/>
-    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="148"/>
-    <tableColumn id="29" xr3:uid="{76399FAE-BA60-4EB8-A76D-B35AF5C448A3}" name="initial_forecast" dataDxfId="147"/>
-    <tableColumn id="8" xr3:uid="{8D11F2D0-2DDA-4833-97A3-0AE2613B5941}" name="core_structural" dataDxfId="146"/>
-    <tableColumn id="18" xr3:uid="{5C5BF075-E0AE-47B3-8E6C-DA1E78BAA23F}" name="core_endog_type" dataDxfId="145"/>
+    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="142"/>
+    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="141"/>
+    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="140"/>
+    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="139"/>
+    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="138"/>
+    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="137"/>
+    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="135"/>
+    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="134"/>
+    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="132"/>
+    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="131"/>
+    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="130"/>
+    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="129"/>
+    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="128"/>
+    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="127"/>
+    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="126"/>
+    <tableColumn id="29" xr3:uid="{76399FAE-BA60-4EB8-A76D-B35AF5C448A3}" name="initial_forecast" dataDxfId="125"/>
+    <tableColumn id="8" xr3:uid="{8D11F2D0-2DDA-4833-97A3-0AE2613B5941}" name="core_structural" dataDxfId="124"/>
+    <tableColumn id="18" xr3:uid="{5C5BF075-E0AE-47B3-8E6C-DA1E78BAA23F}" name="core_endog_type" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:W125" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:W125" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="A1:W125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="142"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="141"/>
-    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="140"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="139"/>
-    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="138"/>
-    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="137"/>
-    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="134"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="133"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="132"/>
-    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="130"/>
-    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="129"/>
-    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="128"/>
-    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="127"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="126"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="125"/>
-    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="124"/>
-    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="123"/>
-    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="122"/>
-    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="121"/>
-    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="97"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="96"/>
+    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="95"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="94"/>
+    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="93"/>
+    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="92"/>
+    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="91"/>
+    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="89"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="84"/>
+    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="83"/>
+    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="81"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="80"/>
+    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="79"/>
+    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="78"/>
+    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="77"/>
+    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="76"/>
+    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4672,23 +4672,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="117"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="112"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="110"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="108"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="107"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="106"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="105"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="67"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="64"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4701,7 +4701,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="55"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4709,39 +4709,39 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="100"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="98"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="97"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="96"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="95"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="92"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="91"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="88"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="85"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="83"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="82"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="81"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="80"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="79"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="78"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="77"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="76"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="75"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="74"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="72"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="26"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="24"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="15"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5049,8 +5049,8 @@
   </sheetPr>
   <dimension ref="A1:W108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11307,84 +11307,84 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K108">
-    <cfRule type="cellIs" dxfId="70" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S109:S9983 P108">
-    <cfRule type="expression" dxfId="66" priority="18">
+    <cfRule type="expression" dxfId="162" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H108">
-    <cfRule type="expression" dxfId="65" priority="17">
+    <cfRule type="expression" dxfId="161" priority="17">
       <formula>$G2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P108">
-    <cfRule type="expression" dxfId="64" priority="16">
+    <cfRule type="expression" dxfId="160" priority="16">
       <formula>AND($K2&lt;&gt;"d", $K2 &lt;&gt; "w", $K2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S108">
-    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q108">
-    <cfRule type="cellIs" dxfId="58" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T108">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="8">
+    <cfRule type="expression" dxfId="148" priority="8">
       <formula>AND($S2 &lt;&gt; "core.endog",$S2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R108">
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11403,8 +11403,8 @@
   </sheetPr>
   <dimension ref="A1:W125"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="S49" sqref="S49"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="T130" sqref="T130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19205,89 +19205,89 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S111:S10000">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="118" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="43" priority="17">
+    <cfRule type="expression" dxfId="117" priority="17">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="42" priority="23">
+    <cfRule type="expression" dxfId="116" priority="23">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S125">
-    <cfRule type="expression" dxfId="41" priority="16">
+    <cfRule type="expression" dxfId="115" priority="16">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V125">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T125">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W125">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="8">
+    <cfRule type="expression" dxfId="103" priority="8">
       <formula>AND($V2 &lt;&gt; "core.endog",$V2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U125">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24242,17 +24242,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="74" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="73" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32403,89 +32403,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="18" priority="22">
+    <cfRule type="expression" dxfId="50" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="49" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="48" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="15" priority="17">
+    <cfRule type="expression" dxfId="47" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="35" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed bankdeposits variable due to excessively large number of vintage changes (v0.20)
</commit_message>
<xml_diff>
--- a/model-inputs/inputs.xlsx
+++ b/model-inputs/inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A722DB-2531-4589-9928-67DF2267D8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B80F63-4399-4D51-8A9E-4249AE72FF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="gdp-model-inputs" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7765" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7748" uniqueCount="759">
   <si>
     <t>gdp</t>
   </si>
@@ -2450,6 +2450,501 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="167">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9393"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4D2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7FBF9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -3012,167 +3507,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3437,25 +3771,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3886,167 +4201,6 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -4417,160 +4571,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4596,61 +4596,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:T108" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:T108" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
   <autoFilter ref="A1:T108" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="142"/>
-    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="141"/>
-    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="140"/>
-    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="139"/>
-    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="138"/>
-    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="137"/>
-    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="136"/>
-    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="135"/>
-    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="134"/>
-    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="133"/>
-    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="132"/>
-    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="130"/>
-    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="129"/>
-    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="128"/>
-    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="127"/>
-    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="126"/>
-    <tableColumn id="29" xr3:uid="{76399FAE-BA60-4EB8-A76D-B35AF5C448A3}" name="initial_forecast" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{8D11F2D0-2DDA-4833-97A3-0AE2613B5941}" name="core_structural" dataDxfId="124"/>
-    <tableColumn id="18" xr3:uid="{5C5BF075-E0AE-47B3-8E6C-DA1E78BAA23F}" name="core_endog_type" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="164"/>
+    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="163"/>
+    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="162"/>
+    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="161"/>
+    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="160"/>
+    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="159"/>
+    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="158"/>
+    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="157"/>
+    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="156"/>
+    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="155"/>
+    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="154"/>
+    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="152"/>
+    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="151"/>
+    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="150"/>
+    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="149"/>
+    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="148"/>
+    <tableColumn id="29" xr3:uid="{76399FAE-BA60-4EB8-A76D-B35AF5C448A3}" name="initial_forecast" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{8D11F2D0-2DDA-4833-97A3-0AE2613B5941}" name="core_structural" dataDxfId="146"/>
+    <tableColumn id="18" xr3:uid="{5C5BF075-E0AE-47B3-8E6C-DA1E78BAA23F}" name="core_endog_type" dataDxfId="145"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:W125" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
-  <autoFilter ref="A1:W125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:W124" totalsRowShown="0" headerRowDxfId="144" dataDxfId="143">
+  <autoFilter ref="A1:W124" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="96"/>
-    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="95"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="94"/>
-    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="93"/>
-    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="92"/>
-    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="91"/>
-    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="89"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="88"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="85"/>
-    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="83"/>
-    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="82"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="81"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="80"/>
-    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="79"/>
-    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="78"/>
-    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="77"/>
-    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="76"/>
-    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="142"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="141"/>
+    <tableColumn id="7" xr3:uid="{08F06606-7021-4E52-9660-46ADE9D5E372}" name="category" dataDxfId="140"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="139"/>
+    <tableColumn id="24" xr3:uid="{5675B337-5638-4136-A846-608D822DBD12}" name="disprank" dataDxfId="138"/>
+    <tableColumn id="25" xr3:uid="{9BA2F34E-1C3D-42FE-B521-452D671DDAE7}" name="disptabs" dataDxfId="137"/>
+    <tableColumn id="31" xr3:uid="{D56C614F-68CF-478F-BAA4-327F75B090C4}" name="disporder" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{492D4F82-F4EA-4E3C-BE49-9BE833FC470D}" name="source" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{D546D480-89FE-48ED-A3A2-21B271A20517}" name="sckey" dataDxfId="134"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="relkey" dataDxfId="133"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{706C8ED1-2F5F-41CE-A4C5-0480444AE901}" name="freq" dataDxfId="131"/>
+    <tableColumn id="5" xr3:uid="{735EAF2C-B95C-4FE2-A0D9-9E3DFE610E9F}" name="append_eom_with_currentval" dataDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{CE3C3317-D60E-4E66-B90C-6EAC0C9FB30D}" name="sa" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{0D80B9B3-7EFB-4282-AE28-1A39DCAED6E8}" name="st" dataDxfId="128"/>
+    <tableColumn id="19" xr3:uid="{F1DAB8A2-5A04-4FCB-8710-7EF09DA839DD}" name="st2" dataDxfId="127"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="126"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="125"/>
+    <tableColumn id="16" xr3:uid="{45C87AF4-A7F8-4A68-9F20-2DAE93A0A7A5}" name="nc_dfm_input" dataDxfId="124"/>
+    <tableColumn id="17" xr3:uid="{65B65B13-E224-4FA2-8D7F-5E6DC66476E3}" name="nc_method" dataDxfId="123"/>
+    <tableColumn id="29" xr3:uid="{2260D190-AE53-4817-8A7C-F49FFCDA204B}" name="initial_forecast" dataDxfId="122"/>
+    <tableColumn id="8" xr3:uid="{6A374888-E280-4CCE-8C96-D61250CCF157}" name="core_structural" dataDxfId="121"/>
+    <tableColumn id="18" xr3:uid="{FE970859-192F-4AF4-919D-F07206B538AF}" name="core_endog_type" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4672,23 +4672,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N97" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="A1:N97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="67"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="64"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="60"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="59"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="117"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="115"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="114"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="112"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="110"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="109"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="108"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="107"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4701,7 +4701,7 @@
     <tableColumn id="1" xr3:uid="{1200786F-7E38-40A6-A987-78A31B68B9F1}" name="fcname"/>
     <tableColumn id="2" xr3:uid="{97045895-B0B7-4CEB-B7DA-ED90C8319FE7}" name="freq"/>
     <tableColumn id="3" xr3:uid="{4F156EE7-4A87-4389-A4C7-46D3EABF7B6E}" name="fullname"/>
-    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{2078932B-4C3D-4CB4-BABD-E7E8C753E1E2}" name="cmefi" dataDxfId="103"/>
     <tableColumn id="5" xr3:uid="{F4C01123-E154-4BD5-A53C-45E96EEB017A}" name="shortname"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4709,39 +4709,39 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:AD125" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <autoFilter ref="A1:AD125" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="26"/>
-    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="25"/>
-    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="24"/>
-    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="8"/>
-    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="7"/>
-    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="6"/>
-    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="3"/>
-    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="100"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="98"/>
+    <tableColumn id="15" xr3:uid="{CDA8D0BF-1E1F-4AEA-9D76-0DFCCBB0530B}" name="dispgroup" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{91E3EFF5-876D-4041-992B-432A28F6D3DE}" name="disprank" dataDxfId="96"/>
+    <tableColumn id="25" xr3:uid="{857A8C83-05F4-4F46-A4D4-E18826F11832}" name="disptabs" dataDxfId="95"/>
+    <tableColumn id="31" xr3:uid="{E41264DE-34E2-43AB-B349-F2D25DE4EFA8}" name="disporder" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="92"/>
+    <tableColumn id="14" xr3:uid="{6D94E881-331E-4563-9FE0-31F2083C7EF8}" name="relkey" dataDxfId="91"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{A581382B-68E8-4159-AD2A-20A164EECC6D}" name="append_eom_with_currentval" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="st" dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{D9B7A04D-639F-4100-8A79-7587967FFA5C}" name="st2" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="d1" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="d2" dataDxfId="83"/>
+    <tableColumn id="20" xr3:uid="{B4904B5A-FEDE-4432-B026-BC1446CD36F3}" name="ext_atl" dataDxfId="82"/>
+    <tableColumn id="21" xr3:uid="{B565BB61-B306-4D71-BE67-952F656343B0}" name="ext_stl" dataDxfId="81"/>
+    <tableColumn id="22" xr3:uid="{7D4D7C84-E16F-487E-9F8A-D0C29C7FEB62}" name="ext_nyf" dataDxfId="80"/>
+    <tableColumn id="23" xr3:uid="{ECC06F80-2CDC-4746-A72E-D0A102B823DB}" name="ext_spf" dataDxfId="79"/>
+    <tableColumn id="26" xr3:uid="{7DCA74BB-02BF-4E52-8DC2-53543E161249}" name="ext_wsj" dataDxfId="78"/>
+    <tableColumn id="27" xr3:uid="{4C1E00F5-F236-4034-B8D5-82EB7DF2B708}" name="ext_cbo" dataDxfId="77"/>
+    <tableColumn id="28" xr3:uid="{563B2464-EB13-44B8-98C4-C5D35F57AB73}" name="ext_mkt" dataDxfId="76"/>
+    <tableColumn id="16" xr3:uid="{C2DD2153-C806-4066-BD87-1D7496470345}" name="nc_dfm_input" dataDxfId="75"/>
+    <tableColumn id="17" xr3:uid="{F981AC56-9903-4E70-A490-7007AAFAE1D6}" name="nc_method" dataDxfId="74"/>
+    <tableColumn id="29" xr3:uid="{62D8107E-C4D3-4FFA-BC99-A564A8A5B18C}" name="initial_forecast" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{0141F8C3-4F4E-48DB-95BB-EE0D1C09F10F}" name="core_structural" dataDxfId="72"/>
+    <tableColumn id="18" xr3:uid="{A65E989C-AC90-407C-B7DA-028F0DA494E9}" name="core_endog_type" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11307,84 +11307,84 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K108">
-    <cfRule type="cellIs" dxfId="166" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S109:S9983 P108">
-    <cfRule type="expression" dxfId="162" priority="18">
+    <cfRule type="expression" dxfId="66" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H108">
-    <cfRule type="expression" dxfId="161" priority="17">
+    <cfRule type="expression" dxfId="65" priority="17">
       <formula>$G2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P108">
-    <cfRule type="expression" dxfId="160" priority="16">
+    <cfRule type="expression" dxfId="64" priority="16">
       <formula>AND($K2&lt;&gt;"d", $K2 &lt;&gt; "w", $K2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S108">
-    <cfRule type="cellIs" dxfId="159" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q108">
-    <cfRule type="cellIs" dxfId="154" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="153" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T108">
-    <cfRule type="cellIs" dxfId="150" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="8">
+    <cfRule type="expression" dxfId="52" priority="8">
       <formula>AND($S2 &lt;&gt; "core.endog",$S2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R108">
-    <cfRule type="cellIs" dxfId="147" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11401,10 +11401,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:W125"/>
+  <dimension ref="A1:W124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="T130" sqref="T130"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15262,13 +15262,13 @@
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>238</v>
+        <v>160</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>667</v>
@@ -15280,13 +15280,13 @@
         <v>1</v>
       </c>
       <c r="G62" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H62" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>655</v>
+        <v>42</v>
       </c>
       <c r="J62" s="10" t="s">
         <v>604</v>
@@ -15316,7 +15316,7 @@
         <v>282</v>
       </c>
       <c r="S62" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T62" s="11" t="s">
         <v>154</v>
@@ -15330,37 +15330,25 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>652</v>
+        <v>47</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>659</v>
+        <v>78</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="E63" s="10">
-        <v>2</v>
-      </c>
-      <c r="F63" s="10">
-        <v>1</v>
-      </c>
-      <c r="G63" s="10">
-        <v>3</v>
+        <v>238</v>
       </c>
       <c r="H63" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>722</v>
+        <v>94</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>388</v>
@@ -15372,13 +15360,13 @@
         <v>405</v>
       </c>
       <c r="O63" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P63" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q63" s="10" t="s">
-        <v>390</v>
+        <v>16</v>
       </c>
       <c r="R63" s="10" t="s">
         <v>282</v>
@@ -15390,45 +15378,52 @@
         <v>154</v>
       </c>
       <c r="V63" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W63" s="11" t="s">
-        <v>663</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="W63" s="11"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>238</v>
       </c>
+      <c r="D64" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="E64" s="10">
+        <v>1</v>
+      </c>
+      <c r="F64" s="10">
+        <v>1</v>
+      </c>
+      <c r="G64" s="10">
+        <v>1</v>
+      </c>
       <c r="H64" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="K64" s="10" t="s">
         <v>94</v>
       </c>
       <c r="L64" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="M64" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N64" s="10" t="s">
         <v>405</v>
       </c>
       <c r="O64" s="10" t="s">
-        <v>16</v>
+        <v>666</v>
       </c>
       <c r="P64" s="10" t="s">
         <v>16</v>
@@ -15446,43 +15441,33 @@
         <v>154</v>
       </c>
       <c r="V64" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="W64" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W64" s="11" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>675</v>
-      </c>
-      <c r="E65" s="10">
-        <v>1</v>
-      </c>
-      <c r="F65" s="10">
-        <v>1</v>
-      </c>
-      <c r="G65" s="10">
-        <v>1</v>
+        <v>252</v>
       </c>
       <c r="H65" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>605</v>
+        <v>611</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>94</v>
+        <v>165</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>30</v>
@@ -15509,33 +15494,43 @@
         <v>154</v>
       </c>
       <c r="V65" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W65" s="11" t="s">
-        <v>663</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="W65" s="11"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>252</v>
+        <v>162</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>718</v>
+      </c>
+      <c r="E66" s="10">
+        <v>1</v>
+      </c>
+      <c r="F66" s="10">
+        <v>1</v>
+      </c>
+      <c r="G66" s="10">
+        <v>2</v>
       </c>
       <c r="H66" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>52</v>
+        <v>716</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>611</v>
+        <v>628</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>165</v>
+        <v>723</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>30</v>
@@ -15544,13 +15539,13 @@
         <v>405</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>666</v>
+        <v>15</v>
       </c>
       <c r="P66" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q66" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="R66" s="10" t="s">
         <v>282</v>
@@ -15562,43 +15557,33 @@
         <v>154</v>
       </c>
       <c r="V66" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="W66" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W66" s="11" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>718</v>
-      </c>
-      <c r="E67" s="10">
-        <v>1</v>
-      </c>
-      <c r="F67" s="10">
-        <v>1</v>
-      </c>
-      <c r="G67" s="10">
-        <v>2</v>
+        <v>252</v>
       </c>
       <c r="H67" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>716</v>
+        <v>55</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>723</v>
+        <v>94</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>30</v>
@@ -15607,13 +15592,13 @@
         <v>405</v>
       </c>
       <c r="O67" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P67" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q67" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="R67" s="10" t="s">
         <v>282</v>
@@ -15622,33 +15607,31 @@
         <v>1</v>
       </c>
       <c r="T67" s="11" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="V67" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W67" s="11" t="s">
-        <v>662</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="W67" s="11"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="H68" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="K68" s="10" t="s">
         <v>94</v>
@@ -15675,7 +15658,7 @@
         <v>1</v>
       </c>
       <c r="T68" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="V68" s="11" t="s">
         <v>282</v>
@@ -15684,22 +15667,22 @@
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>80</v>
+        <v>231</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H69" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="K69" s="10" t="s">
         <v>94</v>
@@ -15711,13 +15694,13 @@
         <v>405</v>
       </c>
       <c r="O69" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P69" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q69" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="R69" s="10" t="s">
         <v>282</v>
@@ -15735,25 +15718,25 @@
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>231</v>
+        <v>96</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H70" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>603</v>
+        <v>630</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>94</v>
+        <v>724</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>30</v>
@@ -15786,28 +15769,40 @@
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>96</v>
+        <v>232</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>98</v>
+        <v>233</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>163</v>
+        <v>238</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="E71" s="10">
+        <v>1</v>
+      </c>
+      <c r="F71" s="10">
+        <v>1</v>
+      </c>
+      <c r="G71" s="10">
+        <v>4</v>
       </c>
       <c r="H71" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>97</v>
+        <v>239</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>724</v>
+        <v>89</v>
       </c>
       <c r="L71" s="10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="N71" s="10" t="s">
         <v>405</v>
@@ -15816,31 +15811,31 @@
         <v>15</v>
       </c>
       <c r="P71" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q71" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="R71" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="S71" s="11">
-        <v>1</v>
-      </c>
+      <c r="S71" s="11"/>
       <c r="T71" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="V71" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="W71" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W71" s="11" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>238</v>
@@ -15855,13 +15850,13 @@
         <v>1</v>
       </c>
       <c r="G72" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H72" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="J72" s="10" t="s">
         <v>631</v>
@@ -15900,10 +15895,10 @@
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C73" s="10" t="s">
         <v>238</v>
@@ -15918,13 +15913,13 @@
         <v>1</v>
       </c>
       <c r="G73" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H73" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I73" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J73" s="10" t="s">
         <v>631</v>
@@ -15963,46 +15958,34 @@
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>237</v>
+        <v>637</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="E74" s="10">
-        <v>1</v>
-      </c>
-      <c r="F74" s="10">
-        <v>1</v>
-      </c>
-      <c r="G74" s="10">
-        <v>6</v>
+        <v>242</v>
       </c>
       <c r="H74" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>241</v>
+        <v>636</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="N74" s="10" t="s">
         <v>405</v>
       </c>
       <c r="O74" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P74" s="10" t="s">
         <v>16</v>
@@ -16013,23 +15996,23 @@
       <c r="R74" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="S74" s="11"/>
+      <c r="S74" s="11">
+        <v>1</v>
+      </c>
       <c r="T74" s="11" t="s">
-        <v>153</v>
+        <v>282</v>
       </c>
       <c r="V74" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W74" s="11" t="s">
-        <v>663</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="W74" s="11"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>637</v>
+        <v>296</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>242</v>
@@ -16038,10 +16021,10 @@
         <v>156</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>636</v>
+        <v>244</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="K75" s="10" t="s">
         <v>94</v>
@@ -16077,10 +16060,10 @@
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>242</v>
@@ -16089,10 +16072,10 @@
         <v>156</v>
       </c>
       <c r="I76" s="10" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="K76" s="10" t="s">
         <v>94</v>
@@ -16128,22 +16111,22 @@
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
       <c r="H77" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I77" s="10" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="K77" s="10" t="s">
         <v>94</v>
@@ -16167,7 +16150,7 @@
         <v>282</v>
       </c>
       <c r="S77" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T77" s="11" t="s">
         <v>282</v>
@@ -16179,28 +16162,31 @@
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>250</v>
+        <v>333</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>251</v>
+        <v>334</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H78" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>253</v>
+        <v>335</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L78" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="M78" s="10">
+        <v>1</v>
       </c>
       <c r="N78" s="10" t="s">
         <v>405</v>
@@ -16218,10 +16204,10 @@
         <v>282</v>
       </c>
       <c r="S78" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T78" s="11" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="V78" s="11" t="s">
         <v>282</v>
@@ -16230,31 +16216,28 @@
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="H79" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I79" s="10" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="K79" s="10" t="s">
         <v>89</v>
       </c>
       <c r="L79" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="M79" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N79" s="10" t="s">
         <v>405</v>
@@ -16284,34 +16267,49 @@
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>336</v>
+        <v>2</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>337</v>
+        <v>60</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>252</v>
+        <v>161</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>720</v>
+      </c>
+      <c r="E80" s="10">
+        <v>1</v>
+      </c>
+      <c r="F80" s="10">
+        <v>1</v>
+      </c>
+      <c r="G80" s="10">
+        <v>1</v>
       </c>
       <c r="H80" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I80" s="10" t="s">
-        <v>338</v>
+        <v>28</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="K80" s="10" t="s">
         <v>89</v>
       </c>
       <c r="L80" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="M80" s="10">
+        <v>1</v>
       </c>
       <c r="N80" s="10" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O80" s="10" t="s">
-        <v>16</v>
+        <v>666</v>
       </c>
       <c r="P80" s="10" t="s">
         <v>16</v>
@@ -16328,17 +16326,20 @@
       <c r="T80" s="11" t="s">
         <v>154</v>
       </c>
+      <c r="U80" s="10" t="s">
+        <v>413</v>
+      </c>
       <c r="V80" s="11" t="s">
-        <v>282</v>
+        <v>534</v>
       </c>
       <c r="W80" s="11"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>161</v>
@@ -16353,16 +16354,16 @@
         <v>1</v>
       </c>
       <c r="G81" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="K81" s="10" t="s">
         <v>89</v>
@@ -16389,7 +16390,7 @@
         <v>282</v>
       </c>
       <c r="S81" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T81" s="11" t="s">
         <v>154</v>
@@ -16404,10 +16405,10 @@
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>161</v>
@@ -16422,16 +16423,16 @@
         <v>1</v>
       </c>
       <c r="G82" s="10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H82" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I82" s="10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="K82" s="10" t="s">
         <v>89</v>
@@ -16458,13 +16459,13 @@
         <v>282</v>
       </c>
       <c r="S82" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T82" s="11" t="s">
         <v>154</v>
       </c>
       <c r="U82" s="10" t="s">
-        <v>413</v>
+        <v>171</v>
       </c>
       <c r="V82" s="11" t="s">
         <v>534</v>
@@ -16473,10 +16474,10 @@
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>161</v>
@@ -16491,13 +16492,13 @@
         <v>1</v>
       </c>
       <c r="G83" s="10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H83" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I83" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J83" s="10" t="s">
         <v>606</v>
@@ -16527,7 +16528,7 @@
         <v>282</v>
       </c>
       <c r="S83" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T83" s="11" t="s">
         <v>154</v>
@@ -16542,10 +16543,10 @@
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>161</v>
@@ -16560,13 +16561,13 @@
         <v>1</v>
       </c>
       <c r="G84" s="10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H84" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I84" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J84" s="10" t="s">
         <v>606</v>
@@ -16611,10 +16612,10 @@
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>161</v>
@@ -16623,19 +16624,19 @@
         <v>720</v>
       </c>
       <c r="E85" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F85" s="10">
         <v>1</v>
       </c>
       <c r="G85" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H85" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I85" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J85" s="10" t="s">
         <v>606</v>
@@ -16680,10 +16681,10 @@
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>161</v>
@@ -16692,19 +16693,19 @@
         <v>720</v>
       </c>
       <c r="E86" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F86" s="10">
         <v>1</v>
       </c>
       <c r="G86" s="10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H86" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I86" s="10" t="s">
-        <v>23</v>
+        <v>399</v>
       </c>
       <c r="J86" s="10" t="s">
         <v>606</v>
@@ -16734,7 +16735,7 @@
         <v>282</v>
       </c>
       <c r="S86" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T86" s="11" t="s">
         <v>154</v>
@@ -16749,10 +16750,10 @@
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>161</v>
@@ -16761,19 +16762,19 @@
         <v>720</v>
       </c>
       <c r="E87" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F87" s="10">
         <v>1</v>
       </c>
       <c r="G87" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H87" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I87" s="10" t="s">
-        <v>399</v>
+        <v>24</v>
       </c>
       <c r="J87" s="10" t="s">
         <v>606</v>
@@ -16803,7 +16804,7 @@
         <v>282</v>
       </c>
       <c r="S87" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T87" s="11" t="s">
         <v>154</v>
@@ -16818,10 +16819,10 @@
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>161</v>
@@ -16836,13 +16837,13 @@
         <v>1</v>
       </c>
       <c r="G88" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H88" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I88" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J88" s="10" t="s">
         <v>606</v>
@@ -16887,10 +16888,10 @@
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>161</v>
@@ -16905,13 +16906,13 @@
         <v>1</v>
       </c>
       <c r="G89" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H89" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I89" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J89" s="10" t="s">
         <v>606</v>
@@ -16956,10 +16957,10 @@
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>161</v>
@@ -16968,19 +16969,19 @@
         <v>720</v>
       </c>
       <c r="E90" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" s="10">
         <v>1</v>
       </c>
       <c r="G90" s="10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H90" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I90" s="10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J90" s="10" t="s">
         <v>606</v>
@@ -17025,10 +17026,10 @@
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>161</v>
@@ -17037,19 +17038,19 @@
         <v>720</v>
       </c>
       <c r="E91" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F91" s="10">
         <v>1</v>
       </c>
       <c r="G91" s="10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H91" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I91" s="10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J91" s="10" t="s">
         <v>606</v>
@@ -17094,40 +17095,40 @@
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>13</v>
+        <v>341</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>67</v>
+        <v>344</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>161</v>
+        <v>313</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>720</v>
       </c>
       <c r="E92" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92" s="10">
         <v>1</v>
       </c>
       <c r="G92" s="10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H92" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I92" s="10" t="s">
-        <v>27</v>
+        <v>348</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>606</v>
+        <v>632</v>
       </c>
       <c r="K92" s="10" t="s">
         <v>89</v>
       </c>
       <c r="L92" s="10" t="s">
-        <v>340</v>
+        <v>388</v>
       </c>
       <c r="M92" s="10">
         <v>1</v>
@@ -17163,10 +17164,10 @@
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>313</v>
@@ -17181,13 +17182,13 @@
         <v>1</v>
       </c>
       <c r="G93" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H93" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I93" s="10" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="J93" s="10" t="s">
         <v>632</v>
@@ -17217,7 +17218,7 @@
         <v>282</v>
       </c>
       <c r="S93" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T93" s="11" t="s">
         <v>154</v>
@@ -17232,31 +17233,19 @@
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>342</v>
+        <v>385</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>720</v>
-      </c>
-      <c r="E94" s="10">
-        <v>1</v>
-      </c>
-      <c r="F94" s="10">
-        <v>1</v>
-      </c>
-      <c r="G94" s="10">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="H94" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I94" s="10" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="J94" s="10" t="s">
         <v>632</v>
@@ -17286,55 +17275,51 @@
         <v>282</v>
       </c>
       <c r="S94" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T94" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="U94" s="10" t="s">
-        <v>171</v>
-      </c>
       <c r="V94" s="11" t="s">
-        <v>534</v>
-      </c>
-      <c r="W94" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W94" s="11" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>385</v>
+        <v>343</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H95" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I95" s="10" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L95" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="M95" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N95" s="10" t="s">
         <v>406</v>
       </c>
       <c r="O95" s="10" t="s">
-        <v>666</v>
+        <v>101</v>
       </c>
       <c r="P95" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="Q95" s="10" t="s">
         <v>16</v>
@@ -17349,33 +17334,40 @@
         <v>154</v>
       </c>
       <c r="V95" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W95" s="11" t="s">
-        <v>663</v>
-      </c>
+        <v>660</v>
+      </c>
+      <c r="W95" s="11"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>163</v>
       </c>
+      <c r="D96" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E96" s="10">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10">
+        <v>1</v>
+      </c>
+      <c r="G96" s="10">
+        <v>1</v>
+      </c>
       <c r="H96" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="I96" s="10" t="s">
-        <v>351</v>
+        <v>171</v>
       </c>
       <c r="J96" s="10" t="s">
         <v>617</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L96" s="10" t="s">
         <v>30</v>
@@ -17384,10 +17376,10 @@
         <v>406</v>
       </c>
       <c r="O96" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="P96" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="Q96" s="10" t="s">
         <v>16</v>
@@ -17401,23 +17393,26 @@
       <c r="T96" s="11" t="s">
         <v>154</v>
       </c>
+      <c r="U96" s="10" t="s">
+        <v>413</v>
+      </c>
       <c r="V96" s="11" t="s">
-        <v>660</v>
+        <v>534</v>
       </c>
       <c r="W96" s="11"/>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>386</v>
+        <v>39</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>387</v>
+        <v>74</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>163</v>
+        <v>238</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>163</v>
+        <v>719</v>
       </c>
       <c r="E97" s="10">
         <v>1</v>
@@ -17429,34 +17424,40 @@
         <v>1</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>171</v>
+        <v>249</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>289</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>617</v>
+        <v>633</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L97" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="M97" s="10">
+        <v>1</v>
       </c>
       <c r="N97" s="10" t="s">
         <v>406</v>
       </c>
       <c r="O97" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P97" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q97" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="R97" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="S97" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T97" s="11" t="s">
         <v>154</v>
@@ -17471,10 +17472,10 @@
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>238</v>
@@ -17483,19 +17484,19 @@
         <v>719</v>
       </c>
       <c r="E98" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F98" s="10">
         <v>1</v>
       </c>
       <c r="G98" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H98" s="10" t="s">
         <v>249</v>
       </c>
       <c r="I98" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J98" s="10" t="s">
         <v>633</v>
@@ -17516,34 +17517,33 @@
         <v>15</v>
       </c>
       <c r="P98" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q98" s="10" t="s">
-        <v>390</v>
+        <v>16</v>
       </c>
       <c r="R98" s="10" t="s">
-        <v>16</v>
+        <v>282</v>
       </c>
       <c r="S98" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T98" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="U98" s="10" t="s">
-        <v>413</v>
-      </c>
       <c r="V98" s="11" t="s">
-        <v>534</v>
-      </c>
-      <c r="W98" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W98" s="11" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>40</v>
+        <v>638</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>58</v>
+        <v>646</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>238</v>
@@ -17558,13 +17558,13 @@
         <v>1</v>
       </c>
       <c r="G99" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H99" s="10" t="s">
         <v>249</v>
       </c>
       <c r="I99" s="10" t="s">
-        <v>290</v>
+        <v>639</v>
       </c>
       <c r="J99" s="10" t="s">
         <v>633</v>
@@ -17585,13 +17585,13 @@
         <v>15</v>
       </c>
       <c r="P99" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q99" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="R99" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="S99" s="11">
         <v>0</v>
@@ -17608,10 +17608,10 @@
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>238</v>
@@ -17626,13 +17626,13 @@
         <v>1</v>
       </c>
       <c r="G100" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H100" s="10" t="s">
         <v>249</v>
       </c>
       <c r="I100" s="10" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="J100" s="10" t="s">
         <v>633</v>
@@ -17676,31 +17676,19 @@
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D101" s="10" t="s">
-        <v>719</v>
-      </c>
-      <c r="E101" s="10">
-        <v>2</v>
-      </c>
-      <c r="F101" s="10">
-        <v>1</v>
-      </c>
-      <c r="G101" s="10">
-        <v>4</v>
-      </c>
       <c r="H101" s="10" t="s">
         <v>249</v>
       </c>
       <c r="I101" s="10" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="J101" s="10" t="s">
         <v>633</v>
@@ -17736,54 +17724,46 @@
         <v>154</v>
       </c>
       <c r="V101" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W101" s="11" t="s">
-        <v>663</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="W101" s="11"/>
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>642</v>
+        <v>391</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>644</v>
+        <v>394</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>238</v>
+        <v>161</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="I102" s="10" t="s">
-        <v>643</v>
+        <v>171</v>
       </c>
       <c r="J102" s="10" t="s">
-        <v>633</v>
+        <v>606</v>
       </c>
       <c r="K102" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L102" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="M102" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N102" s="10" t="s">
         <v>406</v>
       </c>
       <c r="O102" s="10" t="s">
-        <v>15</v>
+        <v>666</v>
       </c>
       <c r="P102" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q102" s="10" t="s">
-        <v>390</v>
+        <v>16</v>
       </c>
       <c r="R102" s="10" t="s">
-        <v>16</v>
+        <v>282</v>
       </c>
       <c r="S102" s="11">
         <v>0</v>
@@ -17791,17 +17771,20 @@
       <c r="T102" s="11" t="s">
         <v>154</v>
       </c>
+      <c r="U102" s="10" t="s">
+        <v>413</v>
+      </c>
       <c r="V102" s="11" t="s">
-        <v>282</v>
+        <v>534</v>
       </c>
       <c r="W102" s="11"/>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>161</v>
@@ -17849,10 +17832,10 @@
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>161</v>
@@ -17900,19 +17883,19 @@
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>393</v>
+        <v>647</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>396</v>
+        <v>648</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>161</v>
+        <v>313</v>
       </c>
       <c r="H105" s="10" t="s">
         <v>171</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>606</v>
+        <v>632</v>
       </c>
       <c r="K105" s="10" t="s">
         <v>89</v>
@@ -17939,22 +17922,22 @@
         <v>0</v>
       </c>
       <c r="T105" s="11" t="s">
-        <v>154</v>
+        <v>282</v>
       </c>
       <c r="U105" s="10" t="s">
         <v>413</v>
       </c>
       <c r="V105" s="11" t="s">
-        <v>534</v>
+        <v>282</v>
       </c>
       <c r="W105" s="11"/>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>647</v>
+        <v>397</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>648</v>
+        <v>398</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>313</v>
@@ -18002,37 +17985,40 @@
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>397</v>
+        <v>217</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>398</v>
+        <v>218</v>
       </c>
       <c r="C107" s="10" t="s">
-        <v>313</v>
+        <v>162</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>171</v>
+        <v>156</v>
+      </c>
+      <c r="I107" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="K107" s="10" t="s">
-        <v>89</v>
+        <v>725</v>
       </c>
       <c r="L107" s="10" t="s">
         <v>30</v>
       </c>
       <c r="N107" s="10" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O107" s="10" t="s">
-        <v>666</v>
+        <v>15</v>
       </c>
       <c r="P107" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q107" s="10" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="R107" s="10" t="s">
         <v>282</v>
@@ -18041,10 +18027,7 @@
         <v>0</v>
       </c>
       <c r="T107" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="U107" s="10" t="s">
-        <v>413</v>
+        <v>154</v>
       </c>
       <c r="V107" s="11" t="s">
         <v>282</v>
@@ -18053,19 +18036,31 @@
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>162</v>
       </c>
+      <c r="D108" s="10" t="s">
+        <v>721</v>
+      </c>
+      <c r="E108" s="10">
+        <v>1</v>
+      </c>
+      <c r="F108" s="10">
+        <v>1</v>
+      </c>
+      <c r="G108" s="10">
+        <v>1</v>
+      </c>
       <c r="H108" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I108" s="10" t="s">
-        <v>221</v>
+        <v>87</v>
       </c>
       <c r="J108" s="10" t="s">
         <v>630</v>
@@ -18089,31 +18084,34 @@
         <v>101</v>
       </c>
       <c r="R108" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="S108" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T108" s="11" t="s">
         <v>154</v>
       </c>
+      <c r="U108" s="10" t="s">
+        <v>413</v>
+      </c>
       <c r="V108" s="11" t="s">
-        <v>282</v>
+        <v>534</v>
       </c>
       <c r="W108" s="11"/>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>222</v>
+        <v>303</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="E109" s="10">
         <v>1</v>
@@ -18128,13 +18126,13 @@
         <v>156</v>
       </c>
       <c r="I109" s="10" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>630</v>
+        <v>611</v>
       </c>
       <c r="K109" s="10" t="s">
-        <v>725</v>
+        <v>89</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>30</v>
@@ -18149,10 +18147,10 @@
         <v>15</v>
       </c>
       <c r="Q109" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="R109" s="10" t="s">
-        <v>16</v>
+        <v>282</v>
       </c>
       <c r="S109" s="11">
         <v>1</v>
@@ -18170,40 +18168,31 @@
     </row>
     <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>35</v>
+        <v>649</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>303</v>
+        <v>650</v>
       </c>
       <c r="C110" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>717</v>
-      </c>
-      <c r="E110" s="10">
-        <v>1</v>
-      </c>
-      <c r="F110" s="10">
-        <v>1</v>
-      </c>
-      <c r="G110" s="10">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="H110" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I110" s="10" t="s">
-        <v>36</v>
+        <v>651</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>89</v>
+        <v>722</v>
       </c>
       <c r="L110" s="10" t="s">
-        <v>30</v>
+        <v>388</v>
+      </c>
+      <c r="M110" s="10">
+        <v>1</v>
       </c>
       <c r="N110" s="10" t="s">
         <v>405</v>
@@ -18215,52 +18204,58 @@
         <v>15</v>
       </c>
       <c r="Q110" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="R110" s="10" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="S110" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T110" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="U110" s="10" t="s">
-        <v>413</v>
-      </c>
       <c r="V110" s="11" t="s">
-        <v>534</v>
+        <v>282</v>
       </c>
       <c r="W110" s="11"/>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>649</v>
+        <v>676</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>650</v>
+        <v>697</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>238</v>
+        <v>162</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>718</v>
+      </c>
+      <c r="E111" s="10">
+        <v>2</v>
+      </c>
+      <c r="F111" s="10">
+        <v>2</v>
+      </c>
+      <c r="G111" s="10">
+        <v>3</v>
       </c>
       <c r="H111" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I111" s="10" t="s">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="J111" s="10" t="s">
-        <v>604</v>
+        <v>628</v>
       </c>
       <c r="K111" s="10" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="L111" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="M111" s="10">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="N111" s="10" t="s">
         <v>405</v>
@@ -18272,7 +18267,7 @@
         <v>15</v>
       </c>
       <c r="Q111" s="10" t="s">
-        <v>390</v>
+        <v>101</v>
       </c>
       <c r="R111" s="10" t="s">
         <v>16</v>
@@ -18283,17 +18278,20 @@
       <c r="T111" s="11" t="s">
         <v>154</v>
       </c>
+      <c r="U111" s="11"/>
       <c r="V111" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="W111" s="11"/>
+        <v>533</v>
+      </c>
+      <c r="W111" s="11" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>162</v>
@@ -18308,13 +18306,13 @@
         <v>2</v>
       </c>
       <c r="G112" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H112" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I112" s="10" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="J112" s="10" t="s">
         <v>628</v>
@@ -18356,10 +18354,10 @@
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>162</v>
@@ -18374,13 +18372,13 @@
         <v>2</v>
       </c>
       <c r="G113" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H113" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I113" s="10" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="J113" s="10" t="s">
         <v>628</v>
@@ -18422,10 +18420,10 @@
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>162</v>
@@ -18440,13 +18438,13 @@
         <v>2</v>
       </c>
       <c r="G114" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H114" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I114" s="10" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="J114" s="10" t="s">
         <v>628</v>
@@ -18488,10 +18486,10 @@
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="C115" s="10" t="s">
         <v>162</v>
@@ -18506,13 +18504,13 @@
         <v>2</v>
       </c>
       <c r="G115" s="10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H115" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I115" s="10" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="J115" s="10" t="s">
         <v>628</v>
@@ -18554,10 +18552,10 @@
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="C116" s="10" t="s">
         <v>162</v>
@@ -18572,13 +18570,13 @@
         <v>2</v>
       </c>
       <c r="G116" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H116" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I116" s="10" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="J116" s="10" t="s">
         <v>628</v>
@@ -18620,10 +18618,10 @@
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>162</v>
@@ -18638,13 +18636,13 @@
         <v>2</v>
       </c>
       <c r="G117" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H117" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I117" s="10" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="J117" s="10" t="s">
         <v>628</v>
@@ -18686,10 +18684,10 @@
     </row>
     <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>162</v>
@@ -18704,13 +18702,13 @@
         <v>2</v>
       </c>
       <c r="G118" s="10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H118" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="J118" s="10" t="s">
         <v>628</v>
@@ -18752,10 +18750,10 @@
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>162</v>
@@ -18770,13 +18768,13 @@
         <v>2</v>
       </c>
       <c r="G119" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H119" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="J119" s="10" t="s">
         <v>628</v>
@@ -18818,10 +18816,10 @@
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>162</v>
@@ -18836,13 +18834,13 @@
         <v>2</v>
       </c>
       <c r="G120" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H120" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="J120" s="10" t="s">
         <v>628</v>
@@ -18884,10 +18882,10 @@
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>685</v>
+        <v>711</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>689</v>
+        <v>712</v>
       </c>
       <c r="C121" s="10" t="s">
         <v>162</v>
@@ -18902,13 +18900,13 @@
         <v>2</v>
       </c>
       <c r="G121" s="10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H121" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="J121" s="10" t="s">
         <v>628</v>
@@ -18950,10 +18948,10 @@
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>711</v>
+        <v>686</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>712</v>
+        <v>688</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>162</v>
@@ -18968,13 +18966,13 @@
         <v>2</v>
       </c>
       <c r="G122" s="10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H122" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I122" s="10" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="J122" s="10" t="s">
         <v>628</v>
@@ -19016,10 +19014,10 @@
     </row>
     <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>688</v>
+        <v>699</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>162</v>
@@ -19034,13 +19032,13 @@
         <v>2</v>
       </c>
       <c r="G123" s="10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H123" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="J123" s="10" t="s">
         <v>628</v>
@@ -19082,55 +19080,46 @@
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>687</v>
+        <v>728</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>699</v>
+        <v>729</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="D124" s="10" t="s">
-        <v>718</v>
-      </c>
-      <c r="E124" s="10">
-        <v>2</v>
-      </c>
-      <c r="F124" s="10">
-        <v>2</v>
-      </c>
-      <c r="G124" s="10">
-        <v>15</v>
+        <v>238</v>
       </c>
       <c r="H124" s="10" t="s">
         <v>156</v>
       </c>
       <c r="I124" s="10" t="s">
-        <v>715</v>
+        <v>730</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>628</v>
+        <v>731</v>
       </c>
       <c r="K124" s="10" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="L124" s="10" t="s">
-        <v>30</v>
+        <v>340</v>
+      </c>
+      <c r="M124" s="10">
+        <v>1</v>
       </c>
       <c r="N124" s="10" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="O124" s="10" t="s">
-        <v>15</v>
+        <v>390</v>
       </c>
       <c r="P124" s="10" t="s">
-        <v>15</v>
+        <v>390</v>
       </c>
       <c r="Q124" s="10" t="s">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="R124" s="10" t="s">
-        <v>16</v>
+        <v>390</v>
       </c>
       <c r="S124" s="11">
         <v>0</v>
@@ -19146,148 +19135,91 @@
         <v>663</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A125" s="7" t="s">
-        <v>728</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="C125" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H125" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="I125" s="10" t="s">
-        <v>730</v>
-      </c>
-      <c r="J125" s="10" t="s">
-        <v>731</v>
-      </c>
-      <c r="K125" s="10" t="s">
-        <v>732</v>
-      </c>
-      <c r="L125" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="M125" s="10">
-        <v>1</v>
-      </c>
-      <c r="N125" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="O125" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="P125" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="Q125" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="R125" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="S125" s="11">
-        <v>0</v>
-      </c>
-      <c r="T125" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="U125" s="11"/>
-      <c r="V125" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="W125" s="11" t="s">
-        <v>663</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="122" priority="19" operator="equal">
+  <conditionalFormatting sqref="L1:M124">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S111:S10000">
-    <cfRule type="expression" dxfId="118" priority="18">
+  <conditionalFormatting sqref="S110:S9999">
+    <cfRule type="expression" dxfId="44" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="117" priority="17">
+  <conditionalFormatting sqref="I2:I124">
+    <cfRule type="expression" dxfId="43" priority="17">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="116" priority="23">
+  <conditionalFormatting sqref="M2:M124">
+    <cfRule type="expression" dxfId="42" priority="23">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S125">
-    <cfRule type="expression" dxfId="115" priority="16">
+  <conditionalFormatting sqref="S2:S124">
+    <cfRule type="expression" dxfId="41" priority="16">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V125">
-    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
+  <conditionalFormatting sqref="V2:V124">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T125">
-    <cfRule type="cellIs" dxfId="109" priority="4" operator="equal">
+  <conditionalFormatting sqref="T2:T124">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W125">
-    <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
+  <conditionalFormatting sqref="W2:W124">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="8">
+    <cfRule type="expression" dxfId="29" priority="8">
       <formula>AND($V2 &lt;&gt; "core.endog",$V2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U125">
-    <cfRule type="cellIs" dxfId="102" priority="5" operator="equal">
+  <conditionalFormatting sqref="U2:U124">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24242,17 +24174,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N97">
-    <cfRule type="expression" dxfId="74" priority="3">
+    <cfRule type="expression" dxfId="25" priority="3">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M97">
-    <cfRule type="expression" dxfId="73" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32403,89 +32335,89 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="L1:M125">
-    <cfRule type="cellIs" dxfId="54" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z112:Z10021">
-    <cfRule type="expression" dxfId="50" priority="22">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I125">
-    <cfRule type="expression" dxfId="49" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>$H2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M125">
-    <cfRule type="expression" dxfId="48" priority="31">
+    <cfRule type="expression" dxfId="16" priority="31">
       <formula>OR($L2="q", $L2 = "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z2:Z125">
-    <cfRule type="expression" dxfId="47" priority="17">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC125">
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"core.exog.p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"post.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"core.endog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"core.exog"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA125">
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD125">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"identity.ll"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"estimated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>AND($AC2 &lt;&gt; "core.endog",$AC2 &lt;&gt; "core.exog.p")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB125">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>